<commit_message>
Use language maps for vocabulary definition, and for natural-language terms.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="800" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="1300" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="258">
-  <si>
-    <t>The separator between cells. The default is ",".</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="264">
   <si>
     <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
 </t>
@@ -151,6 +147,10 @@
     <t>Template,Column</t>
   </si>
   <si>
+    <t>The separator between cells. The default is ",".</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
   </si>
   <si>
@@ -346,6 +346,10 @@
     <t>commentPrefix</t>
   </si>
   <si>
+    <t>xsd:anyURI</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>datatype</t>
   </si>
   <si>
@@ -676,6 +680,14 @@
     <t>http://purl.org/linked-data/cube#</t>
   </si>
   <si>
+    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>required</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>http://www.w3.org/2003/g/data-view#</t>
   </si>
   <si>
@@ -688,9 +700,6 @@
     <t>http://www.w3.org/2002/07/owl#</t>
   </si>
   <si>
-    <t>container</t>
-  </si>
-  <si>
     <t>http://www.w3.org/ns/prov#</t>
   </si>
   <si>
@@ -809,13 +818,35 @@
   </si>
   <si>
     <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
+  </si>
+  <si>
+    <t>predicateUrl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>predicate URL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Column</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -858,6 +889,19 @@
       <sz val="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -881,7 +925,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -895,6 +939,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1228,545 +1274,553 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H86" sqref="H86"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="43.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>"@type"</f>
+        <v>@type</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>"@container"</f>
+        <v>@container</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
         <v>118</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>170</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="B11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
         <v>196</v>
       </c>
-      <c r="B6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>169</v>
-      </c>
-      <c r="B11" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>233</v>
-      </c>
-      <c r="B12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>203</v>
-      </c>
-      <c r="B14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
         <v>211</v>
       </c>
-      <c r="B33" t="s">
-        <v>170</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>185</v>
-      </c>
-      <c r="B34" t="s">
-        <v>170</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>208</v>
-      </c>
-      <c r="B35" t="s">
-        <v>170</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>187</v>
-      </c>
-      <c r="B37" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>209</v>
-      </c>
-      <c r="B38" t="s">
-        <v>170</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>210</v>
-      </c>
       <c r="B39" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
         <v>189</v>
       </c>
-      <c r="B40" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>188</v>
-      </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B43" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
         <v>101</v>
@@ -1777,500 +1831,513 @@
       <c r="F46" t="s">
         <v>92</v>
       </c>
-      <c r="G46" t="str">
+      <c r="H46" t="str">
         <f>"@list"</f>
         <v>@list</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="J46" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="60">
+    <row r="47" spans="1:10" ht="60">
       <c r="A47" t="s">
         <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E47" t="s">
         <v>89</v>
       </c>
-      <c r="H47" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="60">
+      <c r="J47" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="60">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H48" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="J48" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>75</v>
+      </c>
+      <c r="E49" t="s">
+        <v>89</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="E50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" t="s">
         <v>89</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="45">
+      <c r="G50" s="8"/>
+      <c r="J50" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="E51" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F51" t="s">
-        <v>89</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="30">
+        <v>114</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
         <v>89</v>
       </c>
-      <c r="F52" t="s">
-        <v>113</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="30">
+      <c r="J52" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="409">
       <c r="A53" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="E53" t="s">
-        <v>89</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="409">
+        <v>91</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30">
       <c r="A54" t="s">
         <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" t="s">
-        <v>91</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="30">
+        <v>109</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C55" t="s">
-        <v>108</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>111</v>
+      </c>
+      <c r="E55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="45">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="E56" t="s">
         <v>89</v>
       </c>
       <c r="F56" t="s">
+        <v>149</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30">
+      <c r="A57" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="45">
-      <c r="A57" t="s">
-        <v>111</v>
-      </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E57" t="s">
         <v>89</v>
       </c>
       <c r="F57" t="s">
-        <v>148</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="30">
+        <v>149</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30">
       <c r="A58" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s">
+        <v>156</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59" t="s">
+        <v>149</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="30">
+      <c r="A60" t="s">
         <v>116</v>
       </c>
-      <c r="C58" t="s">
-        <v>131</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" t="s">
+        <v>133</v>
+      </c>
+      <c r="E60" t="s">
         <v>89</v>
       </c>
-      <c r="F58" t="s">
-        <v>148</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="30">
-      <c r="A59" t="s">
-        <v>114</v>
-      </c>
-      <c r="B59" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" t="s">
-        <v>114</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="J60" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H59" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" t="s">
-        <v>155</v>
-      </c>
-      <c r="B60" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" t="s">
-        <v>155</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F60" t="s">
-        <v>148</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="30">
-      <c r="A61" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" t="s">
-        <v>132</v>
-      </c>
-      <c r="E61" t="s">
-        <v>89</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="J61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H62" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="J62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H63" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="F63" t="s">
+        <v>149</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C64" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F64" t="s">
-        <v>148</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="J64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H65" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="J65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="F66" t="s">
+        <v>149</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="75">
       <c r="A67" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C67" t="s">
-        <v>31</v>
-      </c>
-      <c r="E67" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" t="s">
         <v>92</v>
       </c>
-      <c r="F67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="75">
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="45">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E68" t="s">
+        <v>88</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" t="s">
+        <v>136</v>
+      </c>
+      <c r="E69" t="s">
         <v>92</v>
       </c>
-      <c r="H68" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="45">
-      <c r="A69" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" t="s">
-        <v>116</v>
-      </c>
-      <c r="C69" t="s">
-        <v>134</v>
-      </c>
-      <c r="E69" t="s">
-        <v>88</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="30">
+      <c r="J69" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="45">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>261</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>262</v>
       </c>
       <c r="E70" t="s">
-        <v>92</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="45">
+        <v>263</v>
+      </c>
+      <c r="F70" t="s">
+        <v>103</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="45">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E71" t="s">
         <v>91</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="J71" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E72" t="s">
         <v>89</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="J72" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="30">
+    <row r="73" spans="1:10" ht="30">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>92</v>
       </c>
       <c r="F73" t="s">
-        <v>113</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="30">
+        <v>114</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="30">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C74" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E74" t="s">
         <v>86</v>
@@ -2278,19 +2345,26 @@
       <c r="F74" t="s">
         <v>88</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" t="str">
+        <f>"@set"</f>
+        <v>@set</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="45">
+    <row r="75" spans="1:10" ht="45">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C75" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E75" t="s">
         <v>64</v>
@@ -2298,187 +2372,191 @@
       <c r="F75" t="s">
         <v>91</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="J75" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="135">
+    <row r="76" spans="1:10" ht="135">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H76" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="45">
+      <c r="J76" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="45">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E77" t="s">
         <v>89</v>
       </c>
       <c r="F77" t="s">
-        <v>113</v>
-      </c>
-      <c r="H77" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J77" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="45">
+    <row r="78" spans="1:10" ht="45">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E78" t="s">
         <v>89</v>
       </c>
       <c r="F78" t="s">
-        <v>148</v>
-      </c>
-      <c r="H78" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J78" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E79" t="s">
         <v>89</v>
       </c>
       <c r="F79" t="s">
-        <v>113</v>
-      </c>
-      <c r="H79" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J79" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="30">
+    <row r="80" spans="1:10" ht="30">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C80" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E80" t="s">
         <v>89</v>
       </c>
       <c r="F80" t="s">
-        <v>148</v>
-      </c>
-      <c r="H80" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J80" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="180">
+    <row r="81" spans="1:10" ht="180">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C81" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E81" t="s">
         <v>90</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="J81" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="75">
+    <row r="82" spans="1:10" ht="75">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E82" t="s">
         <v>64</v>
       </c>
       <c r="F82" t="s">
-        <v>118</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="120">
+        <v>119</v>
+      </c>
+      <c r="G82" t="str">
+        <f>"@vocab"</f>
+        <v>@vocab</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="120">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E83" t="s">
         <v>90</v>
       </c>
-      <c r="H83" s="5" t="s">
+      <c r="J83" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="120">
+    <row r="84" spans="1:10" ht="120">
       <c r="A84" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C84" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E84" t="s">
         <v>90</v>
       </c>
-      <c r="H84" s="5" t="s">
+      <c r="J84" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="45">
+    <row r="85" spans="1:10" ht="45">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B85" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E85" t="s">
         <v>64</v>
@@ -2486,89 +2564,93 @@
       <c r="F85" t="s">
         <v>90</v>
       </c>
-      <c r="H85" s="5" t="s">
+      <c r="J85" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="45">
+    <row r="86" spans="1:10" ht="45">
       <c r="A86" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E86" t="s">
         <v>92</v>
       </c>
       <c r="F86" t="s">
-        <v>118</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="135">
+        <v>119</v>
+      </c>
+      <c r="G86" t="str">
+        <f>"@vocab"</f>
+        <v>@vocab</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="135">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C87" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E87" t="s">
-        <v>37</v>
-      </c>
-      <c r="G87" t="str">
-        <f>"@list"</f>
-        <v>@list</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="30">
+        <v>36</v>
+      </c>
+      <c r="H87" t="str">
+        <f>"@language"</f>
+        <v>@language</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="30">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B88" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C88" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E88" t="s">
         <v>89</v>
       </c>
       <c r="F88" t="s">
-        <v>113</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="45">
+        <v>114</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="45">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B89" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E89" t="s">
         <v>91</v>
       </c>
-      <c r="H89" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="J89" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -2578,11 +2660,11 @@
       <c r="C90" t="s">
         <v>100</v>
       </c>
-      <c r="H90" s="5" t="s">
+      <c r="J90" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="30">
+    <row r="91" spans="1:10" ht="30">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -2590,27 +2672,27 @@
         <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>254</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>256</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B92" t="s">
         <v>87</v>
       </c>
       <c r="C92" t="s">
-        <v>118</v>
-      </c>
-      <c r="H92" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="30">
+      <c r="J92" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="30">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2620,11 +2702,11 @@
       <c r="C93" t="s">
         <v>91</v>
       </c>
-      <c r="H93" s="5" t="s">
+      <c r="J93" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="30">
+    <row r="94" spans="1:10" ht="30">
       <c r="A94" t="s">
         <v>88</v>
       </c>
@@ -2634,11 +2716,11 @@
       <c r="C94" t="s">
         <v>94</v>
       </c>
-      <c r="H94" s="5" t="s">
+      <c r="J94" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="30">
+    <row r="95" spans="1:10" ht="30">
       <c r="A95" t="s">
         <v>86</v>
       </c>
@@ -2648,11 +2730,11 @@
       <c r="C95" t="s">
         <v>93</v>
       </c>
-      <c r="H95" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="45">
+      <c r="J95" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="45">
       <c r="A96" t="s">
         <v>90</v>
       </c>
@@ -2660,13 +2742,13 @@
         <v>87</v>
       </c>
       <c r="C96" t="s">
-        <v>256</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>258</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -2679,11 +2761,11 @@
       <c r="D97" t="s">
         <v>41</v>
       </c>
-      <c r="H97" s="5" t="s">
+      <c r="J97" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>53</v>
       </c>
@@ -2694,7 +2776,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>51</v>
       </c>
@@ -2705,7 +2787,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>52</v>
       </c>
@@ -2716,7 +2798,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>80</v>
       </c>
@@ -2727,7 +2809,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>54</v>
       </c>
@@ -2738,7 +2820,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>82</v>
       </c>
@@ -2749,31 +2831,31 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B104" t="s">
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B105" t="s">
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -2784,7 +2866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>84</v>
       </c>
@@ -2795,9 +2877,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B108" t="s">
         <v>79</v>
@@ -2807,9 +2889,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H109">
-    <sortCondition ref="B2:B109"/>
-    <sortCondition ref="A2:A109"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <sortState ref="A99:XFD109">
+    <sortCondition ref="A99:A109"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -2856,6 +2938,7 @@
     <hyperlink ref="D33" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Organize JSON-LD with Ontology at root, with reverse properties separating classes, properties, datatypes, and instances.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1300" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -839,14 +839,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -948,7 +942,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1273,15 +1267,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
@@ -2889,7 +2883,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A99:XFD109">
     <sortCondition ref="A99:A109"/>
   </sortState>
@@ -2940,7 +2933,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Use "csvw" instead of "csvm" as namespace prefix. Generate unionOf markup in HTML output.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="10620" yWindow="3900" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -21,42 +21,699 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="264">
   <si>
-    <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
-</t>
+    <t>http://www.w3.org/ns/csvw#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of csvw:rtl csvw:ltr or csvw:default. Indicates whether the tables in the group should be displayed with the first column on the right, on the left, or based on the first character in the table that has a specific direction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of csvw:rtl or csvw:ltr. Indicates whether the text within cells should be displayed by default as left-to-right or right-to-left text. </t>
+  </si>
+  <si>
+    <t>csvw:maxInclusive</t>
+  </si>
+  <si>
+    <t>csvw:minInclusive</t>
+  </si>
+  <si>
+    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>A character that, when it appears at the beginning of a skipped row, indicates a comment that should be associated as a comment annotation to the table. The default is "#".</t>
+    <t>required</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>The number of header rows (following the skipped rows) in the file. The default is 1.</t>
+    <t>http://www.w3.org/2003/g/data-view#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/ma-ont#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/org#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2002/07/owl#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/prov#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/rdfa#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2007/rif#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/r2rml#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/sparql-service-description#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2004/02/skos/core#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2008/05/skos-xl#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2007/05/powder#</t>
+  </si>
+  <si>
+    <t>http://rdfs.org/ns/void#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2007/05/powder-s#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/xhtml/vocab#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/XML/1998/namespace</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2001/XMLSchema#</t>
+  </si>
+  <si>
+    <t>dcterms</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/people#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2008/content#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/earl#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2006/http#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2009/pointers#</t>
+  </si>
+  <si>
+    <t>http://creativecommons.org/ns#</t>
+  </si>
+  <si>
+    <t>http://commontag.org/ns#</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/elements/1.1/</t>
+  </si>
+  <si>
+    <t>http://xmlns.com/foaf/0.1/</t>
+  </si>
+  <si>
+    <t>http://purl.org/goodrelations/v1#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2002/12/cal/icaltzd#</t>
+  </si>
+  <si>
+    <t>http://ogp.me/ns#</t>
+  </si>
+  <si>
+    <t>http://purl.org/stuff/rev#</t>
+  </si>
+  <si>
+    <t>http://rdfs.org/sioc/ns#</t>
+  </si>
+  <si>
+    <t>http://rdf.data-vocabulary.org/#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2006/vcard/ns#</t>
+  </si>
+  <si>
+    <t>http://schema.org/</t>
+  </si>
+  <si>
+    <t>A Table Group Description describes a group of Tables.</t>
+  </si>
+  <si>
+    <t>Dialect Description</t>
+  </si>
+  <si>
+    <t>A Dialect Description provides hints to parsers about how to parse a linked file.</t>
+  </si>
+  <si>
+    <t>Template Specification</t>
+  </si>
+  <si>
+    <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
+  </si>
+  <si>
+    <t>predicateUrl</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
-For a Column: A natural language property that provides possible alternative names for the column.</t>
-  </si>
-  <si>
-    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
-  </si>
-  <si>
-    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
-  </si>
-  <si>
-    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
-  </si>
-  <si>
-    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of csvm:rtl or csvm:ltr. Indicates whether the text within cells should be displayed by default as left-to-right or right-to-left text. </t>
-  </si>
-  <si>
-    <t>The character used to separate items in the string value of the cell. If null or unspecified, the cell does not contain a list. Otherwise, application must split the string value of the cell on the specified separator character and parse each of the resulting strings separately. The cell's value will then be a list. Conversion specifications must use the separator to determine the conversion of a cell into the target format. See 3.12 Parsing cells for more details.</t>
-  </si>
-  <si>
-    <t>A definition of the format of the cell, used when parsing the cell.</t>
+    <t>rdf:Property</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>predicate URL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Column</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>csvw</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>xsd:anyURI</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>datatype</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>dialect</t>
+  </si>
+  <si>
+    <t>doubleQuote</t>
+  </si>
+  <si>
+    <t>encoding</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>foreignKeys</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>headerColumnCount</t>
+  </si>
+  <si>
+    <t>headerRowCount</t>
+  </si>
+  <si>
+    <t>xsd:boolean</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>lineTerminator</t>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+  </si>
+  <si>
+    <t>ltr</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>The class of table/text directions.</t>
+  </si>
+  <si>
+    <t>rtl</t>
+  </si>
+  <si>
+    <t>left to right</t>
+  </si>
+  <si>
+    <t>right to left</t>
+  </si>
+  <si>
+    <t>default direction</t>
+  </si>
+  <si>
+    <t>Indicates text should be processed left to right.</t>
+  </si>
+  <si>
+    <t>Indiects text should be processed right to left</t>
+  </si>
+  <si>
+    <t>Indicates to use the default text direction.</t>
+  </si>
+  <si>
+    <t>comment prefix</t>
+  </si>
+  <si>
+    <t>double quote</t>
+  </si>
+  <si>
+    <t>foreign keys</t>
+  </si>
+  <si>
+    <t>header column count</t>
+  </si>
+  <si>
+    <t>header row count</t>
+  </si>
+  <si>
+    <t>line terminator</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>primaryKey</t>
+  </si>
+  <si>
+    <t>quoteChar</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>skipBlankRows</t>
+  </si>
+  <si>
+    <t>skipColumns</t>
+  </si>
+  <si>
+    <t>skipInitialSpace</t>
+  </si>
+  <si>
+    <t>skipRows</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>separator</t>
+  </si>
+  <si>
+    <t>table-direction</t>
+  </si>
+  <si>
+    <t>text-direction</t>
+  </si>
+  <si>
+    <t>xsd:nonNegativeInteger</t>
+  </si>
+  <si>
+    <t>templates</t>
+  </si>
+  <si>
+    <t>targetFormat</t>
+  </si>
+  <si>
+    <t>templateFormat</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>trim</t>
+  </si>
+  <si>
+    <t>uriTemplate</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>minLength</t>
+  </si>
+  <si>
+    <t>maxLength</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>minInclusive</t>
+  </si>
+  <si>
+    <t>maxInclusive</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>subClassOf</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>dcat</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dcat#</t>
+  </si>
+  <si>
+    <t>qb</t>
+  </si>
+  <si>
+    <t>grddl</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>owl</t>
+  </si>
+  <si>
+    <t>prov</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>rdfa</t>
+  </si>
+  <si>
+    <t>rdfs</t>
+  </si>
+  <si>
+    <t>rif</t>
+  </si>
+  <si>
+    <t>rr</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>skos</t>
+  </si>
+  <si>
+    <t>skosxl</t>
+  </si>
+  <si>
+    <t>wdr</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>wrds</t>
+  </si>
+  <si>
+    <t>xhv</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <t>gldp</t>
+  </si>
+  <si>
+    <t>cnt</t>
+  </si>
+  <si>
+    <t>earl</t>
+  </si>
+  <si>
+    <t>ht</t>
+  </si>
+  <si>
+    <t>ptr</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>ctag</t>
+  </si>
+  <si>
+    <t>dc11</t>
+  </si>
+  <si>
+    <t>foaf</t>
+  </si>
+  <si>
+    <t>gr</t>
+  </si>
+  <si>
+    <t>ical</t>
+  </si>
+  <si>
+    <t>og</t>
+  </si>
+  <si>
+    <t>rev</t>
+  </si>
+  <si>
+    <t>sioc</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>vcard</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>http://purl.org/linked-data/cube#</t>
+  </si>
+  <si>
+    <t>An array of Column Descriptions.</t>
+  </si>
+  <si>
+    <t>An array of table descriptions for the tables in the group.</t>
+  </si>
+  <si>
+    <t>TableGroup,Table</t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (inclusive).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
+  </si>
+  <si>
+    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
+  </si>
+  <si>
+    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>The character that is used around escaped cells.</t>
+  </si>
+  <si>
+    <t>If true, sets the escape character flag to ". If false, to \.</t>
+  </si>
+  <si>
+    <t>delimieter</t>
+  </si>
+  <si>
+    <t>delimiter</t>
+  </si>
+  <si>
+    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
+  </si>
+  <si>
+    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
+  </si>
+  <si>
+    <t>The character that is used at the end of a row. The default is CRLF.</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>describedby</t>
+  </si>
+  <si>
+    <t>wrds:describedby</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>xhv:license</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>xhv:role</t>
+  </si>
+  <si>
+    <t>TableGroup</t>
+  </si>
+  <si>
+    <t>rdfs:Class</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Dialect</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Table Group Description</t>
+  </si>
+  <si>
+    <t>Table Description</t>
+  </si>
+  <si>
+    <t>A table description is a JSON object that describes a table within a CSV file.</t>
+  </si>
+  <si>
+    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
+  </si>
+  <si>
+    <t>Indicates whether to ignore wholly empty rows (ie rows in which all the cells are empty). The default is false.</t>
+  </si>
+  <si>
+    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
+  </si>
+  <si>
+    <t>A Column Description describes a single column.</t>
+  </si>
+  <si>
+    <t>Column Description</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>commentPrefix</t>
+  </si>
+  <si>
+    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
+  </si>
+  <si>
+    <t>The maximum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+  </si>
+  <si>
+    <t>rdfs:Literal</t>
+  </si>
+  <si>
+    <t>A literal containing JSON.</t>
+  </si>
+  <si>
+    <t>If true, sets the trim flag to "start". If false, to false.</t>
+  </si>
+  <si>
+    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
+  </si>
+  <si>
+    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
+  </si>
+  <si>
+    <t>If included, the format to which the tabular data should be transformed prior to the transformation using the template. If the value is "json", the tabular data should first be transformed first to JSON based on the simple mapping defined in Generating JSON from Tabular Data on the Web. If the value is "rdf", it should similarly first be transformed to XML based on the simple mapping defined in Generating RDF from Tabular Data on the Web. If the source property is missing or null then the source of the transformation is the annotated tabular data model.</t>
+  </si>
+  <si>
+    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
+  </si>
+  <si>
+    <t>minExclusive</t>
+  </si>
+  <si>
+    <t>maxExclusive</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>xsd:double</t>
+  </si>
+  <si>
+    <t>xsd:base64Binary</t>
+  </si>
+  <si>
+    <t>xsd:dateTime</t>
+  </si>
+  <si>
+    <t>xsd:anySimpleType</t>
+  </si>
+  <si>
+    <t>rdf:XMLLiteral</t>
+  </si>
+  <si>
+    <t>rdf:HTML</t>
   </si>
   <si>
     <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
@@ -69,12 +726,6 @@
   </si>
   <si>
     <t>The maximum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>csvm:minInclusive</t>
-  </si>
-  <si>
-    <t>csvm:maxInclusive</t>
   </si>
   <si>
     <t>An array of foreign key definitions that define how the values from specified columns within this table link to rows within this table or other tables. A foreign key definition is a JSON object with the properties:
@@ -151,696 +802,46 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
-  </si>
-  <si>
-    <t>The maximum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t>rdfs:Datatype</t>
-  </si>
-  <si>
-    <t>rdfs:Literal</t>
-  </si>
-  <si>
-    <t>A literal containing JSON.</t>
-  </si>
-  <si>
-    <t>If true, sets the trim flag to "start". If false, to false.</t>
-  </si>
-  <si>
-    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
-  </si>
-  <si>
-    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
-  </si>
-  <si>
-    <t>If included, the format to which the tabular data should be transformed prior to the transformation using the template. If the value is "json", the tabular data should first be transformed first to JSON based on the simple mapping defined in Generating JSON from Tabular Data on the Web. If the value is "rdf", it should similarly first be transformed to XML based on the simple mapping defined in Generating RDF from Tabular Data on the Web. If the source property is missing or null then the source of the transformation is the annotated tabular data model.</t>
-  </si>
-  <si>
-    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
-  </si>
-  <si>
-    <t>minExclusive</t>
-  </si>
-  <si>
-    <t>maxExclusive</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>binary</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
-    <t>xsd:double</t>
-  </si>
-  <si>
-    <t>xsd:base64Binary</t>
-  </si>
-  <si>
-    <t>xsd:dateTime</t>
-  </si>
-  <si>
-    <t>xsd:anySimpleType</t>
-  </si>
-  <si>
-    <t>rdf:XMLLiteral</t>
-  </si>
-  <si>
-    <t>rdf:HTML</t>
-  </si>
-  <si>
-    <t>An array of Column Descriptions.</t>
-  </si>
-  <si>
-    <t>An array of table descriptions for the tables in the group.</t>
-  </si>
-  <si>
-    <t>TableGroup,Table</t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (inclusive).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
-  </si>
-  <si>
-    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
-  </si>
-  <si>
-    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>The character that is used around escaped cells.</t>
-  </si>
-  <si>
-    <t>If true, sets the escape character flag to ". If false, to \.</t>
-  </si>
-  <si>
-    <t>delimieter</t>
-  </si>
-  <si>
-    <t>delimiter</t>
-  </si>
-  <si>
-    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
-  </si>
-  <si>
-    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
-  </si>
-  <si>
-    <t>The character that is used at the end of a row. The default is CRLF.</t>
-  </si>
-  <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>describedby</t>
-  </si>
-  <si>
-    <t>wrds:describedby</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
-    <t>xhv:license</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>xhv:role</t>
-  </si>
-  <si>
-    <t>TableGroup</t>
-  </si>
-  <si>
-    <t>rdfs:Class</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Dialect</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Schema</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Table Group Description</t>
-  </si>
-  <si>
-    <t>Table Description</t>
-  </si>
-  <si>
-    <t>A table description is a JSON object that describes a table within a CSV file.</t>
-  </si>
-  <si>
-    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
-  </si>
-  <si>
-    <t>Indicates whether to ignore wholly empty rows (ie rows in which all the cells are empty). The default is false.</t>
-  </si>
-  <si>
-    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
-  </si>
-  <si>
-    <t>A Column Description describes a single column.</t>
-  </si>
-  <si>
-    <t>Column Description</t>
-  </si>
-  <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>commentPrefix</t>
-  </si>
-  <si>
-    <t>xsd:anyURI</t>
+    <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
+</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>datatype</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>dialect</t>
-  </si>
-  <si>
-    <t>doubleQuote</t>
-  </si>
-  <si>
-    <t>encoding</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>foreignKeys</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>headerColumnCount</t>
-  </si>
-  <si>
-    <t>headerRowCount</t>
-  </si>
-  <si>
-    <t>xsd:boolean</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>lineTerminator</t>
-  </si>
-  <si>
-    <t>rdf:Property</t>
-  </si>
-  <si>
-    <t>ltr</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>The class of table/text directions.</t>
-  </si>
-  <si>
-    <t>rtl</t>
-  </si>
-  <si>
-    <t>left to right</t>
-  </si>
-  <si>
-    <t>right to left</t>
-  </si>
-  <si>
-    <t>default direction</t>
-  </si>
-  <si>
-    <t>Indicates text should be processed left to right.</t>
-  </si>
-  <si>
-    <t>Indiects text should be processed right to left</t>
-  </si>
-  <si>
-    <t>Indicates to use the default text direction.</t>
-  </si>
-  <si>
-    <t>comment prefix</t>
-  </si>
-  <si>
-    <t>double quote</t>
-  </si>
-  <si>
-    <t>foreign keys</t>
-  </si>
-  <si>
-    <t>header column count</t>
-  </si>
-  <si>
-    <t>header row count</t>
-  </si>
-  <si>
-    <t>line terminator</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>primaryKey</t>
-  </si>
-  <si>
-    <t>quoteChar</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>resources</t>
-  </si>
-  <si>
-    <t>skipBlankRows</t>
-  </si>
-  <si>
-    <t>skipColumns</t>
-  </si>
-  <si>
-    <t>skipInitialSpace</t>
-  </si>
-  <si>
-    <t>skipRows</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>separator</t>
-  </si>
-  <si>
-    <t>table-direction</t>
-  </si>
-  <si>
-    <t>text-direction</t>
-  </si>
-  <si>
-    <t>xsd:nonNegativeInteger</t>
-  </si>
-  <si>
-    <t>templates</t>
-  </si>
-  <si>
-    <t>targetFormat</t>
-  </si>
-  <si>
-    <t>templateFormat</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>trim</t>
-  </si>
-  <si>
-    <t>uriTemplate</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>minLength</t>
-  </si>
-  <si>
-    <t>maxLength</t>
-  </si>
-  <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t>minInclusive</t>
-  </si>
-  <si>
-    <t>maxInclusive</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>subClassOf</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>dcat</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/dcat#</t>
-  </si>
-  <si>
-    <t>csvm</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/csvm#</t>
-  </si>
-  <si>
-    <t>qb</t>
-  </si>
-  <si>
-    <t>grddl</t>
-  </si>
-  <si>
-    <t>ma</t>
-  </si>
-  <si>
-    <t>org</t>
-  </si>
-  <si>
-    <t>owl</t>
-  </si>
-  <si>
-    <t>prov</t>
-  </si>
-  <si>
-    <t>rdf</t>
-  </si>
-  <si>
-    <t>rdfa</t>
-  </si>
-  <si>
-    <t>rdfs</t>
-  </si>
-  <si>
-    <t>rif</t>
-  </si>
-  <si>
-    <t>rr</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>skos</t>
-  </si>
-  <si>
-    <t>skosxl</t>
-  </si>
-  <si>
-    <t>wdr</t>
-  </si>
-  <si>
-    <t>void</t>
-  </si>
-  <si>
-    <t>wrds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of csvm:rtl csvm:ltr or csvm:default. Indicates whether the tables in the group should be displayed with the first column on the right, on the left, or based on the first character in the table that has a specific direction. </t>
-  </si>
-  <si>
-    <t>xhv</t>
-  </si>
-  <si>
-    <t>xml</t>
-  </si>
-  <si>
-    <t>xsd</t>
-  </si>
-  <si>
-    <t>gldp</t>
-  </si>
-  <si>
-    <t>cnt</t>
-  </si>
-  <si>
-    <t>earl</t>
-  </si>
-  <si>
-    <t>ht</t>
-  </si>
-  <si>
-    <t>ptr</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>ctag</t>
-  </si>
-  <si>
-    <t>dc11</t>
-  </si>
-  <si>
-    <t>foaf</t>
-  </si>
-  <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>ical</t>
-  </si>
-  <si>
-    <t>og</t>
-  </si>
-  <si>
-    <t>rev</t>
-  </si>
-  <si>
-    <t>sioc</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>vcard</t>
-  </si>
-  <si>
-    <t>schema</t>
-  </si>
-  <si>
-    <t>http://purl.org/linked-data/cube#</t>
-  </si>
-  <si>
-    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
+    <t>A character that, when it appears at the beginning of a skipped row, indicates a comment that should be associated as a comment annotation to the table. The default is "#".</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>required</t>
+    <t>The number of header rows (following the skipped rows) in the file. The default is 1.</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>http://www.w3.org/2003/g/data-view#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/ma-ont#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/org#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2002/07/owl#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/prov#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/rdfa#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2000/01/rdf-schema#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2007/rif#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/r2rml#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/sparql-service-description#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2004/02/skos/core#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2008/05/skos-xl#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2007/05/powder#</t>
-  </si>
-  <si>
-    <t>http://rdfs.org/ns/void#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2007/05/powder-s#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/1999/xhtml/vocab#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/XML/1998/namespace</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2001/XMLSchema#</t>
-  </si>
-  <si>
-    <t>dcterms</t>
-  </si>
-  <si>
-    <t>dc</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/people#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2008/content#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/earl#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2006/http#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2009/pointers#</t>
-  </si>
-  <si>
-    <t>http://creativecommons.org/ns#</t>
-  </si>
-  <si>
-    <t>http://commontag.org/ns#</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/terms/</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/elements/1.1/</t>
-  </si>
-  <si>
-    <t>http://xmlns.com/foaf/0.1/</t>
-  </si>
-  <si>
-    <t>http://purl.org/goodrelations/v1#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2002/12/cal/icaltzd#</t>
-  </si>
-  <si>
-    <t>http://ogp.me/ns#</t>
-  </si>
-  <si>
-    <t>http://purl.org/stuff/rev#</t>
-  </si>
-  <si>
-    <t>http://rdfs.org/sioc/ns#</t>
-  </si>
-  <si>
-    <t>http://rdf.data-vocabulary.org/#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2006/vcard/ns#</t>
-  </si>
-  <si>
-    <t>http://schema.org/</t>
-  </si>
-  <si>
-    <t>A Table Group Description describes a group of Tables.</t>
-  </si>
-  <si>
-    <t>Dialect Description</t>
-  </si>
-  <si>
-    <t>A Dialect Description provides hints to parsers about how to parse a linked file.</t>
-  </si>
-  <si>
-    <t>Template Specification</t>
-  </si>
-  <si>
-    <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
-  </si>
-  <si>
-    <t>predicateUrl</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>rdf:Property</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>predicate URL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Column</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
+For a Column: A natural language property that provides possible alternative names for the column.</t>
+  </si>
+  <si>
+    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
+  </si>
+  <si>
+    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
+  </si>
+  <si>
+    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
+  </si>
+  <si>
+    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
+  </si>
+  <si>
+    <t>The character used to separate items in the string value of the cell. If null or unspecified, the cell does not contain a list. Otherwise, application must split the string value of the cell on the specified separator character and parse each of the resulting strings separately. The cell's value will then be a list. Conversion specifications must use the separator to determine the conversion of a cell into the target format. See 3.12 Parsing cells for more details.</t>
+  </si>
+  <si>
+    <t>A definition of the format of the cell, used when parsing the cell.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -896,6 +897,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -919,7 +927,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -935,6 +943,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -942,7 +951,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -1267,15 +1276,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
@@ -1284,22 +1293,22 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"@type"</f>
@@ -1310,1034 +1319,1034 @@
         <v>@container</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>215</v>
+        <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>127</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>242</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>238</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>174</v>
+        <v>124</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>243</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>244</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>245</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>244</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>239</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>246</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>247</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>240</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>248</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>217</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>249</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>219</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>220</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>241</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>221</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>222</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>223</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>250</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>224</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>225</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>254</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>226</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>251</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>227</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>228</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>252</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>253</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>230</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>229</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>191</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>231</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>232</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>233</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>234</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="3" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="E46" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="F46" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="H46" t="str">
         <f>"@list"</f>
         <v>@list</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="60">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>204</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>1</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="60">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>11</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="E49" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>37</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="E50" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="F50" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="G50" s="8"/>
       <c r="J50" s="5" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="E51" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F51" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="E52" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="409">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="E53" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30">
       <c r="A54" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>10</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E55" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F55" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="45">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C56" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="E56" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F56" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>0</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="E57" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F57" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>2</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="E58" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>7</v>
+        <v>261</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="F59" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>12</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="E60" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>49</v>
+        <v>216</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>251</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J61" t="s">
-        <v>39</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>33</v>
+        <v>249</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J62" t="s">
-        <v>66</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>247</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="F63" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>215</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>34</v>
+        <v>250</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J64" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>32</v>
+        <v>248</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J65" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>246</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="F66" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>13</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="75">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="E67" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="I67" t="b">
         <v>1</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="45">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="E68" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>70</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="E69" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>6</v>
+        <v>260</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="45">
       <c r="A70" t="s">
-        <v>260</v>
+        <v>51</v>
       </c>
       <c r="B70" t="s">
-        <v>261</v>
+        <v>52</v>
       </c>
       <c r="C70" t="s">
-        <v>262</v>
+        <v>53</v>
       </c>
       <c r="E70" t="s">
-        <v>263</v>
+        <v>54</v>
       </c>
       <c r="F70" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>214</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="45">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>235</v>
       </c>
       <c r="E71" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>236</v>
       </c>
       <c r="E72" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="30">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="F73" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>5</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="30">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="B74" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="F74" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="H74" t="str">
         <f>"@set"</f>
@@ -2347,539 +2356,539 @@
         <v>1</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="45">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="E75" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="F75" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="135">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="45">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C77" t="s">
-        <v>21</v>
+        <v>237</v>
       </c>
       <c r="E77" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F77" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="45">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>238</v>
       </c>
       <c r="E78" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F78" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>239</v>
       </c>
       <c r="E79" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F79" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="30">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C80" t="s">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="E80" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F80" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>76</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="180">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C81" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="E81" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>46</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="75">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C82" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="E82" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="F82" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="G82" t="str">
         <f>"@vocab"</f>
         <v>@vocab</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>192</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="120">
       <c r="A83" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>243</v>
       </c>
       <c r="E83" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="120">
       <c r="A84" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>244</v>
       </c>
       <c r="E84" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>45</v>
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="45">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="E85" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="F85" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="45">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C86" t="s">
-        <v>26</v>
+        <v>242</v>
       </c>
       <c r="E86" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="F86" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="G86" t="str">
         <f>"@vocab"</f>
         <v>@vocab</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="135">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="B87" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C87" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="E87" t="s">
-        <v>36</v>
+        <v>252</v>
       </c>
       <c r="H87" t="str">
         <f>"@language"</f>
         <v>@language</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>3</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="30">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C88" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="E88" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="F88" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>4</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="45">
       <c r="A89" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="C89" t="s">
-        <v>29</v>
+        <v>245</v>
       </c>
       <c r="E89" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>18</v>
+        <v>234</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="B90" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C90" t="s">
-        <v>100</v>
+        <v>202</v>
       </c>
       <c r="J90" s="5" t="s">
-        <v>99</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="30">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="B91" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C91" t="s">
-        <v>256</v>
+        <v>47</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>257</v>
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="B92" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C92" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>120</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="30">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>98</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="30">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="B94" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C94" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="30">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>195</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="45">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="B96" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C96" t="s">
-        <v>258</v>
+        <v>49</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>259</v>
+        <v>50</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>222</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="C97" t="s">
-        <v>55</v>
+        <v>222</v>
       </c>
       <c r="D97" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B98" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D98" t="s">
-        <v>59</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>218</v>
       </c>
       <c r="B99" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D99" t="s">
-        <v>57</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>52</v>
+        <v>219</v>
       </c>
       <c r="B100" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D100" t="s">
-        <v>58</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
       <c r="B101" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D101" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" t="s">
-        <v>54</v>
+        <v>221</v>
       </c>
       <c r="B102" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D102" t="s">
-        <v>61</v>
+        <v>228</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="B103" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D103" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="B104" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D104" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E104" s="6"/>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="B105" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E105" s="6"/>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>50</v>
+        <v>217</v>
       </c>
       <c r="B106" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D106" t="s">
-        <v>56</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="B107" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D107" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B108" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="D108" t="s">
-        <v>60</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2931,9 +2940,8 @@
     <hyperlink ref="D33" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Fix delimiter misspelling in _vocab.xlsx too.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -104,292 +104,239 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
+    <t>delimeter</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
+  </si>
+  <si>
+    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
+  </si>
+  <si>
+    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
+  </si>
+  <si>
+    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
+  </si>
+  <si>
+    <t>A definition of the format of the cell, used when parsing the cell.</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>xsd:double</t>
+  </si>
+  <si>
+    <t>xsd:base64Binary</t>
+  </si>
+  <si>
+    <t>rev</t>
+  </si>
+  <si>
+    <t>sioc</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>vcard</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>rdf:XMLLiteral</t>
+  </si>
+  <si>
+    <t>rdf:HTML</t>
+  </si>
+  <si>
+    <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
+  </si>
+  <si>
+    <t>The exact length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>The minimum length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>The maximum length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>A URI template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
+  </si>
+  <si>
+    <t>primary key</t>
+  </si>
+  <si>
+    <t>quote char</t>
+  </si>
+  <si>
+    <t>skip blank rows</t>
+  </si>
+  <si>
+    <t>skip columns</t>
+  </si>
+  <si>
+    <t>skip initial space</t>
+  </si>
+  <si>
+    <t>skip rows</t>
+  </si>
+  <si>
+    <t>table direction</t>
+  </si>
+  <si>
+    <t>text direction</t>
+  </si>
+  <si>
+    <t>target format</t>
+  </si>
+  <si>
+    <t>template format</t>
+  </si>
+  <si>
+    <t>uri template</t>
+  </si>
+  <si>
+    <t>min length</t>
+  </si>
+  <si>
+    <t>max length</t>
+  </si>
+  <si>
+    <t>min inclusive</t>
+  </si>
+  <si>
+    <t>max inclusive</t>
+  </si>
+  <si>
+    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
+  </si>
+  <si>
+    <t>A Table Group Description describes a group of Tables.</t>
+  </si>
+  <si>
+    <t>Dialect Description</t>
+  </si>
+  <si>
+    <t>Column Description</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
+  </si>
+  <si>
+    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
+  </si>
+  <si>
+    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
+  </si>
+  <si>
+    <t>minExclusive</t>
+  </si>
+  <si>
+    <t>maxExclusive</t>
+  </si>
+  <si>
+    <t>ctag</t>
+  </si>
+  <si>
+    <t>dc11</t>
+  </si>
+  <si>
+    <t>foaf</t>
+  </si>
+  <si>
+    <t>gr</t>
+  </si>
+  <si>
+    <t>ical</t>
+  </si>
+  <si>
+    <t>og</t>
+  </si>
+  <si>
+    <t>xhv</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <t>gldp</t>
+  </si>
+  <si>
+    <t>cnt</t>
+  </si>
+  <si>
+    <t>earl</t>
+  </si>
+  <si>
+    <t>ht</t>
+  </si>
+  <si>
+    <t>ptr</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/csvw#</t>
+  </si>
+  <si>
+    <t>http://purl.org/linked-data/cube#</t>
+  </si>
+  <si>
+    <t>An array of Column Descriptions.</t>
+  </si>
+  <si>
+    <t>An array of table descriptions for the tables in the group.</t>
+  </si>
+  <si>
+    <t>TableGroup,Table</t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (inclusive).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
+  </si>
+  <si>
+    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
     <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
 For a Column: A natural language property that provides possible alternative names for the column.</t>
   </si>
   <si>
-    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
-  </si>
-  <si>
-    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
-  </si>
-  <si>
-    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
-  </si>
-  <si>
-    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
-  </si>
-  <si>
-    <t>A definition of the format of the cell, used when parsing the cell.</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>binary</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
-    <t>xsd:double</t>
-  </si>
-  <si>
-    <t>xsd:base64Binary</t>
-  </si>
-  <si>
-    <t>rev</t>
-  </si>
-  <si>
-    <t>sioc</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>vcard</t>
-  </si>
-  <si>
-    <t>schema</t>
-  </si>
-  <si>
-    <t>rdf:XMLLiteral</t>
-  </si>
-  <si>
-    <t>rdf:HTML</t>
-  </si>
-  <si>
-    <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
-  </si>
-  <si>
-    <t>The exact length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>The minimum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>The maximum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>A URI template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
-  </si>
-  <si>
-    <t>primary key</t>
-  </si>
-  <si>
-    <t>quote char</t>
-  </si>
-  <si>
-    <t>skip blank rows</t>
-  </si>
-  <si>
-    <t>skip columns</t>
-  </si>
-  <si>
-    <t>skip initial space</t>
-  </si>
-  <si>
-    <t>skip rows</t>
-  </si>
-  <si>
-    <t>table direction</t>
-  </si>
-  <si>
-    <t>text direction</t>
-  </si>
-  <si>
-    <t>target format</t>
-  </si>
-  <si>
-    <t>template format</t>
-  </si>
-  <si>
-    <t>uri template</t>
-  </si>
-  <si>
-    <t>min length</t>
-  </si>
-  <si>
-    <t>max length</t>
-  </si>
-  <si>
-    <t>min inclusive</t>
-  </si>
-  <si>
-    <t>max inclusive</t>
-  </si>
-  <si>
-    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
-  </si>
-  <si>
-    <t>A Table Group Description describes a group of Tables.</t>
-  </si>
-  <si>
-    <t>Dialect Description</t>
-  </si>
-  <si>
-    <t>Column Description</t>
-  </si>
-  <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>commentPrefix</t>
-  </si>
-  <si>
-    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
-  </si>
-  <si>
-    <t>The maximum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t>rdfs:Datatype</t>
-  </si>
-  <si>
-    <t>rdfs:Literal</t>
-  </si>
-  <si>
-    <t>A literal containing JSON.</t>
-  </si>
-  <si>
-    <t>If true, sets the trim flag to "start". If false, to false.</t>
-  </si>
-  <si>
-    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
-  </si>
-  <si>
-    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
-  </si>
-  <si>
-    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
-  </si>
-  <si>
-    <t>minExclusive</t>
-  </si>
-  <si>
-    <t>maxExclusive</t>
-  </si>
-  <si>
-    <t>ctag</t>
-  </si>
-  <si>
-    <t>dc11</t>
-  </si>
-  <si>
-    <t>foaf</t>
-  </si>
-  <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>ical</t>
-  </si>
-  <si>
-    <t>og</t>
-  </si>
-  <si>
-    <t>xhv</t>
-  </si>
-  <si>
-    <t>xml</t>
-  </si>
-  <si>
-    <t>xsd</t>
-  </si>
-  <si>
-    <t>gldp</t>
-  </si>
-  <si>
-    <t>cnt</t>
-  </si>
-  <si>
-    <t>earl</t>
-  </si>
-  <si>
-    <t>ht</t>
-  </si>
-  <si>
-    <t>ptr</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/csvw#</t>
-  </si>
-  <si>
-    <t>http://purl.org/linked-data/cube#</t>
-  </si>
-  <si>
-    <t>An array of Column Descriptions.</t>
-  </si>
-  <si>
-    <t>An array of table descriptions for the tables in the group.</t>
-  </si>
-  <si>
-    <t>TableGroup,Table</t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (inclusive).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
-  </si>
-  <si>
-    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
-  </si>
-  <si>
-    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>The character that is used around escaped cells.</t>
-  </si>
-  <si>
-    <t>delimieter</t>
-  </si>
-  <si>
-    <t>delimiter</t>
-  </si>
-  <si>
-    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
-  </si>
-  <si>
-    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
-  </si>
-  <si>
-    <t>The character that is used at the end of a row. The default is CRLF.</t>
-  </si>
-  <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>describedby</t>
-  </si>
-  <si>
-    <t>wrds:describedby</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
     <t>xhv:license</t>
   </si>
   <si>
@@ -516,106 +463,25 @@
     <t>headerColumnCount</t>
   </si>
   <si>
-    <t>headerRowCount</t>
-  </si>
-  <si>
-    <t>xsd:boolean</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>lineTerminator</t>
-  </si>
-  <si>
-    <t>rdf:Property</t>
-  </si>
-  <si>
-    <t>ltr</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>The class of table/text directions.</t>
-  </si>
-  <si>
-    <t>rtl</t>
-  </si>
-  <si>
-    <t>left to right</t>
-  </si>
-  <si>
-    <t>right to left</t>
-  </si>
-  <si>
-    <t>Indicates text should be processed left to right.</t>
-  </si>
-  <si>
-    <t>Indiects text should be processed right to left</t>
-  </si>
-  <si>
-    <t>comment prefix</t>
-  </si>
-  <si>
-    <t>double quote</t>
-  </si>
-  <si>
-    <t>foreign keys</t>
-  </si>
-  <si>
-    <t>header column count</t>
-  </si>
-  <si>
-    <t>header row count</t>
-  </si>
-  <si>
-    <t>line terminator</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>primaryKey</t>
-  </si>
-  <si>
-    <t>quoteChar</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>resources</t>
-  </si>
-  <si>
-    <t>skipBlankRows</t>
-  </si>
-  <si>
-    <t>skipColumns</t>
-  </si>
-  <si>
-    <t>skipInitialSpace</t>
-  </si>
-  <si>
-    <t>skipRows</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>separator</t>
-  </si>
-  <si>
-    <t>table-direction</t>
-  </si>
-  <si>
-    <t>text-direction</t>
+    <t>commentPrefix</t>
+  </si>
+  <si>
+    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
+  </si>
+  <si>
+    <t>The maximum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+  </si>
+  <si>
+    <t>rdfs:Literal</t>
+  </si>
+  <si>
+    <t>A literal containing JSON.</t>
+  </si>
+  <si>
+    <t>If true, sets the trim flag to "start". If false, to false.</t>
   </si>
   <si>
     <t>xsd:nonNegativeInteger</t>
@@ -765,6 +631,39 @@
     <t>csvw:minInclusive</t>
   </si>
   <si>
+    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
+  </si>
+  <si>
+    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>The character that is used around escaped cells.</t>
+  </si>
+  <si>
+    <t>delimiter</t>
+  </si>
+  <si>
+    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
+  </si>
+  <si>
+    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
+  </si>
+  <si>
+    <t>The character that is used at the end of a row. The default is CRLF.</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>describedby</t>
+  </si>
+  <si>
+    <t>wrds:describedby</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
     <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -864,18 +763,114 @@
   </si>
   <si>
     <t>http://xmlns.com/foaf/0.1/</t>
+  </si>
+  <si>
+    <t>headerRowCount</t>
+  </si>
+  <si>
+    <t>xsd:boolean</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>lineTerminator</t>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+  </si>
+  <si>
+    <t>ltr</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>The class of table/text directions.</t>
+  </si>
+  <si>
+    <t>rtl</t>
+  </si>
+  <si>
+    <t>left to right</t>
+  </si>
+  <si>
+    <t>right to left</t>
+  </si>
+  <si>
+    <t>Indicates text should be processed left to right.</t>
+  </si>
+  <si>
+    <t>Indiects text should be processed right to left</t>
+  </si>
+  <si>
+    <t>comment prefix</t>
+  </si>
+  <si>
+    <t>double quote</t>
+  </si>
+  <si>
+    <t>foreign keys</t>
+  </si>
+  <si>
+    <t>header column count</t>
+  </si>
+  <si>
+    <t>header row count</t>
+  </si>
+  <si>
+    <t>line terminator</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>primaryKey</t>
+  </si>
+  <si>
+    <t>quoteChar</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>skipBlankRows</t>
+  </si>
+  <si>
+    <t>skipColumns</t>
+  </si>
+  <si>
+    <t>skipInitialSpace</t>
+  </si>
+  <si>
+    <t>skipRows</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>separator</t>
+  </si>
+  <si>
+    <t>table-direction</t>
+  </si>
+  <si>
+    <t>text-direction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="9">
     <font>
       <sz val="12"/>
@@ -1315,8 +1310,8 @@
   <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J83" sqref="J83"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1328,22 +1323,22 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>207</v>
+        <v>162</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>211</v>
+        <v>166</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"@type"</f>
@@ -1354,313 +1349,313 @@
         <v>@container</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>247</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>248</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>169</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1668,32 +1663,32 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1701,21 +1696,21 @@
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1723,32 +1718,32 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>227</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1756,10 +1751,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1767,76 +1762,76 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="B39" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="B41" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1844,37 +1839,37 @@
         <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C45" t="s">
         <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F45" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="H45" t="str">
         <f>"@list"</f>
         <v>@list</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="60">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C46" t="s">
-        <v>170</v>
+        <v>251</v>
       </c>
       <c r="E46" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>20</v>
@@ -1882,16 +1877,16 @@
     </row>
     <row r="47" spans="1:10" ht="60">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E47" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J47" s="5" t="s">
         <v>43</v>
@@ -1899,33 +1894,33 @@
     </row>
     <row r="48" spans="1:10" ht="75">
       <c r="A48" t="s">
-        <v>233</v>
+        <v>188</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C48" t="s">
-        <v>233</v>
+        <v>188</v>
       </c>
       <c r="E48" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>234</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="E49" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>18</v>
@@ -1933,40 +1928,40 @@
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="E50" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F50" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G50" s="8"/>
       <c r="J50" s="5" t="s">
-        <v>106</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>252</v>
       </c>
       <c r="E51" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F51" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>11</v>
@@ -1974,33 +1969,33 @@
     </row>
     <row r="52" spans="1:10" ht="30">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E52" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>111</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>253</v>
       </c>
       <c r="E53" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>12</v>
@@ -2008,16 +2003,16 @@
     </row>
     <row r="54" spans="1:10" ht="30">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C54" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J54" s="5" t="s">
         <v>27</v>
@@ -2025,36 +2020,36 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C55" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="E55" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F55" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="45">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C56" t="s">
-        <v>173</v>
+        <v>254</v>
       </c>
       <c r="E56" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F56" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J56" s="5" t="s">
         <v>19</v>
@@ -2062,19 +2057,19 @@
     </row>
     <row r="57" spans="1:10" ht="30">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C57" t="s">
-        <v>174</v>
+        <v>255</v>
       </c>
       <c r="E57" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F57" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J57" s="5" t="s">
         <v>21</v>
@@ -2082,16 +2077,16 @@
     </row>
     <row r="58" spans="1:10" ht="30">
       <c r="A58" t="s">
-        <v>159</v>
+        <v>240</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>240</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J58" s="5" t="s">
         <v>26</v>
@@ -2099,19 +2094,19 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C59" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="F59" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J59" s="5" t="s">
         <v>44</v>
@@ -2119,70 +2114,70 @@
     </row>
     <row r="60" spans="1:10" ht="30">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>241</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C60" t="s">
-        <v>175</v>
+        <v>256</v>
       </c>
       <c r="E60" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J61" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C62" t="s">
         <v>62</v>
       </c>
       <c r="E62" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J62" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C63" t="s">
         <v>60</v>
       </c>
       <c r="E63" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="F63" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J63" s="5" t="s">
         <v>46</v>
@@ -2190,53 +2185,53 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C64" t="s">
         <v>15</v>
       </c>
       <c r="E64" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J64" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C65" t="s">
         <v>61</v>
       </c>
       <c r="E65" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J65" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C66" t="s">
         <v>59</v>
       </c>
       <c r="E66" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="F66" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>45</v>
@@ -2244,53 +2239,53 @@
     </row>
     <row r="67" spans="1:10" ht="75">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>257</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>257</v>
       </c>
       <c r="E67" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I67" t="b">
         <v>1</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="45">
       <c r="A68" t="s">
-        <v>177</v>
+        <v>258</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>258</v>
       </c>
       <c r="E68" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>105</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30">
       <c r="A69" t="s">
-        <v>178</v>
+        <v>259</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>259</v>
       </c>
       <c r="E69" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J69" s="5" t="s">
         <v>25</v>
@@ -2298,73 +2293,73 @@
     </row>
     <row r="70" spans="1:10" ht="45">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="E70" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="F70" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="45">
       <c r="A71" t="s">
-        <v>179</v>
+        <v>260</v>
       </c>
       <c r="B71" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C71" t="s">
         <v>48</v>
       </c>
       <c r="E71" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>180</v>
+        <v>261</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C72" t="s">
         <v>49</v>
       </c>
       <c r="E72" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="30">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>262</v>
       </c>
       <c r="B73" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C73" t="s">
-        <v>181</v>
+        <v>262</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="F73" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="J73" s="5" t="s">
         <v>24</v>
@@ -2372,19 +2367,19 @@
     </row>
     <row r="74" spans="1:10" ht="30">
       <c r="A74" t="s">
-        <v>182</v>
+        <v>263</v>
       </c>
       <c r="B74" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C74" t="s">
-        <v>182</v>
+        <v>263</v>
       </c>
       <c r="E74" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F74" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H74" t="str">
         <f>"@set"</f>
@@ -2394,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2426,33 +2421,33 @@
         <v>40</v>
       </c>
       <c r="B76" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C76" t="s">
         <v>40</v>
       </c>
       <c r="E76" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F76" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30">
       <c r="A77" t="s">
-        <v>188</v>
+        <v>269</v>
       </c>
       <c r="B77" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C77" t="s">
-        <v>188</v>
+        <v>269</v>
       </c>
       <c r="E77" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="J77" s="5" t="s">
         <v>13</v>
@@ -2460,96 +2455,96 @@
     </row>
     <row r="78" spans="1:10" ht="45">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>264</v>
       </c>
       <c r="B78" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C78" t="s">
         <v>50</v>
       </c>
       <c r="E78" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F78" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="45">
       <c r="A79" t="s">
-        <v>184</v>
+        <v>265</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C79" t="s">
         <v>51</v>
       </c>
       <c r="E79" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F79" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>266</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C80" t="s">
         <v>52</v>
       </c>
       <c r="E80" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F80" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="30">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C81" t="s">
         <v>53</v>
       </c>
       <c r="E81" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F81" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>110</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="135">
       <c r="A82" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C82" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="E82" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="J82" s="5" t="s">
         <v>0</v>
@@ -2584,115 +2579,115 @@
     </row>
     <row r="84" spans="1:10" ht="75">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>270</v>
       </c>
       <c r="B84" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C84" t="s">
         <v>54</v>
       </c>
       <c r="E84" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F84" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="G84" t="str">
         <f>"@vocab"</f>
         <v>@vocab</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>235</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="120">
       <c r="A85" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C85" t="s">
         <v>56</v>
       </c>
       <c r="E85" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="120">
       <c r="A86" t="s">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C86" t="s">
         <v>57</v>
       </c>
       <c r="E86" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="45">
       <c r="A87" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="B87" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C87" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E87" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F87" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="45">
       <c r="A88" t="s">
-        <v>190</v>
+        <v>271</v>
       </c>
       <c r="B88" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C88" t="s">
         <v>55</v>
       </c>
       <c r="E88" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="F88" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="G88" t="str">
         <f>"@vocab"</f>
         <v>@vocab</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="135">
       <c r="A89" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="E89" t="s">
         <v>17</v>
@@ -2702,24 +2697,24 @@
         <v>@language</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="30">
       <c r="A90" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="E90" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F90" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>23</v>
@@ -2727,16 +2722,16 @@
     </row>
     <row r="91" spans="1:10" ht="45">
       <c r="A91" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="C91" t="s">
         <v>58</v>
       </c>
       <c r="E91" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>47</v>
@@ -2744,10 +2739,10 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B92" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C92" t="s">
         <v>66</v>
@@ -2758,41 +2753,41 @@
     </row>
     <row r="93" spans="1:10" ht="30">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B93" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C93" t="s">
         <v>65</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="B94" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>164</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="30">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J95" s="5" t="s">
         <v>63</v>
@@ -2800,27 +2795,27 @@
     </row>
     <row r="96" spans="1:10" ht="30">
       <c r="A96" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="30">
       <c r="A97" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B97" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C97" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="J97" s="5" t="s">
         <v>64</v>
@@ -2828,16 +2823,16 @@
     </row>
     <row r="98" spans="1:10" ht="45">
       <c r="A98" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" t="s">
+        <v>103</v>
+      </c>
+      <c r="C98" t="s">
+        <v>123</v>
+      </c>
+      <c r="J98" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="B98" t="s">
-        <v>121</v>
-      </c>
-      <c r="C98" t="s">
-        <v>141</v>
-      </c>
-      <c r="J98" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -2845,16 +2840,16 @@
         <v>33</v>
       </c>
       <c r="B99" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="C99" t="s">
         <v>33</v>
       </c>
       <c r="D99" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -2862,7 +2857,7 @@
         <v>31</v>
       </c>
       <c r="B100" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D100" t="s">
         <v>2</v>
@@ -2873,7 +2868,7 @@
         <v>29</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D101" t="s">
         <v>35</v>
@@ -2884,7 +2879,7 @@
         <v>30</v>
       </c>
       <c r="B102" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
@@ -2892,13 +2887,13 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="B103" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D103" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -2906,7 +2901,7 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D104" t="s">
         <v>42</v>
@@ -2914,36 +2909,36 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="B105" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D105" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="B106" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D106" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="E106" s="6"/>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
+        <v>156</v>
+      </c>
+      <c r="B107" t="s">
         <v>201</v>
       </c>
-      <c r="B107" t="s">
-        <v>113</v>
-      </c>
       <c r="D107" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="E107" s="6"/>
     </row>
@@ -2952,7 +2947,7 @@
         <v>28</v>
       </c>
       <c r="B108" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D108" t="s">
         <v>34</v>
@@ -2960,28 +2955,27 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D109" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="D110" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A99:XFD109">
     <sortCondition ref="A99:A109"/>
   </sortState>

</xml_diff>

<commit_message>
Update uriTemplate in namespace to urlTemplate.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -21,6 +21,706 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="292">
   <si>
+    <t>A URL template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gYearMonth</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gYear</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gMonthDay</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gDay</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gMonth</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>hexBinary</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>base64Binary</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>anyURI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>sch</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
+  </si>
+  <si>
+    <t>Table Description</t>
+  </si>
+  <si>
+    <t>A table description is a JSON object that describes a table within a CSV file.</t>
+  </si>
+  <si>
+    <t>Table Group Description</t>
+  </si>
+  <si>
+    <t>A Table Group Description describes a group of Tables.</t>
+  </si>
+  <si>
+    <t>Template Specification</t>
+  </si>
+  <si>
+    <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+  </si>
+  <si>
+    <t>rdfs:Literal</t>
+  </si>
+  <si>
+    <t>A literal containing JSON.</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>xsd:anySimpleType</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>xsd:base64Binary</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>xsd:dateTime</t>
+  </si>
+  <si>
+    <t>describedby</t>
+  </si>
+  <si>
+    <t>wrds:describedby</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>rdf:HTML</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>xhv:license</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>csvw:maxInclusive</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>csvw:minInclusive</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>xsd:double</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>xhv:role</t>
+  </si>
+  <si>
+    <t>rdf:XMLLiteral</t>
+  </si>
+  <si>
+    <t>anySimpleType</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>normalizedString</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCName</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>decimal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonPositiveInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>negativeInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>long</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>short</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonNegativeInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedLong</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedInt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedShort</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedByte</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>positiveInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateTime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>urlTemplate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL template</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
+  </si>
+  <si>
+    <t>templateFormat</t>
+  </si>
+  <si>
+    <t>template format</t>
+  </si>
+  <si>
+    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
+  </si>
+  <si>
+    <t>templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
+  </si>
+  <si>
+    <t>text-direction</t>
+  </si>
+  <si>
+    <t>text direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of csvw:rtl or csvw:ltr. Indicates whether the text within cells should be displayed by default as left-to-right or right-to-left text. </t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Template,Column</t>
+  </si>
+  <si>
+    <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
+For a Column: A natural language property that provides possible alternative names for the column.</t>
+  </si>
+  <si>
+    <t>trim</t>
+  </si>
+  <si>
+    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
+  </si>
+  <si>
+    <t>rdfs:Class</t>
+  </si>
+  <si>
+    <t>Column Description</t>
+  </si>
+  <si>
+    <t>A Column Description describes a single column.</t>
+  </si>
+  <si>
+    <t>Dialect Description</t>
+  </si>
+  <si>
+    <t>A Dialect Description provides hints to parsers about how to parse a linked file.</t>
+  </si>
+  <si>
+    <t>The class of table/text directions.</t>
+  </si>
+  <si>
+    <t>Relates a Table to each Row output.</t>
+  </si>
+  <si>
+    <t>Indicates whether to ignore wholly empty rows (ie rows in which all the cells are empty). The default is false.</t>
+  </si>
+  <si>
+    <t>skipColumns</t>
+  </si>
+  <si>
+    <t>skip columns</t>
+  </si>
+  <si>
+    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
+  </si>
+  <si>
+    <t>skipInitialSpace</t>
+  </si>
+  <si>
+    <t>skip initial space</t>
+  </si>
+  <si>
+    <t>If true, sets the trim flag to "start". If false, to false.</t>
+  </si>
+  <si>
+    <t>skipRows</t>
+  </si>
+  <si>
+    <t>skip rows</t>
+  </si>
+  <si>
+    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>The format to which the tabular data should be transformed prior to the transformation using the template. If the value is "json", the tabular data should first be transformed first to JSON based on the simple mapping defined in Generating JSON from Tabular Data on the Web. If the value is "rdf", it should similarly first be transformed to XML based on the simple mapping defined in Generating RDF from Tabular Data on the Web.</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>Relates an Table group to annotated tables. (Note, this is different from csvw:resources, which relates metadata, rather than resulting annotated table descriptions.</t>
+  </si>
+  <si>
+    <t>table-direction</t>
+  </si>
+  <si>
+    <t>table direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of csvw:rtl csvw:ltr or csvw:default. Indicates whether the tables in the group should be displayed with the first column on the right, on the left, or based on the first character in the table that has a specific direction. </t>
+  </si>
+  <si>
+    <t>targetFormat</t>
+  </si>
+  <si>
+    <t>target format</t>
+  </si>
+  <si>
+    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>The exact length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>lineTerminator</t>
+  </si>
+  <si>
+    <t>line terminator</t>
+  </si>
+  <si>
+    <t>The character that is used at the end of a row. The default is CRLF.</t>
+  </si>
+  <si>
+    <t>maxExclusive</t>
+  </si>
+  <si>
+    <t>The maximum length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>minExclusive</t>
+  </si>
+  <si>
+    <t>min exclusive</t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t>minInclusive</t>
+  </si>
+  <si>
+    <t>min inclusive</t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (inclusive).</t>
+  </si>
+  <si>
+    <t>minLength</t>
+  </si>
+  <si>
+    <t>min length</t>
+  </si>
+  <si>
+    <t>The minimum length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
+  </si>
+  <si>
+    <t>predicateUrl</t>
+  </si>
+  <si>
+    <t>predicate URL</t>
+  </si>
+  <si>
+    <t>xsd:anyURI</t>
+  </si>
+  <si>
+    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
+  </si>
+  <si>
+    <t>primaryKey</t>
+  </si>
+  <si>
+    <t>primary key</t>
+  </si>
+  <si>
+    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
+  </si>
+  <si>
+    <t>quoteChar</t>
+  </si>
+  <si>
+    <t>quote char</t>
+  </si>
+  <si>
+    <t>The character that is used around escaped cells.</t>
+  </si>
+  <si>
+    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>TableGroup</t>
+  </si>
+  <si>
+    <t>An array of table descriptions for the tables in the group.</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>rdfs:member</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://www.w3.org/2001/XMLSchema#</t>
+    </r>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>An array of Column Descriptions.</t>
+  </si>
+  <si>
+    <t>commentPrefix</t>
+  </si>
+  <si>
+    <t>comment prefix</t>
+  </si>
+  <si>
+    <t>Dialect</t>
+  </si>
+  <si>
+    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>separator</t>
+  </si>
+  <si>
+    <t>The character used to separate items in the string value of the cell.</t>
+  </si>
+  <si>
+    <t>skipBlankRows</t>
+  </si>
+  <si>
+    <t>skip blank rows</t>
+  </si>
+  <si>
+    <t>TableGroup,Table,Schema,Column</t>
+  </si>
+  <si>
+    <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>An atomic property holding a single string that provides a default string value for the cell in cases where the original string value is a null value. This default value may be used when converting the table into other formats.</t>
+  </si>
+  <si>
+    <t>delimiter</t>
+  </si>
+  <si>
+    <t>The separator between cells. The default is ",".</t>
+  </si>
+  <si>
+    <t>dialect</t>
+  </si>
+  <si>
+    <t>TableGroup,Table</t>
+  </si>
+  <si>
+    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>doubleQuote</t>
+  </si>
+  <si>
+    <t>double quote</t>
+  </si>
+  <si>
+    <t>xsd:boolean</t>
+  </si>
+  <si>
+    <t>If true, sets the escape character flag to ". If false, to \\.</t>
+  </si>
+  <si>
+    <t>encoding</t>
+  </si>
+  <si>
+    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
+  </si>
+  <si>
+    <t>foreignKeys</t>
+  </si>
+  <si>
+    <t>foreign keys</t>
+  </si>
+  <si>
+    <t>An array of foreign key definitions that define how the values from specified columns within this table link to rows within this table or other tables.</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>A definition of the format of the cell, used when parsing the cell.</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>headerColumnCount</t>
+  </si>
+  <si>
+    <t>header column count</t>
+  </si>
+  <si>
+    <t>xsd:nonNegativeInteger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
+</t>
+  </si>
+  <si>
+    <t>headerRowCount</t>
+  </si>
+  <si>
+    <t>header row count</t>
+  </si>
+  <si>
+    <t>The number of header rows (following the skipped rows) in the file. The default is 1.</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>subClassOf</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>ltr</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>left to right</t>
+  </si>
+  <si>
+    <t>Indicates text should be processed left to right.</t>
+  </si>
+  <si>
+    <t>rtl</t>
+  </si>
+  <si>
+    <t>max exclusive</t>
+  </si>
+  <si>
+    <t>The maximum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t>maxInclusive</t>
+  </si>
+  <si>
+    <t>max inclusive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
+  </si>
+  <si>
+    <t>maxLength</t>
+  </si>
+  <si>
+    <t>max length</t>
+  </si>
+  <si>
     <t>right to left</t>
   </si>
   <si>
@@ -518,714 +1218,11 @@
   <si>
     <t>datatype</t>
   </si>
-  <si>
-    <t>TableGroup,Table,Schema,Column</t>
-  </si>
-  <si>
-    <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>An atomic property holding a single string that provides a default string value for the cell in cases where the original string value is a null value. This default value may be used when converting the table into other formats.</t>
-  </si>
-  <si>
-    <t>delimiter</t>
-  </si>
-  <si>
-    <t>The separator between cells. The default is ",".</t>
-  </si>
-  <si>
-    <t>dialect</t>
-  </si>
-  <si>
-    <t>TableGroup,Table</t>
-  </si>
-  <si>
-    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>doubleQuote</t>
-  </si>
-  <si>
-    <t>double quote</t>
-  </si>
-  <si>
-    <t>xsd:boolean</t>
-  </si>
-  <si>
-    <t>If true, sets the escape character flag to ". If false, to \\.</t>
-  </si>
-  <si>
-    <t>encoding</t>
-  </si>
-  <si>
-    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
-  </si>
-  <si>
-    <t>foreignKeys</t>
-  </si>
-  <si>
-    <t>foreign keys</t>
-  </si>
-  <si>
-    <t>An array of foreign key definitions that define how the values from specified columns within this table link to rows within this table or other tables.</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>A definition of the format of the cell, used when parsing the cell.</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>headerColumnCount</t>
-  </si>
-  <si>
-    <t>header column count</t>
-  </si>
-  <si>
-    <t>xsd:nonNegativeInteger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
-</t>
-  </si>
-  <si>
-    <t>headerRowCount</t>
-  </si>
-  <si>
-    <t>header row count</t>
-  </si>
-  <si>
-    <t>The number of header rows (following the skipped rows) in the file. The default is 1.</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>subClassOf</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>ltr</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>left to right</t>
-  </si>
-  <si>
-    <t>Indicates text should be processed left to right.</t>
-  </si>
-  <si>
-    <t>rtl</t>
-  </si>
-  <si>
-    <t>max exclusive</t>
-  </si>
-  <si>
-    <t>The maximum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t>maxInclusive</t>
-  </si>
-  <si>
-    <t>max inclusive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
-  </si>
-  <si>
-    <t>maxLength</t>
-  </si>
-  <si>
-    <t>max length</t>
-  </si>
-  <si>
-    <t>The maximum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>minExclusive</t>
-  </si>
-  <si>
-    <t>min exclusive</t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t>minInclusive</t>
-  </si>
-  <si>
-    <t>min inclusive</t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (inclusive).</t>
-  </si>
-  <si>
-    <t>minLength</t>
-  </si>
-  <si>
-    <t>min length</t>
-  </si>
-  <si>
-    <t>The minimum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
-  </si>
-  <si>
-    <t>predicateUrl</t>
-  </si>
-  <si>
-    <t>predicate URL</t>
-  </si>
-  <si>
-    <t>xsd:anyURI</t>
-  </si>
-  <si>
-    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
-  </si>
-  <si>
-    <t>primaryKey</t>
-  </si>
-  <si>
-    <t>primary key</t>
-  </si>
-  <si>
-    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
-  </si>
-  <si>
-    <t>quoteChar</t>
-  </si>
-  <si>
-    <t>quote char</t>
-  </si>
-  <si>
-    <t>The character that is used around escaped cells.</t>
-  </si>
-  <si>
-    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
-  </si>
-  <si>
-    <t>resources</t>
-  </si>
-  <si>
-    <t>TableGroup</t>
-  </si>
-  <si>
-    <t>An array of table descriptions for the tables in the group.</t>
-  </si>
-  <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>rdfs:member</t>
-  </si>
-  <si>
-    <t>xsd</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>http://www.w3.org/2001/XMLSchema#</t>
-    </r>
-  </si>
-  <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>rdf:Property</t>
-  </si>
-  <si>
-    <t>Schema</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>An array of Column Descriptions.</t>
-  </si>
-  <si>
-    <t>commentPrefix</t>
-  </si>
-  <si>
-    <t>comment prefix</t>
-  </si>
-  <si>
-    <t>Dialect</t>
-  </si>
-  <si>
-    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>separator</t>
-  </si>
-  <si>
-    <t>The character used to separate items in the string value of the cell.</t>
-  </si>
-  <si>
-    <t>skipBlankRows</t>
-  </si>
-  <si>
-    <t>skip blank rows</t>
-  </si>
-  <si>
-    <t>Indicates whether to ignore wholly empty rows (ie rows in which all the cells are empty). The default is false.</t>
-  </si>
-  <si>
-    <t>skipColumns</t>
-  </si>
-  <si>
-    <t>skip columns</t>
-  </si>
-  <si>
-    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
-  </si>
-  <si>
-    <t>skipInitialSpace</t>
-  </si>
-  <si>
-    <t>skip initial space</t>
-  </si>
-  <si>
-    <t>If true, sets the trim flag to "start". If false, to false.</t>
-  </si>
-  <si>
-    <t>skipRows</t>
-  </si>
-  <si>
-    <t>skip rows</t>
-  </si>
-  <si>
-    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>The format to which the tabular data should be transformed prior to the transformation using the template. If the value is "json", the tabular data should first be transformed first to JSON based on the simple mapping defined in Generating JSON from Tabular Data on the Web. If the value is "rdf", it should similarly first be transformed to XML based on the simple mapping defined in Generating RDF from Tabular Data on the Web.</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
-    <t>Relates an Table group to annotated tables. (Note, this is different from csvw:resources, which relates metadata, rather than resulting annotated table descriptions.</t>
-  </si>
-  <si>
-    <t>table-direction</t>
-  </si>
-  <si>
-    <t>table direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of csvw:rtl csvw:ltr or csvw:default. Indicates whether the tables in the group should be displayed with the first column on the right, on the left, or based on the first character in the table that has a specific direction. </t>
-  </si>
-  <si>
-    <t>targetFormat</t>
-  </si>
-  <si>
-    <t>target format</t>
-  </si>
-  <si>
-    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>The exact length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>lineTerminator</t>
-  </si>
-  <si>
-    <t>line terminator</t>
-  </si>
-  <si>
-    <t>The character that is used at the end of a row. The default is CRLF.</t>
-  </si>
-  <si>
-    <t>maxExclusive</t>
-  </si>
-  <si>
-    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
-  </si>
-  <si>
-    <t>templateFormat</t>
-  </si>
-  <si>
-    <t>template format</t>
-  </si>
-  <si>
-    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
-  </si>
-  <si>
-    <t>templates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
-  </si>
-  <si>
-    <t>text-direction</t>
-  </si>
-  <si>
-    <t>text direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of csvw:rtl or csvw:ltr. Indicates whether the text within cells should be displayed by default as left-to-right or right-to-left text. </t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Template,Column</t>
-  </si>
-  <si>
-    <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
-For a Column: A natural language property that provides possible alternative names for the column.</t>
-  </si>
-  <si>
-    <t>trim</t>
-  </si>
-  <si>
-    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
-  </si>
-  <si>
-    <t>uriTemplate</t>
-  </si>
-  <si>
-    <t>uri template</t>
-  </si>
-  <si>
-    <t>A URI template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
-  </si>
-  <si>
-    <t>rdfs:Class</t>
-  </si>
-  <si>
-    <t>Column Description</t>
-  </si>
-  <si>
-    <t>A Column Description describes a single column.</t>
-  </si>
-  <si>
-    <t>Dialect Description</t>
-  </si>
-  <si>
-    <t>A Dialect Description provides hints to parsers about how to parse a linked file.</t>
-  </si>
-  <si>
-    <t>The class of table/text directions.</t>
-  </si>
-  <si>
-    <t>Relates a Table to each Row output.</t>
-  </si>
-  <si>
-    <t>gYearMonth</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gYear</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gMonthDay</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gDay</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gMonth</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>hexBinary</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>base64Binary</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>anyURI</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>sch</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
-  </si>
-  <si>
-    <t>Table Description</t>
-  </si>
-  <si>
-    <t>A table description is a JSON object that describes a table within a CSV file.</t>
-  </si>
-  <si>
-    <t>Table Group Description</t>
-  </si>
-  <si>
-    <t>A Table Group Description describes a group of Tables.</t>
-  </si>
-  <si>
-    <t>Template Specification</t>
-  </si>
-  <si>
-    <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
-    <t>rdfs:Datatype</t>
-  </si>
-  <si>
-    <t>rdfs:Literal</t>
-  </si>
-  <si>
-    <t>A literal containing JSON.</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>xsd:anySimpleType</t>
-  </si>
-  <si>
-    <t>binary</t>
-  </si>
-  <si>
-    <t>xsd:base64Binary</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>xsd:dateTime</t>
-  </si>
-  <si>
-    <t>describedby</t>
-  </si>
-  <si>
-    <t>wrds:describedby</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>rdf:HTML</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
-    <t>xhv:license</t>
-  </si>
-  <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t>csvw:maxInclusive</t>
-  </si>
-  <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>csvw:minInclusive</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>xsd:double</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>xhv:role</t>
-  </si>
-  <si>
-    <t>rdf:XMLLiteral</t>
-  </si>
-  <si>
-    <t>anySimpleType</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>normalizedString</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>NCName</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>decimal</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>nonPositiveInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>negativeInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>long</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>short</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>byte</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>nonNegativeInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedLong</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedInt</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedShort</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedByte</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>positiveInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>double</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>duration</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>dateTime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>date</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -2633,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:IV140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1"/>
@@ -2649,22 +2646,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>105</v>
+        <v>198</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"@type"</f>
@@ -2675,21 +2672,21 @@
         <v>@container</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>111</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>112</v>
+        <v>205</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>114</v>
+        <v>207</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2698,18 +2695,18 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6" t="s">
-        <v>115</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>209</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2718,19 +2715,19 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6" t="s">
-        <v>1</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>219</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
-        <v>4</v>
+        <v>221</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2741,14 +2738,14 @@
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>222</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>223</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2759,14 +2756,14 @@
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>224</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>225</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2777,14 +2774,14 @@
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2795,14 +2792,14 @@
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>12</v>
+        <v>229</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2813,14 +2810,14 @@
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>230</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -2831,14 +2828,14 @@
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>232</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2849,14 +2846,14 @@
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>233</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>234</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2867,14 +2864,14 @@
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>235</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>236</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2885,14 +2882,14 @@
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>21</v>
+        <v>238</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2903,14 +2900,14 @@
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>239</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>240</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -2921,14 +2918,14 @@
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>241</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -2939,14 +2936,14 @@
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>244</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -2957,14 +2954,14 @@
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>245</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>29</v>
+        <v>246</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -2975,14 +2972,14 @@
     </row>
     <row r="18" spans="1:10" ht="19" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>30</v>
+        <v>247</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2993,14 +2990,14 @@
     </row>
     <row r="19" spans="1:10" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>249</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4" t="s">
-        <v>33</v>
+        <v>250</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -3011,14 +3008,14 @@
     </row>
     <row r="20" spans="1:10" ht="19" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>251</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
-        <v>35</v>
+        <v>252</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3029,14 +3026,14 @@
     </row>
     <row r="21" spans="1:10" ht="19" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -3047,14 +3044,14 @@
     </row>
     <row r="22" spans="1:10" ht="19" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>255</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
-        <v>39</v>
+        <v>256</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3065,14 +3062,14 @@
     </row>
     <row r="23" spans="1:10" ht="19" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>257</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>41</v>
+        <v>258</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3083,14 +3080,14 @@
     </row>
     <row r="24" spans="1:10" ht="19" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>42</v>
+        <v>259</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
-        <v>43</v>
+        <v>260</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -3101,14 +3098,14 @@
     </row>
     <row r="25" spans="1:10" ht="19" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>261</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
-        <v>45</v>
+        <v>262</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -3119,14 +3116,14 @@
     </row>
     <row r="26" spans="1:10" ht="19" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>263</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3137,14 +3134,14 @@
     </row>
     <row r="27" spans="1:10" ht="19" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>231</v>
+        <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4" t="s">
-        <v>49</v>
+        <v>266</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -3155,14 +3152,14 @@
     </row>
     <row r="28" spans="1:10" ht="19" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>50</v>
+        <v>267</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
-        <v>51</v>
+        <v>268</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -3173,14 +3170,14 @@
     </row>
     <row r="29" spans="1:10" ht="19" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>52</v>
+        <v>269</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
-        <v>53</v>
+        <v>270</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -3191,14 +3188,14 @@
     </row>
     <row r="30" spans="1:10" ht="19" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>54</v>
+        <v>271</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>55</v>
+        <v>272</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3209,14 +3206,14 @@
     </row>
     <row r="31" spans="1:10" ht="19" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>56</v>
+        <v>273</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
-        <v>57</v>
+        <v>274</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -3227,14 +3224,14 @@
     </row>
     <row r="32" spans="1:10" ht="19" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>58</v>
+        <v>275</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
-        <v>59</v>
+        <v>276</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -3245,14 +3242,14 @@
     </row>
     <row r="33" spans="1:10" ht="19" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>60</v>
+        <v>277</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
-        <v>61</v>
+        <v>278</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -3263,14 +3260,14 @@
     </row>
     <row r="34" spans="1:10" ht="19" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>62</v>
+        <v>279</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4" t="s">
-        <v>63</v>
+        <v>280</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3281,14 +3278,14 @@
     </row>
     <row r="35" spans="1:10" ht="19" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>64</v>
+        <v>281</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
-        <v>65</v>
+        <v>282</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -3299,14 +3296,14 @@
     </row>
     <row r="36" spans="1:10" ht="19" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>66</v>
+        <v>283</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
-        <v>67</v>
+        <v>284</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3317,14 +3314,14 @@
     </row>
     <row r="37" spans="1:10" ht="19" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>68</v>
+        <v>285</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
-        <v>69</v>
+        <v>286</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -3335,14 +3332,14 @@
     </row>
     <row r="38" spans="1:10" ht="19" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>70</v>
+        <v>287</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>71</v>
+        <v>288</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3353,14 +3350,14 @@
     </row>
     <row r="39" spans="1:10" ht="19" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -3371,20 +3368,20 @@
     </row>
     <row r="40" spans="1:10" ht="19" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="4" t="str">
@@ -3393,227 +3390,227 @@
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="60" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="6" t="s">
-        <v>73</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="60" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="6" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>77</v>
+        <v>170</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>77</v>
+        <v>170</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="6" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="19" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>72</v>
+        <v>289</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>79</v>
+        <v>172</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="6" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="6" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="45" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>90</v>
+        <v>183</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="6" t="s">
-        <v>94</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="19" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -3622,269 +3619,269 @@
     </row>
     <row r="51" spans="1:10" ht="45" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="6" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>101</v>
+        <v>194</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="6" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="6" t="s">
-        <v>192</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="19" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>193</v>
+        <v>114</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>193</v>
+        <v>114</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="6" t="s">
-        <v>194</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>196</v>
+        <v>117</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="6" t="s">
-        <v>197</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="19" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>117</v>
+        <v>210</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="4" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="19" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>120</v>
+        <v>213</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="4" t="s">
-        <v>121</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="19" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>122</v>
+        <v>215</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>123</v>
+        <v>216</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="19" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="19" customHeight="1">
       <c r="A60" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="19" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="75" customHeight="1">
       <c r="A62" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -3893,161 +3890,161 @@
         <v>1</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="30" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="45" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="45" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="19" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="30" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G69" s="5"/>
       <c r="H69" s="4" t="str">
@@ -4058,24 +4055,24 @@
         <v>1</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="19" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4085,191 +4082,191 @@
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="6" t="s">
-        <v>222</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="45" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>48</v>
+        <v>265</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>48</v>
+        <v>265</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="4" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="30" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="45" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6" t="s">
-        <v>172</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6" t="s">
-        <v>175</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="19" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>177</v>
+        <v>98</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6" t="s">
-        <v>178</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="30" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>179</v>
+        <v>100</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>180</v>
+        <v>101</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="135" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>183</v>
+        <v>104</v>
       </c>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6" t="s">
-        <v>184</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="60" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>185</v>
+        <v>106</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>185</v>
+        <v>106</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="4" t="str">
@@ -4278,25 +4275,25 @@
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="6" t="s">
-        <v>186</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="75" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>188</v>
+        <v>109</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="G79" s="4" t="str">
         <f>"@vocab"</f>
@@ -4305,93 +4302,93 @@
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6" t="s">
-        <v>189</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="120" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>190</v>
+        <v>111</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>191</v>
+        <v>112</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>183</v>
+        <v>104</v>
       </c>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="120" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>201</v>
+        <v>74</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>183</v>
+        <v>104</v>
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="6" t="s">
-        <v>202</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="45" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>183</v>
+        <v>104</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6" t="s">
-        <v>204</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="45" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>205</v>
+        <v>78</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="G83" s="4" t="str">
         <f>"@vocab"</f>
@@ -4400,22 +4397,22 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6" t="s">
-        <v>207</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="135" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>208</v>
+        <v>81</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>208</v>
+        <v>81</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>209</v>
+        <v>82</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -4425,64 +4422,64 @@
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="6" t="s">
-        <v>210</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>211</v>
+        <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>211</v>
+        <v>84</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="6" t="s">
-        <v>212</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="45" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>213</v>
+        <v>70</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>214</v>
+        <v>71</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6" t="s">
-        <v>215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="19" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>217</v>
+        <v>87</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -4491,18 +4488,18 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="6" t="s">
-        <v>218</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="30" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>219</v>
+        <v>89</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -4511,18 +4508,18 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="6" t="s">
-        <v>220</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="19" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -4531,18 +4528,18 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="30" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -4551,18 +4548,18 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6" t="s">
-        <v>232</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="30" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>233</v>
+        <v>11</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -4571,18 +4568,18 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6" t="s">
-        <v>234</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="30" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>235</v>
+        <v>13</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -4591,18 +4588,18 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6" t="s">
-        <v>236</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="45" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>183</v>
+        <v>104</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>237</v>
+        <v>15</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -4611,21 +4608,21 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6" t="s">
-        <v>238</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="19" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>239</v>
+        <v>17</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>240</v>
+        <v>18</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>239</v>
+        <v>17</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>241</v>
+        <v>19</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -4633,19 +4630,19 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6" t="s">
-        <v>242</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="19" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>243</v>
+        <v>21</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="4" t="s">
-        <v>245</v>
+        <v>23</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
@@ -4656,14 +4653,14 @@
     </row>
     <row r="96" spans="1:10" ht="19" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>246</v>
+        <v>24</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="4" t="s">
-        <v>247</v>
+        <v>25</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -4674,14 +4671,14 @@
     </row>
     <row r="97" spans="1:10" ht="19" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>248</v>
+        <v>26</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="4" t="s">
-        <v>249</v>
+        <v>27</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -4692,14 +4689,14 @@
     </row>
     <row r="98" spans="1:10" ht="19" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>250</v>
+        <v>28</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="4" t="s">
-        <v>251</v>
+        <v>29</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -4710,14 +4707,14 @@
     </row>
     <row r="99" spans="1:10" ht="19" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>252</v>
+        <v>30</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="4" t="s">
-        <v>253</v>
+        <v>31</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -4728,14 +4725,14 @@
     </row>
     <row r="100" spans="1:10" ht="19" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>254</v>
+        <v>32</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="4" t="s">
-        <v>255</v>
+        <v>33</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -4746,14 +4743,14 @@
     </row>
     <row r="101" spans="1:10" ht="19" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="4" t="s">
-        <v>257</v>
+        <v>35</v>
       </c>
       <c r="E101" s="9"/>
       <c r="F101" s="5"/>
@@ -4764,14 +4761,14 @@
     </row>
     <row r="102" spans="1:10" ht="19" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>258</v>
+        <v>36</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="4" t="s">
-        <v>259</v>
+        <v>37</v>
       </c>
       <c r="E102" s="9"/>
       <c r="F102" s="5"/>
@@ -4782,14 +4779,14 @@
     </row>
     <row r="103" spans="1:10" ht="19" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>260</v>
+        <v>38</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
-        <v>261</v>
+        <v>39</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -4800,14 +4797,14 @@
     </row>
     <row r="104" spans="1:10" ht="19" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>262</v>
+        <v>40</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="4" t="s">
-        <v>263</v>
+        <v>41</v>
       </c>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
@@ -4818,14 +4815,14 @@
     </row>
     <row r="105" spans="1:10" ht="19" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>70</v>
+        <v>287</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="4" t="s">
-        <v>264</v>
+        <v>42</v>
       </c>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
@@ -4836,10 +4833,10 @@
     </row>
     <row r="106" spans="1:10" ht="15" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>265</v>
+        <v>43</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C106" s="4"/>
       <c r="D106" s="4" t="str">
@@ -4855,10 +4852,10 @@
     </row>
     <row r="107" spans="1:10" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>266</v>
+        <v>44</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="4" t="str">
@@ -4874,10 +4871,10 @@
     </row>
     <row r="108" spans="1:10" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4" t="str">
@@ -4893,10 +4890,10 @@
     </row>
     <row r="109" spans="1:10" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>268</v>
+        <v>46</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4" t="str">
@@ -4912,10 +4909,10 @@
     </row>
     <row r="110" spans="1:10" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>269</v>
+        <v>47</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="str">
@@ -4931,10 +4928,10 @@
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>270</v>
+        <v>48</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="str">
@@ -4950,10 +4947,10 @@
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>271</v>
+        <v>49</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="str">
@@ -4969,10 +4966,10 @@
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>272</v>
+        <v>50</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="str">
@@ -4988,10 +4985,10 @@
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>273</v>
+        <v>51</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="str">
@@ -5007,10 +5004,10 @@
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>274</v>
+        <v>52</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="str">
@@ -5026,10 +5023,10 @@
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>275</v>
+        <v>53</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="str">
@@ -5045,10 +5042,10 @@
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>276</v>
+        <v>54</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="str">
@@ -5064,10 +5061,10 @@
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="str">
@@ -5083,10 +5080,10 @@
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>278</v>
+        <v>56</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="str">
@@ -5102,10 +5099,10 @@
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>279</v>
+        <v>57</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="str">
@@ -5121,10 +5118,10 @@
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>280</v>
+        <v>58</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="str">
@@ -5140,10 +5137,10 @@
     </row>
     <row r="122" spans="1:10" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>281</v>
+        <v>59</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="str">
@@ -5159,10 +5156,10 @@
     </row>
     <row r="123" spans="1:10" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>282</v>
+        <v>60</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="str">
@@ -5178,10 +5175,10 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>283</v>
+        <v>61</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="str">
@@ -5197,10 +5194,10 @@
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>284</v>
+        <v>62</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="str">
@@ -5216,10 +5213,10 @@
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>285</v>
+        <v>63</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="str">
@@ -5235,10 +5232,10 @@
     </row>
     <row r="127" spans="1:10" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>286</v>
+        <v>64</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="str">
@@ -5254,10 +5251,10 @@
     </row>
     <row r="128" spans="1:10" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>287</v>
+        <v>65</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="str">
@@ -5273,10 +5270,10 @@
     </row>
     <row r="129" spans="1:10" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>288</v>
+        <v>66</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4" t="str">
@@ -5292,10 +5289,10 @@
     </row>
     <row r="130" spans="1:10" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>289</v>
+        <v>67</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="4" t="str">
@@ -5311,10 +5308,10 @@
     </row>
     <row r="131" spans="1:10" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>290</v>
+        <v>68</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4" t="str">
@@ -5330,10 +5327,10 @@
     </row>
     <row r="132" spans="1:10" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>291</v>
+        <v>69</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="4" t="str">
@@ -5349,10 +5346,10 @@
     </row>
     <row r="133" spans="1:10" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>223</v>
+        <v>1</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C133" s="4"/>
       <c r="D133" s="4" t="str">
@@ -5368,10 +5365,10 @@
     </row>
     <row r="134" spans="1:10" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>224</v>
+        <v>2</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4" t="str">
@@ -5387,10 +5384,10 @@
     </row>
     <row r="135" spans="1:10" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>225</v>
+        <v>3</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4" t="str">
@@ -5406,10 +5403,10 @@
     </row>
     <row r="136" spans="1:10" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>226</v>
+        <v>4</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C136" s="4"/>
       <c r="D136" s="4" t="str">
@@ -5425,10 +5422,10 @@
     </row>
     <row r="137" spans="1:10" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>227</v>
+        <v>5</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="str">
@@ -5444,10 +5441,10 @@
     </row>
     <row r="138" spans="1:10" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>228</v>
+        <v>6</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="str">
@@ -5463,10 +5460,10 @@
     </row>
     <row r="139" spans="1:10" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>229</v>
+        <v>7</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C139" s="4"/>
       <c r="D139" s="4" t="str">
@@ -5482,10 +5479,10 @@
     </row>
     <row r="140" spans="1:10" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>230</v>
+        <v>8</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="C140" s="4"/>
       <c r="D140" s="4" t="str">
@@ -5500,7 +5497,6 @@
       <c r="J140" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>

</xml_diff>

<commit_message>
Update namespace/context to indicate that string values or xsd:string, and have `@language: null`.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="-80" windowWidth="23600" windowHeight="26560"/>
+    <workbookView xWindow="5060" yWindow="-320" windowWidth="23600" windowHeight="26560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="300">
+  <si>
+    <t>xsd:anyURI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>csvw:uriTemplate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>A URL template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -276,6 +284,18 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>uriTemplate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>uri template</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
   </si>
   <si>
@@ -347,15 +367,6 @@
   </si>
   <si>
     <t>skip columns</t>
-  </si>
-  <si>
-    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
-  </si>
-  <si>
-    <t>skipInitialSpace</t>
-  </si>
-  <si>
-    <t>skip initial space</t>
   </si>
   <si>
     <t>If true, sets the trim flag to "start". If false, to false.</t>
@@ -582,6 +593,15 @@
     <t>default</t>
   </si>
   <si>
+    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
+  </si>
+  <si>
+    <t>skipInitialSpace</t>
+  </si>
+  <si>
+    <t>skip initial space</t>
+  </si>
+  <si>
     <t>An atomic property holding a single string that provides a default string value for the cell in cases where the original string value is a null value. This default value may be used when converting the table into other formats.</t>
   </si>
   <si>
@@ -1218,11 +1238,29 @@
   <si>
     <t>datatype</t>
   </si>
+  <si>
+    <t>xsd:string</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>xsd:integer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>xsd:anyURI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -2628,10 +2666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:IV140"/>
+  <dimension ref="A1:IV141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1"/>
@@ -2646,22 +2684,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"@type"</f>
@@ -2672,21 +2710,21 @@
         <v>@container</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2695,18 +2733,18 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2715,19 +2753,19 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2738,14 +2776,14 @@
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2756,14 +2794,14 @@
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2774,14 +2812,14 @@
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2792,14 +2830,14 @@
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2810,14 +2848,14 @@
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -2828,14 +2866,14 @@
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2846,14 +2884,14 @@
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2864,14 +2902,14 @@
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2882,14 +2920,14 @@
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2900,14 +2938,14 @@
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -2918,14 +2956,14 @@
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -2936,14 +2974,14 @@
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -2954,14 +2992,14 @@
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -2972,14 +3010,14 @@
     </row>
     <row r="18" spans="1:10" ht="19" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2990,14 +3028,14 @@
     </row>
     <row r="19" spans="1:10" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -3008,14 +3046,14 @@
     </row>
     <row r="20" spans="1:10" ht="19" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3026,14 +3064,14 @@
     </row>
     <row r="21" spans="1:10" ht="19" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -3044,14 +3082,14 @@
     </row>
     <row r="22" spans="1:10" ht="19" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3062,14 +3100,14 @@
     </row>
     <row r="23" spans="1:10" ht="19" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3080,14 +3118,14 @@
     </row>
     <row r="24" spans="1:10" ht="19" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -3098,14 +3136,14 @@
     </row>
     <row r="25" spans="1:10" ht="19" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -3116,14 +3154,14 @@
     </row>
     <row r="26" spans="1:10" ht="19" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3134,14 +3172,14 @@
     </row>
     <row r="27" spans="1:10" ht="19" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -3152,14 +3190,14 @@
     </row>
     <row r="28" spans="1:10" ht="19" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -3170,14 +3208,14 @@
     </row>
     <row r="29" spans="1:10" ht="19" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -3188,14 +3226,14 @@
     </row>
     <row r="30" spans="1:10" ht="19" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3206,14 +3244,14 @@
     </row>
     <row r="31" spans="1:10" ht="19" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -3224,14 +3262,14 @@
     </row>
     <row r="32" spans="1:10" ht="19" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -3242,14 +3280,14 @@
     </row>
     <row r="33" spans="1:10" ht="19" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -3260,14 +3298,14 @@
     </row>
     <row r="34" spans="1:10" ht="19" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3278,14 +3316,14 @@
     </row>
     <row r="35" spans="1:10" ht="19" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -3296,14 +3334,14 @@
     </row>
     <row r="36" spans="1:10" ht="19" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3314,14 +3352,14 @@
     </row>
     <row r="37" spans="1:10" ht="19" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -3332,14 +3370,14 @@
     </row>
     <row r="38" spans="1:10" ht="19" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3350,14 +3388,14 @@
     </row>
     <row r="39" spans="1:10" ht="19" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -3368,20 +3406,20 @@
     </row>
     <row r="40" spans="1:10" ht="19" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="4" t="str">
@@ -3390,227 +3428,241 @@
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="60" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="6" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="60" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="6" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="19" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="6" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="6" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="45" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>159</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="6" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="19" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -3619,432 +3671,452 @@
     </row>
     <row r="51" spans="1:10" ht="45" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="6" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="6" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="19" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="19" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>298</v>
+      </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="19" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>298</v>
+      </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="4" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="19" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="19" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>298</v>
+      </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="19" customHeight="1">
       <c r="A60" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>298</v>
+      </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="19" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="75" customHeight="1">
       <c r="A62" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>160</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5" t="b">
         <v>1</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="30" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="45" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="45" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>159</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="19" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="30" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G69" s="5"/>
       <c r="H69" s="4" t="str">
@@ -4055,24 +4127,24 @@
         <v>1</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="19" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4082,191 +4154,195 @@
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="45" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="30" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F72" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="45" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="19" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="30" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="135" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="60" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="4" t="str">
@@ -4275,25 +4351,25 @@
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="75" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G79" s="4" t="str">
         <f>"@vocab"</f>
@@ -4302,93 +4378,97 @@
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="120" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F80" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>299</v>
+      </c>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="120" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F81" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>299</v>
+      </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="45" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="45" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G83" s="4" t="str">
         <f>"@vocab"</f>
@@ -4397,22 +4477,22 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="135" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -4422,64 +4502,66 @@
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="45" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F86" s="5"/>
+        <v>159</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="19" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -4488,18 +4570,18 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="30" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -4508,18 +4590,18 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="19" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -4528,18 +4610,18 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="30" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -4548,18 +4630,18 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="30" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -4568,18 +4650,18 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="30" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -4588,18 +4670,18 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="45" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -4608,21 +4690,21 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="19" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -4630,33 +4712,35 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="19" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="D95" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
-      <c r="J95" s="7"/>
+      <c r="J95" s="6"/>
     </row>
     <row r="96" spans="1:10" ht="19" customHeight="1">
       <c r="A96" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="4" t="s">
@@ -4674,7 +4758,7 @@
         <v>26</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="4" t="s">
@@ -4692,7 +4776,7 @@
         <v>28</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="4" t="s">
@@ -4710,7 +4794,7 @@
         <v>30</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="4" t="s">
@@ -4728,7 +4812,7 @@
         <v>32</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="4" t="s">
@@ -4746,13 +4830,13 @@
         <v>34</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E101" s="9"/>
+      <c r="E101" s="5"/>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
@@ -4764,7 +4848,7 @@
         <v>36</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="4" t="s">
@@ -4782,13 +4866,13 @@
         <v>38</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E103" s="5"/>
+      <c r="E103" s="9"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
@@ -4800,7 +4884,7 @@
         <v>40</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="4" t="s">
@@ -4815,14 +4899,14 @@
     </row>
     <row r="105" spans="1:10" ht="19" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>287</v>
+        <v>42</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
@@ -4831,17 +4915,16 @@
       <c r="I105" s="5"/>
       <c r="J105" s="7"/>
     </row>
-    <row r="106" spans="1:10" ht="15" customHeight="1">
+    <row r="106" spans="1:10" ht="19" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>43</v>
+        <v>292</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4" t="str">
-        <f>CONCATENATE("xsd:",A106)</f>
-        <v>xsd:anySimpleType</v>
+        <v>24</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
@@ -4852,15 +4935,15 @@
     </row>
     <row r="107" spans="1:10" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="4" t="str">
-        <f t="shared" ref="D107:D140" si="0">CONCATENATE("xsd:",A107)</f>
-        <v>xsd:string</v>
+        <f>CONCATENATE("xsd:",A107)</f>
+        <v>xsd:anySimpleType</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
@@ -4871,15 +4954,15 @@
     </row>
     <row r="108" spans="1:10" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:normalizedString</v>
+        <f t="shared" ref="D108:D141" si="0">CONCATENATE("xsd:",A108)</f>
+        <v>xsd:string</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
@@ -4890,15 +4973,15 @@
     </row>
     <row r="109" spans="1:10" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:token</v>
+        <v>xsd:normalizedString</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
@@ -4909,15 +4992,15 @@
     </row>
     <row r="110" spans="1:10" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:Name</v>
+        <v>xsd:token</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
@@ -4928,15 +5011,15 @@
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:NCName</v>
+        <v>xsd:Name</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
@@ -4947,15 +5030,15 @@
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:boolean</v>
+        <v>xsd:NCName</v>
       </c>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
@@ -4966,15 +5049,15 @@
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:decimal</v>
+        <v>xsd:boolean</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
@@ -4985,15 +5068,15 @@
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:integer</v>
+        <v>xsd:decimal</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
@@ -5004,15 +5087,15 @@
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonPositiveInteger</v>
+        <v>xsd:integer</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
@@ -5023,15 +5106,15 @@
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:negativeInteger</v>
+        <v>xsd:nonPositiveInteger</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
@@ -5042,15 +5125,15 @@
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:long</v>
+        <v>xsd:negativeInteger</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
@@ -5061,15 +5144,15 @@
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:int</v>
+        <v>xsd:long</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
@@ -5080,15 +5163,15 @@
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:short</v>
+        <v>xsd:int</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
@@ -5099,15 +5182,15 @@
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:byte</v>
+        <v>xsd:short</v>
       </c>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
@@ -5118,15 +5201,15 @@
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonNegativeInteger</v>
+        <v>xsd:byte</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
@@ -5137,15 +5220,15 @@
     </row>
     <row r="122" spans="1:10" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedLong</v>
+        <v>xsd:nonNegativeInteger</v>
       </c>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -5156,15 +5239,15 @@
     </row>
     <row r="123" spans="1:10" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedInt</v>
+        <v>xsd:unsignedLong</v>
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -5175,15 +5258,15 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedShort</v>
+        <v>xsd:unsignedInt</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
@@ -5194,15 +5277,15 @@
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedByte</v>
+        <v>xsd:unsignedShort</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
@@ -5213,15 +5296,15 @@
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:positiveInteger</v>
+        <v>xsd:unsignedByte</v>
       </c>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
@@ -5232,15 +5315,15 @@
     </row>
     <row r="127" spans="1:10" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:float</v>
+        <v>xsd:positiveInteger</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
@@ -5251,15 +5334,15 @@
     </row>
     <row r="128" spans="1:10" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:double</v>
+        <v>xsd:float</v>
       </c>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
@@ -5270,15 +5353,15 @@
     </row>
     <row r="129" spans="1:10" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:duration</v>
+        <v>xsd:double</v>
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
@@ -5289,15 +5372,15 @@
     </row>
     <row r="130" spans="1:10" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:dateTime</v>
+        <v>xsd:duration</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
@@ -5308,15 +5391,15 @@
     </row>
     <row r="131" spans="1:10" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:time</v>
+        <v>xsd:dateTime</v>
       </c>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
@@ -5327,15 +5410,15 @@
     </row>
     <row r="132" spans="1:10" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:date</v>
+        <v>xsd:time</v>
       </c>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
@@ -5346,15 +5429,15 @@
     </row>
     <row r="133" spans="1:10" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C133" s="4"/>
       <c r="D133" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYearMonth</v>
+        <v>xsd:date</v>
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
@@ -5365,15 +5448,15 @@
     </row>
     <row r="134" spans="1:10" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYear</v>
+        <v>xsd:gYearMonth</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
@@ -5384,15 +5467,15 @@
     </row>
     <row r="135" spans="1:10" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonthDay</v>
+        <v>xsd:gYear</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
@@ -5403,15 +5486,15 @@
     </row>
     <row r="136" spans="1:10" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C136" s="4"/>
       <c r="D136" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gDay</v>
+        <v>xsd:gMonthDay</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
@@ -5422,15 +5505,15 @@
     </row>
     <row r="137" spans="1:10" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonth</v>
+        <v>xsd:gDay</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
@@ -5441,15 +5524,15 @@
     </row>
     <row r="138" spans="1:10" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:hexBinary</v>
+        <v>xsd:gMonth</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
@@ -5460,15 +5543,15 @@
     </row>
     <row r="139" spans="1:10" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C139" s="4"/>
       <c r="D139" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:base64Binary</v>
+        <v>xsd:hexBinary</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
@@ -5479,15 +5562,15 @@
     </row>
     <row r="140" spans="1:10" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C140" s="4"/>
       <c r="D140" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:anyURI</v>
+        <v>xsd:base64Binary</v>
       </c>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
@@ -5495,6 +5578,25 @@
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
       <c r="J140" s="7"/>
+    </row>
+    <row r="141" spans="1:10" ht="15" customHeight="1">
+      <c r="A141" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:anyURI</v>
+      </c>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="5"/>
+      <c r="J141" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -5537,6 +5639,7 @@
     <hyperlink ref="D39" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Pervasively update `language` to `lang` (other than `@context` usage) and `schema` to `tableSchema` as resolved in issues #86 and #128. Also change `sch:` prefix back to `schema:`.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -19,7 +19,801 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="305">
+  <si>
+    <t>xsd:language</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tableSchema</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>table schema</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>csvw:uriTemplate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A URL template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gYearMonth</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gYear</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gMonthDay</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gDay</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gMonth</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>hexBinary</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>base64Binary</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>anyURI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
+  </si>
+  <si>
+    <t>Table Description</t>
+  </si>
+  <si>
+    <t>A table description is a JSON object that describes a table within a CSV file.</t>
+  </si>
+  <si>
+    <t>Table Group Description</t>
+  </si>
+  <si>
+    <t>A Table Group Description describes a group of Tables.</t>
+  </si>
+  <si>
+    <t>Template Specification</t>
+  </si>
+  <si>
+    <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+  </si>
+  <si>
+    <t>rdfs:Literal</t>
+  </si>
+  <si>
+    <t>A literal containing JSON.</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>xsd:anySimpleType</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>xsd:base64Binary</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>xsd:dateTime</t>
+  </si>
+  <si>
+    <t>describedby</t>
+  </si>
+  <si>
+    <t>wrds:describedby</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>rdf:HTML</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>xhv:license</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>csvw:maxInclusive</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>csvw:minInclusive</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>xsd:double</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>xhv:role</t>
+  </si>
+  <si>
+    <t>rdf:XMLLiteral</t>
+  </si>
+  <si>
+    <t>anySimpleType</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>normalizedString</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCName</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>decimal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonPositiveInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>negativeInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>long</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>short</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonNegativeInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedLong</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedInt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedShort</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsignedByte</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>positiveInteger</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateTime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>urlTemplate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL template</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>uriTemplate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>lang</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>term</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
+  </si>
+  <si>
+    <t>templateFormat</t>
+  </si>
+  <si>
+    <t>template format</t>
+  </si>
+  <si>
+    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
+  </si>
+  <si>
+    <t>templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
+  </si>
+  <si>
+    <t>text-direction</t>
+  </si>
+  <si>
+    <t>text direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of csvw:rtl or csvw:ltr. Indicates whether the text within cells should be displayed by default as left-to-right or right-to-left text. </t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Template,Column</t>
+  </si>
+  <si>
+    <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
+For a Column: A natural language property that provides possible alternative names for the column.</t>
+  </si>
+  <si>
+    <t>trim</t>
+  </si>
+  <si>
+    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
+  </si>
+  <si>
+    <t>rdfs:Class</t>
+  </si>
+  <si>
+    <t>Column Description</t>
+  </si>
+  <si>
+    <t>A Column Description describes a single column.</t>
+  </si>
+  <si>
+    <t>Dialect Description</t>
+  </si>
+  <si>
+    <t>A Dialect Description provides hints to parsers about how to parse a linked file.</t>
+  </si>
+  <si>
+    <t>The class of table/text directions.</t>
+  </si>
+  <si>
+    <t>Relates a Table to each Row output.</t>
+  </si>
+  <si>
+    <t>Indicates whether to ignore wholly empty rows (ie rows in which all the cells are empty). The default is false.</t>
+  </si>
+  <si>
+    <t>skipColumns</t>
+  </si>
+  <si>
+    <t>xsd:anyURI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>skip columns</t>
+  </si>
+  <si>
+    <t>If true, sets the trim flag to "start". If false, to false.</t>
+  </si>
+  <si>
+    <t>skipRows</t>
+  </si>
+  <si>
+    <t>skip rows</t>
+  </si>
+  <si>
+    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>The format to which the tabular data should be transformed prior to the transformation using the template. If the value is "json", the tabular data should first be transformed first to JSON based on the simple mapping defined in Generating JSON from Tabular Data on the Web. If the value is "rdf", it should similarly first be transformed to XML based on the simple mapping defined in Generating RDF from Tabular Data on the Web.</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>Relates an Table group to annotated tables. (Note, this is different from csvw:resources, which relates metadata, rather than resulting annotated table descriptions.</t>
+  </si>
+  <si>
+    <t>table-direction</t>
+  </si>
+  <si>
+    <t>table direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of csvw:rtl csvw:ltr or csvw:default. Indicates whether the tables in the group should be displayed with the first column on the right, on the left, or based on the first character in the table that has a specific direction. </t>
+  </si>
+  <si>
+    <t>targetFormat</t>
+  </si>
+  <si>
+    <t>target format</t>
+  </si>
+  <si>
+    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>The exact length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>lineTerminator</t>
+  </si>
+  <si>
+    <t>line terminator</t>
+  </si>
+  <si>
+    <t>The character that is used at the end of a row. The default is CRLF.</t>
+  </si>
+  <si>
+    <t>maxExclusive</t>
+  </si>
+  <si>
+    <t>The maximum length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>minExclusive</t>
+  </si>
+  <si>
+    <t>min exclusive</t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t>minInclusive</t>
+  </si>
+  <si>
+    <t>min inclusive</t>
+  </si>
+  <si>
+    <t>The minimum value for the cell (inclusive).</t>
+  </si>
+  <si>
+    <t>minLength</t>
+  </si>
+  <si>
+    <t>min length</t>
+  </si>
+  <si>
+    <t>The minimum length of the value of the cell.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>uri template</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
+  </si>
+  <si>
+    <t>predicateUrl</t>
+  </si>
+  <si>
+    <t>predicate URL</t>
+  </si>
+  <si>
+    <t>xsd:anyURI</t>
+  </si>
+  <si>
+    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
+  </si>
+  <si>
+    <t>primaryKey</t>
+  </si>
+  <si>
+    <t>primary key</t>
+  </si>
+  <si>
+    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
+  </si>
+  <si>
+    <t>quoteChar</t>
+  </si>
+  <si>
+    <t>quote char</t>
+  </si>
+  <si>
+    <t>The character that is used around escaped cells.</t>
+  </si>
+  <si>
+    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>TableGroup</t>
+  </si>
+  <si>
+    <t>An array of table descriptions for the tables in the group.</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>rdfs:member</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://www.w3.org/2001/XMLSchema#</t>
+    </r>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>An array of Column Descriptions.</t>
+  </si>
+  <si>
+    <t>commentPrefix</t>
+  </si>
+  <si>
+    <t>comment prefix</t>
+  </si>
+  <si>
+    <t>Dialect</t>
+  </si>
+  <si>
+    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>separator</t>
+  </si>
+  <si>
+    <t>The character used to separate items in the string value of the cell.</t>
+  </si>
+  <si>
+    <t>skipBlankRows</t>
+  </si>
+  <si>
+    <t>skip blank rows</t>
+  </si>
+  <si>
+    <t>TableGroup,Table,Schema,Column</t>
+  </si>
+  <si>
+    <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
+  </si>
+  <si>
+    <t>skipInitialSpace</t>
+  </si>
+  <si>
+    <t>skip initial space</t>
+  </si>
+  <si>
+    <t>An atomic property holding a single string that provides a default string value for the cell in cases where the original string value is a null value. This default value may be used when converting the table into other formats.</t>
+  </si>
+  <si>
+    <t>delimiter</t>
+  </si>
+  <si>
+    <t>The separator between cells. The default is ",".</t>
+  </si>
+  <si>
+    <t>dialect</t>
+  </si>
+  <si>
+    <t>TableGroup,Table</t>
+  </si>
+  <si>
+    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
+  </si>
+  <si>
+    <t>doubleQuote</t>
+  </si>
+  <si>
+    <t>double quote</t>
+  </si>
+  <si>
+    <t>xsd:boolean</t>
+  </si>
+  <si>
+    <t>If true, sets the escape character flag to ". If false, to \\.</t>
+  </si>
+  <si>
+    <t>encoding</t>
+  </si>
+  <si>
+    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
+  </si>
+  <si>
+    <t>foreignKeys</t>
+  </si>
+  <si>
+    <t>foreign keys</t>
+  </si>
+  <si>
+    <t>An array of foreign key definitions that define how the values from specified columns within this table link to rows within this table or other tables.</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>A definition of the format of the cell, used when parsing the cell.</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>headerColumnCount</t>
+  </si>
+  <si>
+    <t>header column count</t>
+  </si>
+  <si>
+    <t>xsd:nonNegativeInteger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
+</t>
+  </si>
+  <si>
+    <t>headerRowCount</t>
+  </si>
+  <si>
+    <t>header row count</t>
+  </si>
+  <si>
+    <t>The number of header rows (following the skipped rows) in the file. The default is 1.</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>subClassOf</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>ltr</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>left to right</t>
+  </si>
+  <si>
+    <t>Indicates text should be processed left to right.</t>
+  </si>
+  <si>
+    <t>rtl</t>
+  </si>
+  <si>
+    <t>max exclusive</t>
+  </si>
+  <si>
+    <t>The maximum value for the cell (exclusive).</t>
+  </si>
+  <si>
+    <t>maxInclusive</t>
+  </si>
+  <si>
+    <t>max inclusive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
+  </si>
+  <si>
+    <t>maxLength</t>
+  </si>
+  <si>
+    <t>max length</t>
+  </si>
+  <si>
+    <t>right to left</t>
+  </si>
+  <si>
+    <t>Indiects text should be processed right to left</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://creativecommons.org/ns#</t>
+    </r>
+  </si>
+  <si>
+    <t>csvw</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://www.w3.org/ns/csvw#</t>
+    </r>
+  </si>
+  <si>
+    <t>ctag</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://commontag.org/ns#</t>
+    </r>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
   <si>
     <r>
       <rPr>
@@ -287,9 +1081,6 @@
     </r>
   </si>
   <si>
-    <t>schema</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -479,791 +1270,11 @@
   <si>
     <t>@vocab</t>
   </si>
-  <si>
-    <t>An atomic property holding a single string that provides a default string value for the cell in cases where the original string value is a null value. This default value may be used when converting the table into other formats.</t>
-  </si>
-  <si>
-    <t>delimiter</t>
-  </si>
-  <si>
-    <t>The separator between cells. The default is ",".</t>
-  </si>
-  <si>
-    <t>dialect</t>
-  </si>
-  <si>
-    <t>TableGroup,Table</t>
-  </si>
-  <si>
-    <t>Provides hints to processors about how to parse the referenced files for to create tabular data models for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>doubleQuote</t>
-  </si>
-  <si>
-    <t>double quote</t>
-  </si>
-  <si>
-    <t>xsd:boolean</t>
-  </si>
-  <si>
-    <t>If true, sets the escape character flag to ". If false, to \\.</t>
-  </si>
-  <si>
-    <t>encoding</t>
-  </si>
-  <si>
-    <t>The character encoding for the file, one of the encodings listed in [encoding]. The default is utf-8.</t>
-  </si>
-  <si>
-    <t>foreignKeys</t>
-  </si>
-  <si>
-    <t>foreign keys</t>
-  </si>
-  <si>
-    <t>An array of foreign key definitions that define how the values from specified columns within this table link to rows within this table or other tables.</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>A definition of the format of the cell, used when parsing the cell.</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>headerColumnCount</t>
-  </si>
-  <si>
-    <t>header column count</t>
-  </si>
-  <si>
-    <t>xsd:nonNegativeInteger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of header columns (following the skipped columns) in each row. The default is 0.
-</t>
-  </si>
-  <si>
-    <t>headerRowCount</t>
-  </si>
-  <si>
-    <t>header row count</t>
-  </si>
-  <si>
-    <t>The number of header rows (following the skipped rows) in the file. The default is 1.</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>subClassOf</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>ltr</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>left to right</t>
-  </si>
-  <si>
-    <t>Indicates text should be processed left to right.</t>
-  </si>
-  <si>
-    <t>rtl</t>
-  </si>
-  <si>
-    <t>max exclusive</t>
-  </si>
-  <si>
-    <t>The maximum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t>maxInclusive</t>
-  </si>
-  <si>
-    <t>max inclusive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum value for the cell (inclusive). </t>
-  </si>
-  <si>
-    <t>maxLength</t>
-  </si>
-  <si>
-    <t>max length</t>
-  </si>
-  <si>
-    <t>right to left</t>
-  </si>
-  <si>
-    <t>Indiects text should be processed right to left</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>http://creativecommons.org/ns#</t>
-    </r>
-  </si>
-  <si>
-    <t>csvw</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>http://www.w3.org/ns/csvw#</t>
-    </r>
-  </si>
-  <si>
-    <t>ctag</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>http://commontag.org/ns#</t>
-    </r>
-  </si>
-  <si>
-    <t>dc</t>
-  </si>
-  <si>
-    <t>An atomic property that gives a canonical name for the column. This must be a string. Conversion specifications must use this property as the basis for the names of properties/elements/attributes in the results of conversions.</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>An array of objects representing annotations. This specification does not place any constraints on the structure of these objects.</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>The string used for null values. If not specified, the default for this is the empty string.</t>
-  </si>
-  <si>
-    <t>predicateUrl</t>
-  </si>
-  <si>
-    <t>predicate URL</t>
-  </si>
-  <si>
-    <t>xsd:anyURI</t>
-  </si>
-  <si>
-    <t>An atomic property that holds one or more URIs that may be used as URIs for predicates if the table is mapped to another format.</t>
-  </si>
-  <si>
-    <t>primaryKey</t>
-  </si>
-  <si>
-    <t>primary key</t>
-  </si>
-  <si>
-    <t>A column reference property that holds either a single reference to a column description object or an array of references.</t>
-  </si>
-  <si>
-    <t>quoteChar</t>
-  </si>
-  <si>
-    <t>quote char</t>
-  </si>
-  <si>
-    <t>The character that is used around escaped cells.</t>
-  </si>
-  <si>
-    <t>A boolean value which indicates whether every cell within the column must have a non-null value.</t>
-  </si>
-  <si>
-    <t>resources</t>
-  </si>
-  <si>
-    <t>TableGroup</t>
-  </si>
-  <si>
-    <t>An array of table descriptions for the tables in the group.</t>
-  </si>
-  <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>rdfs:member</t>
-  </si>
-  <si>
-    <t>xsd</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>http://www.w3.org/2001/XMLSchema#</t>
-    </r>
-  </si>
-  <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>rdf:Property</t>
-  </si>
-  <si>
-    <t>Schema</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>An array of Column Descriptions.</t>
-  </si>
-  <si>
-    <t>commentPrefix</t>
-  </si>
-  <si>
-    <t>comment prefix</t>
-  </si>
-  <si>
-    <t>Dialect</t>
-  </si>
-  <si>
-    <t>An object property that provides a schema description for an individual table, or all the tables in a group.</t>
-  </si>
-  <si>
-    <t>separator</t>
-  </si>
-  <si>
-    <t>The character used to separate items in the string value of the cell.</t>
-  </si>
-  <si>
-    <t>skipBlankRows</t>
-  </si>
-  <si>
-    <t>skip blank rows</t>
-  </si>
-  <si>
-    <t>TableGroup,Table,Schema,Column</t>
-  </si>
-  <si>
-    <t>The main datatype of the values of the cell. If the cell contains a list (ie separator is specified and not null) then this is the datatype of each value within the list.</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>The number of columns to skip at the beginning of each row, before any header columns. The default is 0.</t>
-  </si>
-  <si>
-    <t>skipInitialSpace</t>
-  </si>
-  <si>
-    <t>skip initial space</t>
-  </si>
-  <si>
-    <t>skip columns</t>
-  </si>
-  <si>
-    <t>If true, sets the trim flag to "start". If false, to false.</t>
-  </si>
-  <si>
-    <t>skipRows</t>
-  </si>
-  <si>
-    <t>skip rows</t>
-  </si>
-  <si>
-    <t>The number of rows to skip at the beginning of the file, before a header row or tabular data.</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>The format to which the tabular data should be transformed prior to the transformation using the template. If the value is "json", the tabular data should first be transformed first to JSON based on the simple mapping defined in Generating JSON from Tabular Data on the Web. If the value is "rdf", it should similarly first be transformed to XML based on the simple mapping defined in Generating RDF from Tabular Data on the Web.</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
-    <t>Relates an Table group to annotated tables. (Note, this is different from csvw:resources, which relates metadata, rather than resulting annotated table descriptions.</t>
-  </si>
-  <si>
-    <t>table-direction</t>
-  </si>
-  <si>
-    <t>table direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of csvw:rtl csvw:ltr or csvw:default. Indicates whether the tables in the group should be displayed with the first column on the right, on the left, or based on the first character in the table that has a specific direction. </t>
-  </si>
-  <si>
-    <t>targetFormat</t>
-  </si>
-  <si>
-    <t>target format</t>
-  </si>
-  <si>
-    <t>A language code as defined by [BCP47]. Indicates the language of the value within the cell.</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>The exact length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>lineTerminator</t>
-  </si>
-  <si>
-    <t>line terminator</t>
-  </si>
-  <si>
-    <t>The character that is used at the end of a row. The default is CRLF.</t>
-  </si>
-  <si>
-    <t>maxExclusive</t>
-  </si>
-  <si>
-    <t>The maximum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>minExclusive</t>
-  </si>
-  <si>
-    <t>min exclusive</t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (exclusive).</t>
-  </si>
-  <si>
-    <t>minInclusive</t>
-  </si>
-  <si>
-    <t>min inclusive</t>
-  </si>
-  <si>
-    <t>The minimum value for the cell (inclusive).</t>
-  </si>
-  <si>
-    <t>minLength</t>
-  </si>
-  <si>
-    <t>min length</t>
-  </si>
-  <si>
-    <t>The minimum length of the value of the cell.</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>uri template</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>A URL for the format that will be created through the transformation. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/text/calendar. Otherwise, it can be any URL that describes the target format.</t>
-  </si>
-  <si>
-    <t>templateFormat</t>
-  </si>
-  <si>
-    <t>template format</t>
-  </si>
-  <si>
-    <t>A URL for the format that is used by the template. If one has been defined, this should be a URL for a media type, in the form http://www.iana.org/assignments/media-types/media-type such as http://www.iana.org/assignments/media-types/application/javascript. Otherwise, it can be any URL that describes the template format.</t>
-  </si>
-  <si>
-    <t>templates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An array of template specifications that provide mechanisms to transform the tabular data into other formats. </t>
-  </si>
-  <si>
-    <t>text-direction</t>
-  </si>
-  <si>
-    <t>text direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of csvw:rtl or csvw:ltr. Indicates whether the text within cells should be displayed by default as left-to-right or right-to-left text. </t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Template,Column</t>
-  </si>
-  <si>
-    <t>For a Template: A natural language property that describes the format that will be generated from the transformation. This is useful if the target format is a generic format (such as application/json) and the transformation is creating a specific profile of that format.
-For a Column: A natural language property that provides possible alternative names for the column.</t>
-  </si>
-  <si>
-    <t>trim</t>
-  </si>
-  <si>
-    <t>Indicates whether to trim whitespace around cells; may be true, false, start or end. The default is false.</t>
-  </si>
-  <si>
-    <t>rdfs:Class</t>
-  </si>
-  <si>
-    <t>Column Description</t>
-  </si>
-  <si>
-    <t>A Column Description describes a single column.</t>
-  </si>
-  <si>
-    <t>Dialect Description</t>
-  </si>
-  <si>
-    <t>A Dialect Description provides hints to parsers about how to parse a linked file.</t>
-  </si>
-  <si>
-    <t>The class of table/text directions.</t>
-  </si>
-  <si>
-    <t>Relates a Table to each Row output.</t>
-  </si>
-  <si>
-    <t>Indicates whether to ignore wholly empty rows (ie rows in which all the cells are empty). The default is false.</t>
-  </si>
-  <si>
-    <t>skipColumns</t>
-  </si>
-  <si>
-    <t>xsd:anyURI</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>csvw:uriTemplate</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>A URL template property that may be used to create a unique identifier for each row when mapping data to other formats.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gYearMonth</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gYear</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gMonthDay</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gDay</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gMonth</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>hexBinary</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>base64Binary</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>anyURI</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>sch</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Schema is a definition of a tabular format that may be common to multiple tables.</t>
-  </si>
-  <si>
-    <t>Table Description</t>
-  </si>
-  <si>
-    <t>A table description is a JSON object that describes a table within a CSV file.</t>
-  </si>
-  <si>
-    <t>Table Group Description</t>
-  </si>
-  <si>
-    <t>A Table Group Description describes a group of Tables.</t>
-  </si>
-  <si>
-    <t>Template Specification</t>
-  </si>
-  <si>
-    <t>A Template Specification is a definition of how tabular data can be transformed into another format.</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
-    <t>rdfs:Datatype</t>
-  </si>
-  <si>
-    <t>rdfs:Literal</t>
-  </si>
-  <si>
-    <t>A literal containing JSON.</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>xsd:anySimpleType</t>
-  </si>
-  <si>
-    <t>binary</t>
-  </si>
-  <si>
-    <t>xsd:base64Binary</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>xsd:dateTime</t>
-  </si>
-  <si>
-    <t>describedby</t>
-  </si>
-  <si>
-    <t>wrds:describedby</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>rdf:HTML</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
-    <t>xhv:license</t>
-  </si>
-  <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t>csvw:maxInclusive</t>
-  </si>
-  <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>csvw:minInclusive</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>xsd:double</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>xhv:role</t>
-  </si>
-  <si>
-    <t>rdf:XMLLiteral</t>
-  </si>
-  <si>
-    <t>anySimpleType</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>normalizedString</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>NCName</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>decimal</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>nonPositiveInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>negativeInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>long</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>short</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>byte</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>nonNegativeInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedLong</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedInt</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedShort</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>unsignedByte</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>positiveInteger</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>double</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>duration</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>dateTime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>date</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>urlTemplate</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>URL template</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>uriTemplate</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>rdfs:Datatype</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -2688,11 +2699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:IV141"/>
+  <dimension ref="A1:IV142"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:IV42"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1"/>
@@ -2707,22 +2718,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>96</v>
+        <v>208</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>97</v>
+        <v>209</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>99</v>
+        <v>211</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"@type"</f>
@@ -2733,21 +2744,21 @@
         <v>@container</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>105</v>
+        <v>217</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2756,18 +2767,18 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>115</v>
+        <v>227</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2776,19 +2787,19 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6" t="s">
-        <v>116</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>229</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2799,14 +2810,14 @@
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2817,14 +2828,14 @@
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2835,14 +2846,14 @@
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>0</v>
+        <v>237</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2853,14 +2864,14 @@
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>2</v>
+        <v>239</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2871,14 +2882,14 @@
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>3</v>
+        <v>240</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -2889,14 +2900,14 @@
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>242</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>0</v>
+        <v>237</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2907,14 +2918,14 @@
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>6</v>
+        <v>243</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4" t="s">
-        <v>7</v>
+        <v>244</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2925,14 +2936,14 @@
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>8</v>
+        <v>245</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>246</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2943,14 +2954,14 @@
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>247</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>248</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2961,14 +2972,14 @@
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>249</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>13</v>
+        <v>250</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -2979,14 +2990,14 @@
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>251</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -2997,14 +3008,14 @@
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>253</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>17</v>
+        <v>254</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -3015,14 +3026,14 @@
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>255</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>19</v>
+        <v>256</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -3033,14 +3044,14 @@
     </row>
     <row r="18" spans="1:10" ht="19" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>257</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -3051,14 +3062,14 @@
     </row>
     <row r="19" spans="1:10" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>259</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4" t="s">
-        <v>23</v>
+        <v>260</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -3069,14 +3080,14 @@
     </row>
     <row r="20" spans="1:10" ht="19" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>261</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>262</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3087,14 +3098,14 @@
     </row>
     <row r="21" spans="1:10" ht="19" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>264</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -3105,14 +3116,14 @@
     </row>
     <row r="22" spans="1:10" ht="19" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>265</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>266</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3123,14 +3134,14 @@
     </row>
     <row r="23" spans="1:10" ht="19" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>30</v>
+        <v>267</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>268</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3141,14 +3152,14 @@
     </row>
     <row r="24" spans="1:10" ht="19" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>269</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
-        <v>33</v>
+        <v>270</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -3159,14 +3170,14 @@
     </row>
     <row r="25" spans="1:10" ht="19" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>34</v>
+        <v>271</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
-        <v>35</v>
+        <v>272</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -3177,14 +3188,14 @@
     </row>
     <row r="26" spans="1:10" ht="19" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>273</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
-        <v>37</v>
+        <v>274</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3195,14 +3206,14 @@
     </row>
     <row r="27" spans="1:10" ht="19" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>236</v>
+        <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4" t="s">
-        <v>39</v>
+        <v>275</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -3213,14 +3224,14 @@
     </row>
     <row r="28" spans="1:10" ht="19" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
-        <v>41</v>
+        <v>277</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -3231,14 +3242,14 @@
     </row>
     <row r="29" spans="1:10" ht="19" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>42</v>
+        <v>278</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>279</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -3249,14 +3260,14 @@
     </row>
     <row r="30" spans="1:10" ht="19" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>44</v>
+        <v>280</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>45</v>
+        <v>281</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3267,14 +3278,14 @@
     </row>
     <row r="31" spans="1:10" ht="19" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>46</v>
+        <v>282</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
-        <v>47</v>
+        <v>283</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -3285,14 +3296,14 @@
     </row>
     <row r="32" spans="1:10" ht="19" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>48</v>
+        <v>284</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -3303,14 +3314,14 @@
     </row>
     <row r="33" spans="1:256" ht="19" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>50</v>
+        <v>286</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
-        <v>51</v>
+        <v>287</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -3321,14 +3332,14 @@
     </row>
     <row r="34" spans="1:256" ht="19" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4" t="s">
-        <v>53</v>
+        <v>289</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3339,14 +3350,14 @@
     </row>
     <row r="35" spans="1:256" ht="19" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>54</v>
+        <v>290</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
-        <v>55</v>
+        <v>291</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -3357,14 +3368,14 @@
     </row>
     <row r="36" spans="1:256" ht="19" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>56</v>
+        <v>292</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
-        <v>57</v>
+        <v>293</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3375,14 +3386,14 @@
     </row>
     <row r="37" spans="1:256" ht="19" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
-        <v>59</v>
+        <v>295</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -3393,14 +3404,14 @@
     </row>
     <row r="38" spans="1:256" ht="19" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>60</v>
+        <v>296</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>61</v>
+        <v>297</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3411,14 +3422,14 @@
     </row>
     <row r="39" spans="1:256" ht="19" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="4" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -3429,20 +3440,20 @@
     </row>
     <row r="40" spans="1:256" ht="19" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="4" t="str">
@@ -3451,57 +3462,57 @@
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="6" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:256" ht="60" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="6" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:256" ht="60" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>64</v>
+        <v>300</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>64</v>
+        <v>300</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>68</v>
+        <v>304</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="11" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
@@ -3752,188 +3763,188 @@
     </row>
     <row r="43" spans="1:256" ht="75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="6" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:256" ht="19" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>62</v>
+        <v>298</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>70</v>
+        <v>182</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:256" ht="45" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>72</v>
+        <v>184</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>72</v>
+        <v>184</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="6" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:256" ht="30" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>75</v>
+        <v>187</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:256" ht="30" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>79</v>
+        <v>191</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>79</v>
+        <v>191</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="6" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:256" ht="45" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="6" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="19" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -3942,284 +3953,284 @@
     </row>
     <row r="51" spans="1:10" ht="45" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="6" t="s">
-        <v>90</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>91</v>
+        <v>203</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>92</v>
+        <v>204</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="6" t="s">
-        <v>93</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="6" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="19" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="6" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>186</v>
+        <v>122</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="6" t="s">
-        <v>188</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="19" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>108</v>
+        <v>220</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>66</v>
+        <v>302</v>
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="4" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="19" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>110</v>
+        <v>222</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>66</v>
+        <v>302</v>
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="4" t="s">
-        <v>112</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="19" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>113</v>
+        <v>225</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="6" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="19" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>66</v>
+        <v>302</v>
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="4" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="19" customHeight="1">
       <c r="A60" s="4" t="s">
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>66</v>
+        <v>302</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="4" t="s">
-        <v>196</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="19" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="6" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="75" customHeight="1">
       <c r="A62" s="4" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
@@ -4227,167 +4238,167 @@
         <v>1</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="6" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="30" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="45" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="6" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="45" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="6" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="19" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="30" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="G69" s="5"/>
       <c r="H69" s="4" t="str">
@@ -4398,24 +4409,24 @@
         <v>1</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="19" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4425,195 +4436,195 @@
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="6" t="s">
-        <v>222</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="45" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="4" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="6" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="30" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="6" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="45" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6" t="s">
-        <v>223</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>224</v>
+        <v>102</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="19" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="30" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="135" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>65</v>
+        <v>301</v>
       </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="60" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="4" t="str">
@@ -4622,25 +4633,25 @@
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="6" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="75" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>178</v>
+        <v>114</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>179</v>
+        <v>115</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="G79" s="4" t="str">
         <f>"@vocab"</f>
@@ -4649,97 +4660,97 @@
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="120" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>182</v>
+        <v>118</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>67</v>
+        <v>303</v>
       </c>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6" t="s">
-        <v>202</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="120" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>204</v>
+        <v>82</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>67</v>
+        <v>303</v>
       </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="6" t="s">
-        <v>205</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="45" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>206</v>
+        <v>84</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>206</v>
+        <v>84</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="45" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>208</v>
+        <v>86</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>209</v>
+        <v>87</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="G83" s="4" t="str">
         <f>"@vocab"</f>
@@ -4748,22 +4759,22 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6" t="s">
-        <v>210</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="135" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>211</v>
+        <v>89</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>211</v>
+        <v>89</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>212</v>
+        <v>90</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -4773,66 +4784,66 @@
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="6" t="s">
-        <v>213</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>214</v>
+        <v>92</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>214</v>
+        <v>92</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="6" t="s">
-        <v>215</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="45" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>297</v>
+        <v>74</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>298</v>
+        <v>75</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>226</v>
+        <v>4</v>
       </c>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6" t="s">
-        <v>227</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="19" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>217</v>
+        <v>95</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -4841,18 +4852,18 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="6" t="s">
-        <v>218</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="30" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>219</v>
+        <v>97</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -4861,18 +4872,18 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="6" t="s">
-        <v>220</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="19" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -4881,18 +4892,18 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6" t="s">
-        <v>221</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="30" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -4901,18 +4912,18 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6" t="s">
-        <v>237</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="30" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>238</v>
+        <v>15</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -4921,18 +4932,18 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6" t="s">
-        <v>239</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="30" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>240</v>
+        <v>17</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -4941,18 +4952,18 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6" t="s">
-        <v>241</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="45" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>242</v>
+        <v>19</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -4961,21 +4972,21 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6" t="s">
-        <v>243</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="19" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>244</v>
+        <v>21</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>244</v>
+        <v>21</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>246</v>
+        <v>23</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -4983,21 +4994,21 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6" t="s">
-        <v>247</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="19" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>299</v>
+        <v>76</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>300</v>
+        <v>77</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>225</v>
+        <v>103</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
@@ -5008,14 +5019,14 @@
     </row>
     <row r="96" spans="1:10" ht="19" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>248</v>
+        <v>25</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="4" t="s">
-        <v>250</v>
+        <v>27</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -5026,14 +5037,14 @@
     </row>
     <row r="97" spans="1:10" ht="19" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>251</v>
+        <v>28</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="4" t="s">
-        <v>252</v>
+        <v>29</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -5044,14 +5055,14 @@
     </row>
     <row r="98" spans="1:10" ht="19" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>253</v>
+        <v>30</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="4" t="s">
-        <v>254</v>
+        <v>31</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -5062,14 +5073,14 @@
     </row>
     <row r="99" spans="1:10" ht="19" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>255</v>
+        <v>32</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="4" t="s">
-        <v>256</v>
+        <v>33</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -5080,14 +5091,14 @@
     </row>
     <row r="100" spans="1:10" ht="19" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>257</v>
+        <v>34</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="4" t="s">
-        <v>258</v>
+        <v>35</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -5098,14 +5109,14 @@
     </row>
     <row r="101" spans="1:10" ht="19" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>259</v>
+        <v>36</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="4" t="s">
-        <v>260</v>
+        <v>37</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
@@ -5116,14 +5127,14 @@
     </row>
     <row r="102" spans="1:10" ht="19" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>261</v>
+        <v>38</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="4" t="s">
-        <v>262</v>
+        <v>39</v>
       </c>
       <c r="E102" s="9"/>
       <c r="F102" s="5"/>
@@ -5134,14 +5145,14 @@
     </row>
     <row r="103" spans="1:10" ht="19" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>263</v>
+        <v>40</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
-        <v>264</v>
+        <v>41</v>
       </c>
       <c r="E103" s="9"/>
       <c r="F103" s="5"/>
@@ -5152,14 +5163,14 @@
     </row>
     <row r="104" spans="1:10" ht="19" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>265</v>
+        <v>42</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="4" t="s">
-        <v>266</v>
+        <v>43</v>
       </c>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
@@ -5170,14 +5181,14 @@
     </row>
     <row r="105" spans="1:10" ht="19" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>267</v>
+        <v>44</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="4" t="s">
-        <v>268</v>
+        <v>45</v>
       </c>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
@@ -5188,14 +5199,14 @@
     </row>
     <row r="106" spans="1:10" ht="19" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>60</v>
+        <v>296</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="4" t="s">
-        <v>269</v>
+        <v>46</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
@@ -5206,10 +5217,10 @@
     </row>
     <row r="107" spans="1:10" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>270</v>
+        <v>47</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="4" t="str">
@@ -5225,14 +5236,14 @@
     </row>
     <row r="108" spans="1:10" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>271</v>
+        <v>48</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4" t="str">
-        <f t="shared" ref="D108:D141" si="0">CONCATENATE("xsd:",A108)</f>
+        <f t="shared" ref="D108:D142" si="0">CONCATENATE("xsd:",A108)</f>
         <v>xsd:string</v>
       </c>
       <c r="E108" s="5"/>
@@ -5244,10 +5255,10 @@
     </row>
     <row r="109" spans="1:10" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>272</v>
+        <v>49</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4" t="str">
@@ -5263,10 +5274,10 @@
     </row>
     <row r="110" spans="1:10" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="str">
@@ -5282,10 +5293,10 @@
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>274</v>
+        <v>51</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="str">
@@ -5301,10 +5312,10 @@
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>275</v>
+        <v>52</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="str">
@@ -5320,10 +5331,10 @@
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>276</v>
+        <v>53</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="str">
@@ -5339,15 +5350,14 @@
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>277</v>
+        <v>78</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>249</v>
+        <v>79</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:decimal</v>
+      <c r="D114" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
@@ -5358,15 +5368,15 @@
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>278</v>
+        <v>54</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:integer</v>
+        <v>xsd:decimal</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
@@ -5377,15 +5387,15 @@
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>279</v>
+        <v>55</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonPositiveInteger</v>
+        <v>xsd:integer</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
@@ -5396,15 +5406,15 @@
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>280</v>
+        <v>56</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:negativeInteger</v>
+        <v>xsd:nonPositiveInteger</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
@@ -5415,15 +5425,15 @@
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>281</v>
+        <v>57</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:long</v>
+        <v>xsd:negativeInteger</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
@@ -5434,15 +5444,15 @@
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>282</v>
+        <v>58</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:int</v>
+        <v>xsd:long</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
@@ -5453,15 +5463,15 @@
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>283</v>
+        <v>59</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:short</v>
+        <v>xsd:int</v>
       </c>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
@@ -5472,15 +5482,15 @@
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>284</v>
+        <v>60</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:byte</v>
+        <v>xsd:short</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
@@ -5491,15 +5501,15 @@
     </row>
     <row r="122" spans="1:10" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>285</v>
+        <v>61</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonNegativeInteger</v>
+        <v>xsd:byte</v>
       </c>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -5510,15 +5520,15 @@
     </row>
     <row r="123" spans="1:10" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>286</v>
+        <v>62</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedLong</v>
+        <v>xsd:nonNegativeInteger</v>
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -5529,15 +5539,15 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>287</v>
+        <v>63</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedInt</v>
+        <v>xsd:unsignedLong</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
@@ -5548,15 +5558,15 @@
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>288</v>
+        <v>64</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedShort</v>
+        <v>xsd:unsignedInt</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
@@ -5567,15 +5577,15 @@
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>289</v>
+        <v>65</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedByte</v>
+        <v>xsd:unsignedShort</v>
       </c>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
@@ -5586,15 +5596,15 @@
     </row>
     <row r="127" spans="1:10" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>290</v>
+        <v>66</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:positiveInteger</v>
+        <v>xsd:unsignedByte</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
@@ -5605,15 +5615,15 @@
     </row>
     <row r="128" spans="1:10" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>291</v>
+        <v>67</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:float</v>
+        <v>xsd:positiveInteger</v>
       </c>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
@@ -5624,15 +5634,15 @@
     </row>
     <row r="129" spans="1:10" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>292</v>
+        <v>68</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:double</v>
+        <v>xsd:float</v>
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
@@ -5643,15 +5653,15 @@
     </row>
     <row r="130" spans="1:10" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>293</v>
+        <v>69</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:duration</v>
+        <v>xsd:double</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
@@ -5662,15 +5672,15 @@
     </row>
     <row r="131" spans="1:10" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>294</v>
+        <v>70</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:dateTime</v>
+        <v>xsd:duration</v>
       </c>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
@@ -5681,15 +5691,15 @@
     </row>
     <row r="132" spans="1:10" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>295</v>
+        <v>71</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:time</v>
+        <v>xsd:dateTime</v>
       </c>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
@@ -5700,15 +5710,15 @@
     </row>
     <row r="133" spans="1:10" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>296</v>
+        <v>72</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C133" s="4"/>
       <c r="D133" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:date</v>
+        <v>xsd:time</v>
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
@@ -5719,15 +5729,15 @@
     </row>
     <row r="134" spans="1:10" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>228</v>
+        <v>73</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYearMonth</v>
+        <v>xsd:date</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
@@ -5738,15 +5748,15 @@
     </row>
     <row r="135" spans="1:10" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>229</v>
+        <v>6</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYear</v>
+        <v>xsd:gYearMonth</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
@@ -5757,15 +5767,15 @@
     </row>
     <row r="136" spans="1:10" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>230</v>
+        <v>7</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C136" s="4"/>
       <c r="D136" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonthDay</v>
+        <v>xsd:gYear</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
@@ -5776,15 +5786,15 @@
     </row>
     <row r="137" spans="1:10" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>231</v>
+        <v>8</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gDay</v>
+        <v>xsd:gMonthDay</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
@@ -5795,15 +5805,15 @@
     </row>
     <row r="138" spans="1:10" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>232</v>
+        <v>9</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonth</v>
+        <v>xsd:gDay</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
@@ -5814,15 +5824,15 @@
     </row>
     <row r="139" spans="1:10" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>233</v>
+        <v>10</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C139" s="4"/>
       <c r="D139" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:hexBinary</v>
+        <v>xsd:gMonth</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
@@ -5833,15 +5843,15 @@
     </row>
     <row r="140" spans="1:10" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>234</v>
+        <v>11</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C140" s="4"/>
       <c r="D140" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:base64Binary</v>
+        <v>xsd:hexBinary</v>
       </c>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
@@ -5852,15 +5862,15 @@
     </row>
     <row r="141" spans="1:10" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:anyURI</v>
+        <v>xsd:base64Binary</v>
       </c>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
@@ -5868,6 +5878,25 @@
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
       <c r="J141" s="7"/>
+    </row>
+    <row r="142" spans="1:10" ht="15" customHeight="1">
+      <c r="A142" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C142" s="4"/>
+      <c r="D142" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:anyURI</v>
+      </c>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="5"/>
+      <c r="J142" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Update namespace description for `Table` and `TableGroup`. This fixes issue #113.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="-320" windowWidth="23600" windowHeight="26560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -176,13 +176,7 @@
     <t>Table Description</t>
   </si>
   <si>
-    <t>A table description is a JSON object that describes a table within a CSV file.</t>
-  </si>
-  <si>
     <t>Table Group Description</t>
-  </si>
-  <si>
-    <t>A Table Group Description describes a group of Tables.</t>
   </si>
   <si>
     <t>Template Specification</t>
@@ -1303,18 +1297,18 @@
     <t>delimiter</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>A Table describes an Annotated Table.</t>
+  </si>
+  <si>
+    <t>A Table Group describes an Annotated Table Group.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1339,6 +1333,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -1389,8 +1389,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
@@ -1420,11 +1423,12 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2737,15 +2741,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J89" sqref="J89"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="8.125" style="1"/>
     <col min="4" max="4" width="20.25" style="1" customWidth="1"/>
@@ -2757,22 +2761,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"@type"</f>
@@ -2783,21 +2787,21 @@
         <v>@container</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2806,18 +2810,18 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2826,19 +2830,19 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2849,14 +2853,14 @@
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2867,14 +2871,14 @@
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2885,14 +2889,14 @@
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2903,14 +2907,14 @@
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2921,14 +2925,14 @@
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -2939,14 +2943,14 @@
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2957,14 +2961,14 @@
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2975,14 +2979,14 @@
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2993,14 +2997,14 @@
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -3011,14 +3015,14 @@
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -3029,14 +3033,14 @@
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -3047,14 +3051,14 @@
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -3065,14 +3069,14 @@
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -3083,14 +3087,14 @@
     </row>
     <row r="18" spans="1:10" ht="19" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -3101,14 +3105,14 @@
     </row>
     <row r="19" spans="1:10" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -3119,14 +3123,14 @@
     </row>
     <row r="20" spans="1:10" ht="19" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3137,14 +3141,14 @@
     </row>
     <row r="21" spans="1:10" ht="19" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -3155,14 +3159,14 @@
     </row>
     <row r="22" spans="1:10" ht="19" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3173,14 +3177,14 @@
     </row>
     <row r="23" spans="1:10" ht="19" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3191,14 +3195,14 @@
     </row>
     <row r="24" spans="1:10" ht="19" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -3209,14 +3213,14 @@
     </row>
     <row r="25" spans="1:10" ht="19" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -3227,14 +3231,14 @@
     </row>
     <row r="26" spans="1:10" ht="19" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3248,11 +3252,11 @@
         <v>27</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -3263,14 +3267,14 @@
     </row>
     <row r="28" spans="1:10" ht="19" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -3281,14 +3285,14 @@
     </row>
     <row r="29" spans="1:10" ht="19" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -3299,14 +3303,14 @@
     </row>
     <row r="30" spans="1:10" ht="19" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3317,14 +3321,14 @@
     </row>
     <row r="31" spans="1:10" ht="19" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -3335,14 +3339,14 @@
     </row>
     <row r="32" spans="1:10" ht="19" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -3353,14 +3357,14 @@
     </row>
     <row r="33" spans="1:256" ht="19" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -3371,14 +3375,14 @@
     </row>
     <row r="34" spans="1:256" ht="19" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3389,14 +3393,14 @@
     </row>
     <row r="35" spans="1:256" ht="19" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -3407,14 +3411,14 @@
     </row>
     <row r="36" spans="1:256" ht="19" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3425,14 +3429,14 @@
     </row>
     <row r="37" spans="1:256" ht="19" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -3443,14 +3447,14 @@
     </row>
     <row r="38" spans="1:256" ht="19" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3461,14 +3465,14 @@
     </row>
     <row r="39" spans="1:256" ht="19" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -3482,14 +3486,14 @@
         <v>11</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>30</v>
@@ -3503,20 +3507,20 @@
     </row>
     <row r="41" spans="1:256" ht="19" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="4" t="str">
@@ -3525,57 +3529,57 @@
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:256" ht="60" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:256" ht="60" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K43"/>
       <c r="L43"/>
@@ -3826,188 +3830,188 @@
     </row>
     <row r="44" spans="1:256" ht="75" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:256" ht="19" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:256" ht="45" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G46" s="9"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:256" ht="30" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:256" ht="30" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="19" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
@@ -4016,284 +4020,284 @@
     </row>
     <row r="52" spans="1:10" ht="45" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="19" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="19" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="19" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="19" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="19" customHeight="1">
       <c r="A60" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="19" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="19" customHeight="1">
       <c r="A62" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="75" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
@@ -4301,53 +4305,53 @@
         <v>1</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="45" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="30" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="45" customHeight="1">
@@ -4355,14 +4359,14 @@
         <v>12</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>30</v>
@@ -4376,92 +4380,92 @@
     </row>
     <row r="67" spans="1:10" ht="45" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="19" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="30" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G70" s="5"/>
       <c r="H70" s="4" t="str">
@@ -4472,24 +4476,24 @@
         <v>1</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="19" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
@@ -4507,187 +4511,187 @@
         <v>28</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="30" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="45" customHeight="1">
       <c r="A75" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="19" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="135" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="60" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G79" s="5"/>
       <c r="H79" s="4" t="str">
@@ -4696,25 +4700,25 @@
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="75" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G80" s="4" t="str">
         <f>"@vocab"</f>
@@ -4723,97 +4727,97 @@
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="120" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="120" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="45" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="45" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G84" s="4" t="str">
         <f>"@vocab"</f>
@@ -4822,22 +4826,22 @@
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="135" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
@@ -4847,55 +4851,55 @@
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="30" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="45" customHeight="1">
@@ -4903,14 +4907,14 @@
         <v>16</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>30</v>
@@ -4924,7 +4928,7 @@
     </row>
     <row r="89" spans="1:10" ht="19" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>19</v>
@@ -4944,7 +4948,7 @@
     </row>
     <row r="90" spans="1:10" ht="30" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>19</v>
@@ -4964,13 +4968,13 @@
     </row>
     <row r="91" spans="1:10" ht="19" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -4984,13 +4988,13 @@
     </row>
     <row r="92" spans="1:10" ht="30" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -5004,7 +5008,7 @@
     </row>
     <row r="93" spans="1:10" ht="30" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>19</v>
@@ -5019,18 +5023,18 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6" t="s">
-        <v>41</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="30" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
@@ -5039,18 +5043,18 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6" t="s">
-        <v>43</v>
+        <v>311</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="45" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
@@ -5059,21 +5063,21 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="19" customHeight="1">
       <c r="A96" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -5081,21 +5085,21 @@
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="19" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -5106,14 +5110,14 @@
     </row>
     <row r="98" spans="1:10" ht="19" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -5124,14 +5128,14 @@
     </row>
     <row r="99" spans="1:10" ht="19" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -5142,14 +5146,14 @@
     </row>
     <row r="100" spans="1:10" ht="19" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -5160,14 +5164,14 @@
     </row>
     <row r="101" spans="1:10" ht="19" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
@@ -5178,14 +5182,14 @@
     </row>
     <row r="102" spans="1:10" ht="19" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
@@ -5196,14 +5200,14 @@
     </row>
     <row r="103" spans="1:10" ht="19" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -5214,14 +5218,14 @@
     </row>
     <row r="104" spans="1:10" ht="19" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E104" s="9"/>
       <c r="F104" s="5"/>
@@ -5232,14 +5236,14 @@
     </row>
     <row r="105" spans="1:10" ht="19" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E105" s="9"/>
       <c r="F105" s="5"/>
@@ -5250,14 +5254,14 @@
     </row>
     <row r="106" spans="1:10" ht="19" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
@@ -5268,14 +5272,14 @@
     </row>
     <row r="107" spans="1:10" ht="19" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
@@ -5286,14 +5290,14 @@
     </row>
     <row r="108" spans="1:10" ht="19" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
@@ -5304,10 +5308,10 @@
     </row>
     <row r="109" spans="1:10" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4" t="str">
@@ -5323,10 +5327,10 @@
     </row>
     <row r="110" spans="1:10" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="str">
@@ -5342,10 +5346,10 @@
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="str">
@@ -5361,10 +5365,10 @@
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="str">
@@ -5380,10 +5384,10 @@
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="str">
@@ -5399,10 +5403,10 @@
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="str">
@@ -5418,10 +5422,10 @@
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="str">
@@ -5437,10 +5441,10 @@
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="s">
@@ -5455,10 +5459,10 @@
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="str">
@@ -5474,10 +5478,10 @@
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="str">
@@ -5493,10 +5497,10 @@
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="str">
@@ -5512,10 +5516,10 @@
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="str">
@@ -5531,10 +5535,10 @@
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="str">
@@ -5550,10 +5554,10 @@
     </row>
     <row r="122" spans="1:10" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="str">
@@ -5569,10 +5573,10 @@
     </row>
     <row r="123" spans="1:10" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="str">
@@ -5588,10 +5592,10 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="str">
@@ -5607,10 +5611,10 @@
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="str">
@@ -5626,10 +5630,10 @@
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="str">
@@ -5648,7 +5652,7 @@
         <v>0</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="str">
@@ -5667,7 +5671,7 @@
         <v>1</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="str">
@@ -5686,7 +5690,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4" t="str">
@@ -5705,7 +5709,7 @@
         <v>3</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="4" t="str">
@@ -5724,7 +5728,7 @@
         <v>4</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4" t="str">
@@ -5743,7 +5747,7 @@
         <v>5</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="4" t="str">
@@ -5762,7 +5766,7 @@
         <v>6</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C133" s="4"/>
       <c r="D133" s="4" t="str">
@@ -5781,7 +5785,7 @@
         <v>7</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4" t="str">
@@ -5800,7 +5804,7 @@
         <v>8</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4" t="str">
@@ -5819,7 +5823,7 @@
         <v>9</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C136" s="4"/>
       <c r="D136" s="4" t="str">
@@ -5838,7 +5842,7 @@
         <v>31</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="str">
@@ -5857,7 +5861,7 @@
         <v>32</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="str">
@@ -5876,7 +5880,7 @@
         <v>33</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C139" s="4"/>
       <c r="D139" s="4" t="str">
@@ -5895,7 +5899,7 @@
         <v>34</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C140" s="4"/>
       <c r="D140" s="4" t="str">
@@ -5914,7 +5918,7 @@
         <v>35</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="4" t="str">
@@ -5933,7 +5937,7 @@
         <v>36</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C142" s="4"/>
       <c r="D142" s="4" t="str">
@@ -5952,7 +5956,7 @@
         <v>37</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C143" s="4"/>
       <c r="D143" s="4" t="str">
@@ -5971,7 +5975,7 @@
         <v>38</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C144" s="4"/>
       <c r="D144" s="4" t="str">
@@ -5986,7 +5990,6 @@
       <c r="J144" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -6027,12 +6030,12 @@
     <hyperlink ref="D39" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Add prov roles relating to issue #147.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="320">
   <si>
     <t>unsignedInt</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1305,6 +1305,27 @@
   </si>
   <si>
     <t>JSON</t>
+  </si>
+  <si>
+    <t>csvEncodedTabularData</t>
+  </si>
+  <si>
+    <t>prov:Role</t>
+  </si>
+  <si>
+    <t>CSV Encoded Tabular Data</t>
+  </si>
+  <si>
+    <t>tabularMetadata</t>
+  </si>
+  <si>
+    <t>Tabular Metadata</t>
+  </si>
+  <si>
+    <t>Describes the role of a CSV file in the tabular data mapping.</t>
+  </si>
+  <si>
+    <t>Describes the role of a Metadata file in the tabular data mapping.</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1413,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1426,8 +1450,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2745,11 +2770,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV144"/>
+  <dimension ref="A1:IV146"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -2838,50 +2863,54 @@
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>156</v>
+        <v>313</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="6" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>159</v>
+        <v>316</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4" t="s">
-        <v>160</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="6" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2892,14 +2921,14 @@
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>247</v>
+        <v>160</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2910,14 +2939,14 @@
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>248</v>
+        <v>161</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>249</v>
+        <v>162</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2928,14 +2957,14 @@
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>250</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -2946,14 +2975,14 @@
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2964,14 +2993,14 @@
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2982,14 +3011,14 @@
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -3000,14 +3029,14 @@
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -3018,14 +3047,14 @@
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -3036,14 +3065,14 @@
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -3054,14 +3083,14 @@
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -3072,14 +3101,14 @@
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -3090,14 +3119,14 @@
     </row>
     <row r="18" spans="1:10" ht="19" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -3108,14 +3137,14 @@
     </row>
     <row r="19" spans="1:10" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -3126,14 +3155,14 @@
     </row>
     <row r="20" spans="1:10" ht="19" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3144,14 +3173,14 @@
     </row>
     <row r="21" spans="1:10" ht="19" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -3162,14 +3191,14 @@
     </row>
     <row r="22" spans="1:10" ht="19" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3180,14 +3209,14 @@
     </row>
     <row r="23" spans="1:10" ht="19" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3198,14 +3227,14 @@
     </row>
     <row r="24" spans="1:10" ht="19" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -3216,14 +3245,14 @@
     </row>
     <row r="25" spans="1:10" ht="19" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -3234,14 +3263,14 @@
     </row>
     <row r="26" spans="1:10" ht="19" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3252,14 +3281,14 @@
     </row>
     <row r="27" spans="1:10" ht="19" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>27</v>
+        <v>281</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -3270,14 +3299,14 @@
     </row>
     <row r="28" spans="1:10" ht="19" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -3288,14 +3317,14 @@
     </row>
     <row r="29" spans="1:10" ht="19" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>288</v>
+        <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -3306,14 +3335,14 @@
     </row>
     <row r="30" spans="1:10" ht="19" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3324,14 +3353,14 @@
     </row>
     <row r="31" spans="1:10" ht="19" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -3342,14 +3371,14 @@
     </row>
     <row r="32" spans="1:10" ht="19" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -3360,14 +3389,14 @@
     </row>
     <row r="33" spans="1:256" ht="19" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -3378,14 +3407,14 @@
     </row>
     <row r="34" spans="1:256" ht="19" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3396,14 +3425,14 @@
     </row>
     <row r="35" spans="1:256" ht="19" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -3414,14 +3443,14 @@
     </row>
     <row r="36" spans="1:256" ht="19" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3432,14 +3461,14 @@
     </row>
     <row r="37" spans="1:256" ht="19" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -3450,14 +3479,14 @@
     </row>
     <row r="38" spans="1:256" ht="19" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3468,14 +3497,14 @@
     </row>
     <row r="39" spans="1:256" ht="19" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>182</v>
+        <v>304</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="4" t="s">
-        <v>183</v>
+        <v>305</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -3484,366 +3513,106 @@
       <c r="I39" s="5"/>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="1:256" ht="45" customHeight="1">
+    <row r="40" spans="1:256" ht="19" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>11</v>
+        <v>306</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:256" ht="19" customHeight="1">
-      <c r="A41" s="8" t="s">
-        <v>184</v>
+      <c r="A41" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="4" t="str">
-        <f>"@list"</f>
-        <v>@list</v>
-      </c>
+      <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:256" ht="60" customHeight="1">
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:256" ht="45" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>190</v>
+        <v>14</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:256" ht="60" customHeight="1">
-      <c r="A43" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B43" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:256" ht="19" customHeight="1">
+      <c r="A43" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-      <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
-      <c r="Q43"/>
-      <c r="R43"/>
-      <c r="S43"/>
-      <c r="T43"/>
-      <c r="U43"/>
-      <c r="V43"/>
-      <c r="W43"/>
-      <c r="X43"/>
-      <c r="Y43"/>
-      <c r="Z43"/>
-      <c r="AA43"/>
-      <c r="AB43"/>
-      <c r="AC43"/>
-      <c r="AD43"/>
-      <c r="AE43"/>
-      <c r="AF43"/>
-      <c r="AG43"/>
-      <c r="AH43"/>
-      <c r="AI43"/>
-      <c r="AJ43"/>
-      <c r="AK43"/>
-      <c r="AL43"/>
-      <c r="AM43"/>
-      <c r="AN43"/>
-      <c r="AO43"/>
-      <c r="AP43"/>
-      <c r="AQ43"/>
-      <c r="AR43"/>
-      <c r="AS43"/>
-      <c r="AT43"/>
-      <c r="AU43"/>
-      <c r="AV43"/>
-      <c r="AW43"/>
-      <c r="AX43"/>
-      <c r="AY43"/>
-      <c r="AZ43"/>
-      <c r="BA43"/>
-      <c r="BB43"/>
-      <c r="BC43"/>
-      <c r="BD43"/>
-      <c r="BE43"/>
-      <c r="BF43"/>
-      <c r="BG43"/>
-      <c r="BH43"/>
-      <c r="BI43"/>
-      <c r="BJ43"/>
-      <c r="BK43"/>
-      <c r="BL43"/>
-      <c r="BM43"/>
-      <c r="BN43"/>
-      <c r="BO43"/>
-      <c r="BP43"/>
-      <c r="BQ43"/>
-      <c r="BR43"/>
-      <c r="BS43"/>
-      <c r="BT43"/>
-      <c r="BU43"/>
-      <c r="BV43"/>
-      <c r="BW43"/>
-      <c r="BX43"/>
-      <c r="BY43"/>
-      <c r="BZ43"/>
-      <c r="CA43"/>
-      <c r="CB43"/>
-      <c r="CC43"/>
-      <c r="CD43"/>
-      <c r="CE43"/>
-      <c r="CF43"/>
-      <c r="CG43"/>
-      <c r="CH43"/>
-      <c r="CI43"/>
-      <c r="CJ43"/>
-      <c r="CK43"/>
-      <c r="CL43"/>
-      <c r="CM43"/>
-      <c r="CN43"/>
-      <c r="CO43"/>
-      <c r="CP43"/>
-      <c r="CQ43"/>
-      <c r="CR43"/>
-      <c r="CS43"/>
-      <c r="CT43"/>
-      <c r="CU43"/>
-      <c r="CV43"/>
-      <c r="CW43"/>
-      <c r="CX43"/>
-      <c r="CY43"/>
-      <c r="CZ43"/>
-      <c r="DA43"/>
-      <c r="DB43"/>
-      <c r="DC43"/>
-      <c r="DD43"/>
-      <c r="DE43"/>
-      <c r="DF43"/>
-      <c r="DG43"/>
-      <c r="DH43"/>
-      <c r="DI43"/>
-      <c r="DJ43"/>
-      <c r="DK43"/>
-      <c r="DL43"/>
-      <c r="DM43"/>
-      <c r="DN43"/>
-      <c r="DO43"/>
-      <c r="DP43"/>
-      <c r="DQ43"/>
-      <c r="DR43"/>
-      <c r="DS43"/>
-      <c r="DT43"/>
-      <c r="DU43"/>
-      <c r="DV43"/>
-      <c r="DW43"/>
-      <c r="DX43"/>
-      <c r="DY43"/>
-      <c r="DZ43"/>
-      <c r="EA43"/>
-      <c r="EB43"/>
-      <c r="EC43"/>
-      <c r="ED43"/>
-      <c r="EE43"/>
-      <c r="EF43"/>
-      <c r="EG43"/>
-      <c r="EH43"/>
-      <c r="EI43"/>
-      <c r="EJ43"/>
-      <c r="EK43"/>
-      <c r="EL43"/>
-      <c r="EM43"/>
-      <c r="EN43"/>
-      <c r="EO43"/>
-      <c r="EP43"/>
-      <c r="EQ43"/>
-      <c r="ER43"/>
-      <c r="ES43"/>
-      <c r="ET43"/>
-      <c r="EU43"/>
-      <c r="EV43"/>
-      <c r="EW43"/>
-      <c r="EX43"/>
-      <c r="EY43"/>
-      <c r="EZ43"/>
-      <c r="FA43"/>
-      <c r="FB43"/>
-      <c r="FC43"/>
-      <c r="FD43"/>
-      <c r="FE43"/>
-      <c r="FF43"/>
-      <c r="FG43"/>
-      <c r="FH43"/>
-      <c r="FI43"/>
-      <c r="FJ43"/>
-      <c r="FK43"/>
-      <c r="FL43"/>
-      <c r="FM43"/>
-      <c r="FN43"/>
-      <c r="FO43"/>
-      <c r="FP43"/>
-      <c r="FQ43"/>
-      <c r="FR43"/>
-      <c r="FS43"/>
-      <c r="FT43"/>
-      <c r="FU43"/>
-      <c r="FV43"/>
-      <c r="FW43"/>
-      <c r="FX43"/>
-      <c r="FY43"/>
-      <c r="FZ43"/>
-      <c r="GA43"/>
-      <c r="GB43"/>
-      <c r="GC43"/>
-      <c r="GD43"/>
-      <c r="GE43"/>
-      <c r="GF43"/>
-      <c r="GG43"/>
-      <c r="GH43"/>
-      <c r="GI43"/>
-      <c r="GJ43"/>
-      <c r="GK43"/>
-      <c r="GL43"/>
-      <c r="GM43"/>
-      <c r="GN43"/>
-      <c r="GO43"/>
-      <c r="GP43"/>
-      <c r="GQ43"/>
-      <c r="GR43"/>
-      <c r="GS43"/>
-      <c r="GT43"/>
-      <c r="GU43"/>
-      <c r="GV43"/>
-      <c r="GW43"/>
-      <c r="GX43"/>
-      <c r="GY43"/>
-      <c r="GZ43"/>
-      <c r="HA43"/>
-      <c r="HB43"/>
-      <c r="HC43"/>
-      <c r="HD43"/>
-      <c r="HE43"/>
-      <c r="HF43"/>
-      <c r="HG43"/>
-      <c r="HH43"/>
-      <c r="HI43"/>
-      <c r="HJ43"/>
-      <c r="HK43"/>
-      <c r="HL43"/>
-      <c r="HM43"/>
-      <c r="HN43"/>
-      <c r="HO43"/>
-      <c r="HP43"/>
-      <c r="HQ43"/>
-      <c r="HR43"/>
-      <c r="HS43"/>
-      <c r="HT43"/>
-      <c r="HU43"/>
-      <c r="HV43"/>
-      <c r="HW43"/>
-      <c r="HX43"/>
-      <c r="HY43"/>
-      <c r="HZ43"/>
-      <c r="IA43"/>
-      <c r="IB43"/>
-      <c r="IC43"/>
-      <c r="ID43"/>
-      <c r="IE43"/>
-      <c r="IF43"/>
-      <c r="IG43"/>
-      <c r="IH43"/>
-      <c r="II43"/>
-      <c r="IJ43"/>
-      <c r="IK43"/>
-      <c r="IL43"/>
-      <c r="IM43"/>
-      <c r="IN43"/>
-      <c r="IO43"/>
-      <c r="IP43"/>
-      <c r="IQ43"/>
-      <c r="IR43"/>
-      <c r="IS43"/>
-      <c r="IT43"/>
-      <c r="IU43"/>
-      <c r="IV43"/>
-    </row>
-    <row r="44" spans="1:256" ht="75" customHeight="1">
+      <c r="C43" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="4" t="str">
+        <f>"@list"</f>
+        <v>@list</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:256" ht="60" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>118</v>
+        <v>191</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>198</v>
@@ -3852,142 +3621,390 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="1:256" ht="19" customHeight="1">
-      <c r="A45" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B45" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:256" ht="60" customHeight="1">
+      <c r="A45" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="46" spans="1:256" ht="45" customHeight="1">
+      <c r="C45" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+      <c r="Z45"/>
+      <c r="AA45"/>
+      <c r="AB45"/>
+      <c r="AC45"/>
+      <c r="AD45"/>
+      <c r="AE45"/>
+      <c r="AF45"/>
+      <c r="AG45"/>
+      <c r="AH45"/>
+      <c r="AI45"/>
+      <c r="AJ45"/>
+      <c r="AK45"/>
+      <c r="AL45"/>
+      <c r="AM45"/>
+      <c r="AN45"/>
+      <c r="AO45"/>
+      <c r="AP45"/>
+      <c r="AQ45"/>
+      <c r="AR45"/>
+      <c r="AS45"/>
+      <c r="AT45"/>
+      <c r="AU45"/>
+      <c r="AV45"/>
+      <c r="AW45"/>
+      <c r="AX45"/>
+      <c r="AY45"/>
+      <c r="AZ45"/>
+      <c r="BA45"/>
+      <c r="BB45"/>
+      <c r="BC45"/>
+      <c r="BD45"/>
+      <c r="BE45"/>
+      <c r="BF45"/>
+      <c r="BG45"/>
+      <c r="BH45"/>
+      <c r="BI45"/>
+      <c r="BJ45"/>
+      <c r="BK45"/>
+      <c r="BL45"/>
+      <c r="BM45"/>
+      <c r="BN45"/>
+      <c r="BO45"/>
+      <c r="BP45"/>
+      <c r="BQ45"/>
+      <c r="BR45"/>
+      <c r="BS45"/>
+      <c r="BT45"/>
+      <c r="BU45"/>
+      <c r="BV45"/>
+      <c r="BW45"/>
+      <c r="BX45"/>
+      <c r="BY45"/>
+      <c r="BZ45"/>
+      <c r="CA45"/>
+      <c r="CB45"/>
+      <c r="CC45"/>
+      <c r="CD45"/>
+      <c r="CE45"/>
+      <c r="CF45"/>
+      <c r="CG45"/>
+      <c r="CH45"/>
+      <c r="CI45"/>
+      <c r="CJ45"/>
+      <c r="CK45"/>
+      <c r="CL45"/>
+      <c r="CM45"/>
+      <c r="CN45"/>
+      <c r="CO45"/>
+      <c r="CP45"/>
+      <c r="CQ45"/>
+      <c r="CR45"/>
+      <c r="CS45"/>
+      <c r="CT45"/>
+      <c r="CU45"/>
+      <c r="CV45"/>
+      <c r="CW45"/>
+      <c r="CX45"/>
+      <c r="CY45"/>
+      <c r="CZ45"/>
+      <c r="DA45"/>
+      <c r="DB45"/>
+      <c r="DC45"/>
+      <c r="DD45"/>
+      <c r="DE45"/>
+      <c r="DF45"/>
+      <c r="DG45"/>
+      <c r="DH45"/>
+      <c r="DI45"/>
+      <c r="DJ45"/>
+      <c r="DK45"/>
+      <c r="DL45"/>
+      <c r="DM45"/>
+      <c r="DN45"/>
+      <c r="DO45"/>
+      <c r="DP45"/>
+      <c r="DQ45"/>
+      <c r="DR45"/>
+      <c r="DS45"/>
+      <c r="DT45"/>
+      <c r="DU45"/>
+      <c r="DV45"/>
+      <c r="DW45"/>
+      <c r="DX45"/>
+      <c r="DY45"/>
+      <c r="DZ45"/>
+      <c r="EA45"/>
+      <c r="EB45"/>
+      <c r="EC45"/>
+      <c r="ED45"/>
+      <c r="EE45"/>
+      <c r="EF45"/>
+      <c r="EG45"/>
+      <c r="EH45"/>
+      <c r="EI45"/>
+      <c r="EJ45"/>
+      <c r="EK45"/>
+      <c r="EL45"/>
+      <c r="EM45"/>
+      <c r="EN45"/>
+      <c r="EO45"/>
+      <c r="EP45"/>
+      <c r="EQ45"/>
+      <c r="ER45"/>
+      <c r="ES45"/>
+      <c r="ET45"/>
+      <c r="EU45"/>
+      <c r="EV45"/>
+      <c r="EW45"/>
+      <c r="EX45"/>
+      <c r="EY45"/>
+      <c r="EZ45"/>
+      <c r="FA45"/>
+      <c r="FB45"/>
+      <c r="FC45"/>
+      <c r="FD45"/>
+      <c r="FE45"/>
+      <c r="FF45"/>
+      <c r="FG45"/>
+      <c r="FH45"/>
+      <c r="FI45"/>
+      <c r="FJ45"/>
+      <c r="FK45"/>
+      <c r="FL45"/>
+      <c r="FM45"/>
+      <c r="FN45"/>
+      <c r="FO45"/>
+      <c r="FP45"/>
+      <c r="FQ45"/>
+      <c r="FR45"/>
+      <c r="FS45"/>
+      <c r="FT45"/>
+      <c r="FU45"/>
+      <c r="FV45"/>
+      <c r="FW45"/>
+      <c r="FX45"/>
+      <c r="FY45"/>
+      <c r="FZ45"/>
+      <c r="GA45"/>
+      <c r="GB45"/>
+      <c r="GC45"/>
+      <c r="GD45"/>
+      <c r="GE45"/>
+      <c r="GF45"/>
+      <c r="GG45"/>
+      <c r="GH45"/>
+      <c r="GI45"/>
+      <c r="GJ45"/>
+      <c r="GK45"/>
+      <c r="GL45"/>
+      <c r="GM45"/>
+      <c r="GN45"/>
+      <c r="GO45"/>
+      <c r="GP45"/>
+      <c r="GQ45"/>
+      <c r="GR45"/>
+      <c r="GS45"/>
+      <c r="GT45"/>
+      <c r="GU45"/>
+      <c r="GV45"/>
+      <c r="GW45"/>
+      <c r="GX45"/>
+      <c r="GY45"/>
+      <c r="GZ45"/>
+      <c r="HA45"/>
+      <c r="HB45"/>
+      <c r="HC45"/>
+      <c r="HD45"/>
+      <c r="HE45"/>
+      <c r="HF45"/>
+      <c r="HG45"/>
+      <c r="HH45"/>
+      <c r="HI45"/>
+      <c r="HJ45"/>
+      <c r="HK45"/>
+      <c r="HL45"/>
+      <c r="HM45"/>
+      <c r="HN45"/>
+      <c r="HO45"/>
+      <c r="HP45"/>
+      <c r="HQ45"/>
+      <c r="HR45"/>
+      <c r="HS45"/>
+      <c r="HT45"/>
+      <c r="HU45"/>
+      <c r="HV45"/>
+      <c r="HW45"/>
+      <c r="HX45"/>
+      <c r="HY45"/>
+      <c r="HZ45"/>
+      <c r="IA45"/>
+      <c r="IB45"/>
+      <c r="IC45"/>
+      <c r="ID45"/>
+      <c r="IE45"/>
+      <c r="IF45"/>
+      <c r="IG45"/>
+      <c r="IH45"/>
+      <c r="II45"/>
+      <c r="IJ45"/>
+      <c r="IK45"/>
+      <c r="IL45"/>
+      <c r="IM45"/>
+      <c r="IN45"/>
+      <c r="IO45"/>
+      <c r="IP45"/>
+      <c r="IQ45"/>
+      <c r="IR45"/>
+      <c r="IS45"/>
+      <c r="IT45"/>
+      <c r="IU45"/>
+      <c r="IV45"/>
+    </row>
+    <row r="46" spans="1:256" ht="75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G46" s="9"/>
+        <v>118</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="47" spans="1:256" ht="30" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:256" ht="19" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>212</v>
+        <v>308</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>214</v>
+      <c r="F47" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="48" spans="1:256" ht="30" customHeight="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:256" ht="45" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="G48" s="5"/>
+      <c r="G48" s="9"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="45" customHeight="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4" t="s">
-        <v>118</v>
+        <v>191</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>198</v>
@@ -3996,116 +4013,116 @@
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="19" customHeight="1">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="45" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>214</v>
+        <v>186</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="7"/>
-    </row>
-    <row r="52" spans="1:10" ht="45" customHeight="1">
+      <c r="J51" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>226</v>
+        <v>118</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="30" customHeight="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="19" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4" t="s">
         <v>191</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
-      <c r="J53" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="30" customHeight="1">
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:10" ht="45" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="19" customHeight="1">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="30" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>143</v>
+        <v>228</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4" t="s">
-        <v>118</v>
+        <v>191</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>226</v>
@@ -4114,22 +4131,22 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="6" t="s">
-        <v>144</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>146</v>
+        <v>231</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>198</v>
@@ -4138,90 +4155,90 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="19" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>86</v>
+        <v>143</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>245</v>
+        <v>143</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>199</v>
+      <c r="F57" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="19" customHeight="1">
+      <c r="J57" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4" t="s">
-        <v>118</v>
+        <v>191</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="4" t="s">
-        <v>151</v>
+      <c r="J58" s="6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="19" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>226</v>
+      <c r="F59" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="6" t="s">
-        <v>87</v>
+      <c r="J59" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="19" customHeight="1">
       <c r="A60" s="4" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
@@ -4234,166 +4251,166 @@
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="4" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="19" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F61" s="5" t="s">
-        <v>199</v>
+      <c r="F61" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="4" t="s">
-        <v>93</v>
+      <c r="J61" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="19" customHeight="1">
       <c r="A62" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>226</v>
+      <c r="F62" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
-      <c r="J62" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="75" customHeight="1">
+      <c r="J62" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="19" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="4" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="45" customHeight="1">
+      <c r="I63" s="5"/>
+      <c r="J63" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="19" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>118</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="30" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="75" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>198</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="I65" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J65" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="45" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>13</v>
+        <v>165</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="45" customHeight="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>198</v>
@@ -4402,218 +4419,218 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="19" customHeight="1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="45" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="45" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>238</v>
+        <v>170</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>238</v>
+        <v>171</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>214</v>
+        <v>186</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="30" customHeight="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="19" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="30" customHeight="1">
+      <c r="A71" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="30" customHeight="1">
+      <c r="A72" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="F72" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G70" s="5"/>
-      <c r="H70" s="4" t="str">
+      <c r="G72" s="5"/>
+      <c r="H72" s="4" t="str">
         <f>"@set"</f>
         <v>@set</v>
       </c>
-      <c r="I70" s="5" t="b">
+      <c r="I72" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J70" s="6" t="s">
+      <c r="J72" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="19" customHeight="1">
-      <c r="A71" s="4" t="s">
+    <row r="73" spans="1:10" ht="19" customHeight="1">
+      <c r="A73" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D73" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="4" t="str">
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="4" t="str">
         <f>"@set"</f>
         <v>@set</v>
       </c>
-      <c r="I71" s="5"/>
-      <c r="J71" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="45" customHeight="1">
-      <c r="A72" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="30" customHeight="1">
-      <c r="A73" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>195</v>
+        <v>28</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="4" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="45" customHeight="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="30" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>125</v>
+        <v>193</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>226</v>
+        <v>118</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="19" customHeight="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="45" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
@@ -4626,18 +4643,18 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="30" customHeight="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="45" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
@@ -4650,334 +4667,342 @@
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="135" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="19" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="60" customHeight="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="30" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
       <c r="G79" s="5"/>
-      <c r="H79" s="4" t="str">
-        <f>"@set"</f>
-        <v>@set</v>
-      </c>
+      <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="75" customHeight="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="135" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G80" s="4" t="str">
-        <f>"@vocab"</f>
-        <v>@vocab</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="120" customHeight="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="60" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D81" s="5"/>
+        <v>135</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="E81" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>200</v>
+        <v>178</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
+      <c r="H81" s="4" t="str">
+        <f>"@set"</f>
+        <v>@set</v>
+      </c>
       <c r="I81" s="5"/>
       <c r="J81" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="120" customHeight="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="75" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G82" s="5"/>
+        <v>210</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G82" s="4" t="str">
+        <f>"@vocab"</f>
+        <v>@vocab</v>
+      </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="45" customHeight="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="120" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F83" s="4" t="s">
         <v>133</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="45" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="120" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G84" s="4" t="str">
-        <f>"@vocab"</f>
-        <v>@vocab</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G84" s="5"/>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="135" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="45" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F85" s="5"/>
+        <v>210</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="G85" s="5"/>
-      <c r="H85" s="4" t="str">
-        <f>"@language"</f>
-        <v>@language</v>
-      </c>
+      <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="30" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="45" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G86" s="5"/>
+        <v>241</v>
+      </c>
+      <c r="G86" s="4" t="str">
+        <f>"@vocab"</f>
+        <v>@vocab</v>
+      </c>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="30" customHeight="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="135" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>205</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F87" s="5"/>
       <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
+      <c r="H87" s="4" t="str">
+        <f>"@language"</f>
+        <v>@language</v>
+      </c>
       <c r="I87" s="5"/>
       <c r="J87" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="45" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="30" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>30</v>
+        <v>191</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="19" customHeight="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="30" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="E89" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>205</v>
+      </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="30" customHeight="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="45" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>191</v>
+        <v>16</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
+      <c r="E90" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="19" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>241</v>
+        <v>20</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -4986,18 +5011,18 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="30" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>186</v>
+        <v>22</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -5006,18 +5031,18 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="19" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>166</v>
+        <v>241</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>40</v>
+        <v>241</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -5026,18 +5051,18 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6" t="s">
-        <v>309</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="30" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>41</v>
+        <v>186</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
@@ -5046,18 +5071,18 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="45" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="30" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
@@ -5066,97 +5091,101 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="19" customHeight="1">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="30" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>312</v>
+        <v>178</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>311</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="19" customHeight="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="45" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>126</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
-      <c r="J97" s="6"/>
+      <c r="J97" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="98" spans="1:10" ht="19" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>47</v>
+        <v>312</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C98" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="D98" s="4" t="s">
-        <v>49</v>
+        <v>311</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
-      <c r="J98" s="7"/>
+      <c r="J98" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="99" spans="1:10" ht="19" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C99" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D99" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
-      <c r="J99" s="7"/>
+      <c r="J99" s="6"/>
     </row>
     <row r="100" spans="1:10" ht="19" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -5167,14 +5196,14 @@
     </row>
     <row r="101" spans="1:10" ht="19" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
@@ -5185,14 +5214,14 @@
     </row>
     <row r="102" spans="1:10" ht="19" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
@@ -5203,14 +5232,14 @@
     </row>
     <row r="103" spans="1:10" ht="19" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -5221,16 +5250,16 @@
     </row>
     <row r="104" spans="1:10" ht="19" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E104" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="E104" s="5"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
@@ -5239,16 +5268,16 @@
     </row>
     <row r="105" spans="1:10" ht="19" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E105" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="E105" s="5"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
@@ -5257,16 +5286,16 @@
     </row>
     <row r="106" spans="1:10" ht="19" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E106" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="E106" s="9"/>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
@@ -5275,16 +5304,16 @@
     </row>
     <row r="107" spans="1:10" ht="19" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E107" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="E107" s="9"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
@@ -5293,14 +5322,14 @@
     </row>
     <row r="108" spans="1:10" ht="19" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>306</v>
+        <v>64</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
@@ -5309,17 +5338,16 @@
       <c r="I108" s="5"/>
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1">
+    <row r="109" spans="1:10" ht="19" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4" t="str">
-        <f>CONCATENATE("xsd:",A109)</f>
-        <v>xsd:anySimpleType</v>
+      <c r="C109" s="5"/>
+      <c r="D109" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
@@ -5328,17 +5356,16 @@
       <c r="I109" s="5"/>
       <c r="J109" s="7"/>
     </row>
-    <row r="110" spans="1:10" ht="15" customHeight="1">
+    <row r="110" spans="1:10" ht="19" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>70</v>
+        <v>306</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4" t="str">
-        <f t="shared" ref="D110:D144" si="0">CONCATENATE("xsd:",A110)</f>
-        <v>xsd:string</v>
+      <c r="C110" s="5"/>
+      <c r="D110" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
@@ -5349,15 +5376,15 @@
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:normalizedString</v>
+        <f>CONCATENATE("xsd:",A111)</f>
+        <v>xsd:anySimpleType</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
@@ -5368,15 +5395,15 @@
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:token</v>
+        <f t="shared" ref="D112:D146" si="0">CONCATENATE("xsd:",A112)</f>
+        <v>xsd:string</v>
       </c>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
@@ -5387,7 +5414,7 @@
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>48</v>
@@ -5395,7 +5422,7 @@
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:Name</v>
+        <v>xsd:normalizedString</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
@@ -5406,7 +5433,7 @@
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>48</v>
@@ -5414,7 +5441,7 @@
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:NCName</v>
+        <v>xsd:token</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
@@ -5425,7 +5452,7 @@
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>48</v>
@@ -5433,7 +5460,7 @@
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:boolean</v>
+        <v>xsd:Name</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
@@ -5444,14 +5471,15 @@
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="C116" s="4"/>
-      <c r="D116" s="4" t="s">
-        <v>26</v>
+      <c r="D116" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:NCName</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
@@ -5462,7 +5490,7 @@
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>48</v>
@@ -5470,7 +5498,7 @@
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:decimal</v>
+        <v>xsd:boolean</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
@@ -5481,15 +5509,14 @@
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C118" s="4"/>
-      <c r="D118" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:integer</v>
+      <c r="D118" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
@@ -5500,7 +5527,7 @@
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>48</v>
@@ -5508,7 +5535,7 @@
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonPositiveInteger</v>
+        <v>xsd:decimal</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
@@ -5519,7 +5546,7 @@
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>48</v>
@@ -5527,7 +5554,7 @@
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:negativeInteger</v>
+        <v>xsd:integer</v>
       </c>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
@@ -5538,7 +5565,7 @@
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>48</v>
@@ -5546,7 +5573,7 @@
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:long</v>
+        <v>xsd:nonPositiveInteger</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
@@ -5557,7 +5584,7 @@
     </row>
     <row r="122" spans="1:10" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>48</v>
@@ -5565,7 +5592,7 @@
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:int</v>
+        <v>xsd:negativeInteger</v>
       </c>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -5576,7 +5603,7 @@
     </row>
     <row r="123" spans="1:10" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>48</v>
@@ -5584,7 +5611,7 @@
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:short</v>
+        <v>xsd:long</v>
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -5595,7 +5622,7 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>48</v>
@@ -5603,7 +5630,7 @@
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:byte</v>
+        <v>xsd:int</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
@@ -5614,7 +5641,7 @@
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>48</v>
@@ -5622,7 +5649,7 @@
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonNegativeInteger</v>
+        <v>xsd:short</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
@@ -5633,7 +5660,7 @@
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>48</v>
@@ -5641,7 +5668,7 @@
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedLong</v>
+        <v>xsd:byte</v>
       </c>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
@@ -5652,7 +5679,7 @@
     </row>
     <row r="127" spans="1:10" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>48</v>
@@ -5660,7 +5687,7 @@
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedInt</v>
+        <v>xsd:nonNegativeInteger</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
@@ -5671,7 +5698,7 @@
     </row>
     <row r="128" spans="1:10" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>48</v>
@@ -5679,7 +5706,7 @@
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedShort</v>
+        <v>xsd:unsignedLong</v>
       </c>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
@@ -5690,7 +5717,7 @@
     </row>
     <row r="129" spans="1:10" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>48</v>
@@ -5698,7 +5725,7 @@
       <c r="C129" s="4"/>
       <c r="D129" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedByte</v>
+        <v>xsd:unsignedInt</v>
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
@@ -5709,7 +5736,7 @@
     </row>
     <row r="130" spans="1:10" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>48</v>
@@ -5717,7 +5744,7 @@
       <c r="C130" s="4"/>
       <c r="D130" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:positiveInteger</v>
+        <v>xsd:unsignedShort</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
@@ -5728,7 +5755,7 @@
     </row>
     <row r="131" spans="1:10" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>48</v>
@@ -5736,7 +5763,7 @@
       <c r="C131" s="4"/>
       <c r="D131" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:float</v>
+        <v>xsd:unsignedByte</v>
       </c>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
@@ -5747,7 +5774,7 @@
     </row>
     <row r="132" spans="1:10" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>48</v>
@@ -5755,7 +5782,7 @@
       <c r="C132" s="4"/>
       <c r="D132" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:double</v>
+        <v>xsd:positiveInteger</v>
       </c>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
@@ -5766,7 +5793,7 @@
     </row>
     <row r="133" spans="1:10" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>48</v>
@@ -5774,7 +5801,7 @@
       <c r="C133" s="4"/>
       <c r="D133" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:duration</v>
+        <v>xsd:float</v>
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
@@ -5785,7 +5812,7 @@
     </row>
     <row r="134" spans="1:10" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>48</v>
@@ -5793,7 +5820,7 @@
       <c r="C134" s="4"/>
       <c r="D134" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:dateTime</v>
+        <v>xsd:double</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
@@ -5804,7 +5831,7 @@
     </row>
     <row r="135" spans="1:10" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>48</v>
@@ -5812,7 +5839,7 @@
       <c r="C135" s="4"/>
       <c r="D135" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:time</v>
+        <v>xsd:duration</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
@@ -5823,7 +5850,7 @@
     </row>
     <row r="136" spans="1:10" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>48</v>
@@ -5831,7 +5858,7 @@
       <c r="C136" s="4"/>
       <c r="D136" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:date</v>
+        <v>xsd:dateTime</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
@@ -5842,7 +5869,7 @@
     </row>
     <row r="137" spans="1:10" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>48</v>
@@ -5850,7 +5877,7 @@
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYearMonth</v>
+        <v>xsd:time</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
@@ -5861,7 +5888,7 @@
     </row>
     <row r="138" spans="1:10" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>48</v>
@@ -5869,7 +5896,7 @@
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYear</v>
+        <v>xsd:date</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
@@ -5880,7 +5907,7 @@
     </row>
     <row r="139" spans="1:10" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>48</v>
@@ -5888,7 +5915,7 @@
       <c r="C139" s="4"/>
       <c r="D139" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonthDay</v>
+        <v>xsd:gYearMonth</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
@@ -5899,7 +5926,7 @@
     </row>
     <row r="140" spans="1:10" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>48</v>
@@ -5907,7 +5934,7 @@
       <c r="C140" s="4"/>
       <c r="D140" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gDay</v>
+        <v>xsd:gYear</v>
       </c>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
@@ -5918,7 +5945,7 @@
     </row>
     <row r="141" spans="1:10" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>48</v>
@@ -5926,7 +5953,7 @@
       <c r="C141" s="4"/>
       <c r="D141" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonth</v>
+        <v>xsd:gMonthDay</v>
       </c>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
@@ -5937,7 +5964,7 @@
     </row>
     <row r="142" spans="1:10" ht="15" customHeight="1">
       <c r="A142" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>48</v>
@@ -5945,7 +5972,7 @@
       <c r="C142" s="4"/>
       <c r="D142" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:hexBinary</v>
+        <v>xsd:gDay</v>
       </c>
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
@@ -5956,7 +5983,7 @@
     </row>
     <row r="143" spans="1:10" ht="15" customHeight="1">
       <c r="A143" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>48</v>
@@ -5964,7 +5991,7 @@
       <c r="C143" s="4"/>
       <c r="D143" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:base64Binary</v>
+        <v>xsd:gMonth</v>
       </c>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
@@ -5975,7 +6002,7 @@
     </row>
     <row r="144" spans="1:10" ht="15" customHeight="1">
       <c r="A144" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>48</v>
@@ -5983,7 +6010,7 @@
       <c r="C144" s="4"/>
       <c r="D144" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:anyURI</v>
+        <v>xsd:hexBinary</v>
       </c>
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
@@ -5992,45 +6019,83 @@
       <c r="I144" s="5"/>
       <c r="J144" s="7"/>
     </row>
+    <row r="145" spans="1:10" ht="15" customHeight="1">
+      <c r="A145" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:base64Binary</v>
+      </c>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+      <c r="I145" s="5"/>
+      <c r="J145" s="7"/>
+    </row>
+    <row r="146" spans="1:10" ht="15" customHeight="1">
+      <c r="A146" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:anyURI</v>
+      </c>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="J146" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D6" r:id="rId3"/>
-    <hyperlink ref="D7" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D9" r:id="rId6"/>
-    <hyperlink ref="D10" r:id="rId7"/>
-    <hyperlink ref="D11" r:id="rId8"/>
-    <hyperlink ref="D12" r:id="rId9"/>
-    <hyperlink ref="D13" r:id="rId10"/>
-    <hyperlink ref="D14" r:id="rId11"/>
-    <hyperlink ref="D15" r:id="rId12"/>
-    <hyperlink ref="D16" r:id="rId13"/>
-    <hyperlink ref="D17" r:id="rId14"/>
-    <hyperlink ref="D18" r:id="rId15"/>
-    <hyperlink ref="D19" r:id="rId16"/>
-    <hyperlink ref="D20" r:id="rId17"/>
-    <hyperlink ref="D21" r:id="rId18"/>
-    <hyperlink ref="D22" r:id="rId19"/>
-    <hyperlink ref="D23" r:id="rId20"/>
-    <hyperlink ref="D24" r:id="rId21"/>
-    <hyperlink ref="D25" r:id="rId22"/>
-    <hyperlink ref="D26" r:id="rId23"/>
-    <hyperlink ref="D27" r:id="rId24"/>
-    <hyperlink ref="D28" r:id="rId25"/>
-    <hyperlink ref="D29" r:id="rId26"/>
-    <hyperlink ref="D30" r:id="rId27"/>
-    <hyperlink ref="D31" r:id="rId28"/>
-    <hyperlink ref="D32" r:id="rId29"/>
-    <hyperlink ref="D33" r:id="rId30"/>
-    <hyperlink ref="D34" r:id="rId31"/>
-    <hyperlink ref="D35" r:id="rId32"/>
-    <hyperlink ref="D36" r:id="rId33"/>
-    <hyperlink ref="D37" r:id="rId34"/>
-    <hyperlink ref="D38" r:id="rId35"/>
-    <hyperlink ref="D39" r:id="rId36"/>
+    <hyperlink ref="D6" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId8"/>
+    <hyperlink ref="D14" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D17" r:id="rId12"/>
+    <hyperlink ref="D18" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21"/>
+    <hyperlink ref="D27" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D35" r:id="rId30"/>
+    <hyperlink ref="D36" r:id="rId31"/>
+    <hyperlink ref="D37" r:id="rId32"/>
+    <hyperlink ref="D38" r:id="rId33"/>
+    <hyperlink ref="D39" r:id="rId34"/>
+    <hyperlink ref="D40" r:id="rId35"/>
+    <hyperlink ref="D41" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add information on virtual columns. This fixes #179.
</commit_message>
<xml_diff>
--- a/ns/_vocab.xlsx
+++ b/ns/_vocab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="240" yWindow="2340" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="314">
   <si>
     <t>unsignedInt</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1302,6 +1302,12 @@
   </si>
   <si>
     <t>A Table Group describes an Annotated Table Group.</t>
+  </si>
+  <si>
+    <t>virtual</t>
+  </si>
+  <si>
+    <t>A boolean atomic property taking a single value which indicates whether the column is a virtual column not present in the original source</t>
   </si>
 </sst>
 </file>
@@ -1389,8 +1395,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1423,8 +1432,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2742,11 +2752,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV144"/>
+  <dimension ref="A1:IV145"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4926,35 +4936,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="19" customHeight="1">
+    <row r="89" spans="1:10" ht="45" customHeight="1">
       <c r="A89" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="F89" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="30" customHeight="1">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="19" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -4963,18 +4977,18 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="19" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="30" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>242</v>
+        <v>22</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -4983,18 +4997,18 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="19" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>187</v>
+        <v>242</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>187</v>
+        <v>242</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -5003,18 +5017,18 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="30" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -5023,18 +5037,18 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6" t="s">
-        <v>310</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="30" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
@@ -5043,18 +5057,18 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="45" customHeight="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="30" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
@@ -5063,79 +5077,81 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="19" customHeight="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="45" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="19" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
-      <c r="J97" s="6"/>
+      <c r="J97" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="98" spans="1:10" ht="19" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C98" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D98" s="4" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
-      <c r="J98" s="7"/>
+      <c r="J98" s="6"/>
     </row>
     <row r="99" spans="1:10" ht="19" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -5146,14 +5162,14 @@
     </row>
     <row r="100" spans="1:10" ht="19" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -5164,14 +5180,14 @@
     </row>
     <row r="101" spans="1:10" ht="19" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
@@ -5182,14 +5198,14 @@
     </row>
     <row r="102" spans="1:10" ht="19" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
@@ -5200,14 +5216,14 @@
     </row>
     <row r="103" spans="1:10" ht="19" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -5218,16 +5234,16 @@
     </row>
     <row r="104" spans="1:10" ht="19" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E104" s="9"/>
+        <v>60</v>
+      </c>
+      <c r="E104" s="5"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
@@ -5236,14 +5252,14 @@
     </row>
     <row r="105" spans="1:10" ht="19" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E105" s="9"/>
       <c r="F105" s="5"/>
@@ -5254,16 +5270,16 @@
     </row>
     <row r="106" spans="1:10" ht="19" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E106" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="E106" s="9"/>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
@@ -5272,14 +5288,14 @@
     </row>
     <row r="107" spans="1:10" ht="19" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
@@ -5290,14 +5306,14 @@
     </row>
     <row r="108" spans="1:10" ht="19" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>307</v>
+        <v>67</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
@@ -5306,17 +5322,16 @@
       <c r="I108" s="5"/>
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1">
+    <row r="109" spans="1:10" ht="19" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4" t="str">
-        <f>CONCATENATE("xsd:",A109)</f>
-        <v>xsd:anySimpleType</v>
+      <c r="C109" s="5"/>
+      <c r="D109" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
@@ -5327,15 +5342,15 @@
     </row>
     <row r="110" spans="1:10" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="str">
-        <f t="shared" ref="D110:D144" si="0">CONCATENATE("xsd:",A110)</f>
-        <v>xsd:string</v>
+        <f>CONCATENATE("xsd:",A110)</f>
+        <v>xsd:anySimpleType</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
@@ -5346,15 +5361,15 @@
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:normalizedString</v>
+        <f t="shared" ref="D111:D145" si="0">CONCATENATE("xsd:",A111)</f>
+        <v>xsd:string</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
@@ -5365,7 +5380,7 @@
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>49</v>
@@ -5373,7 +5388,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:token</v>
+        <v>xsd:normalizedString</v>
       </c>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
@@ -5384,7 +5399,7 @@
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>49</v>
@@ -5392,7 +5407,7 @@
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:Name</v>
+        <v>xsd:token</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
@@ -5403,7 +5418,7 @@
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>49</v>
@@ -5411,7 +5426,7 @@
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:NCName</v>
+        <v>xsd:Name</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
@@ -5422,7 +5437,7 @@
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>49</v>
@@ -5430,7 +5445,7 @@
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:boolean</v>
+        <v>xsd:NCName</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
@@ -5441,14 +5456,15 @@
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="C116" s="4"/>
-      <c r="D116" s="4" t="s">
-        <v>26</v>
+      <c r="D116" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:boolean</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
@@ -5459,15 +5475,14 @@
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="C117" s="4"/>
-      <c r="D117" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>xsd:decimal</v>
+      <c r="D117" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
@@ -5478,7 +5493,7 @@
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>49</v>
@@ -5486,7 +5501,7 @@
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:integer</v>
+        <v>xsd:decimal</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
@@ -5497,7 +5512,7 @@
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>49</v>
@@ -5505,7 +5520,7 @@
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonPositiveInteger</v>
+        <v>xsd:integer</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
@@ -5516,7 +5531,7 @@
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>49</v>
@@ -5524,7 +5539,7 @@
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:negativeInteger</v>
+        <v>xsd:nonPositiveInteger</v>
       </c>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
@@ -5535,7 +5550,7 @@
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>49</v>
@@ -5543,7 +5558,7 @@
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:long</v>
+        <v>xsd:negativeInteger</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
@@ -5554,7 +5569,7 @@
     </row>
     <row r="122" spans="1:10" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>49</v>
@@ -5562,7 +5577,7 @@
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:int</v>
+        <v>xsd:long</v>
       </c>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -5573,7 +5588,7 @@
     </row>
     <row r="123" spans="1:10" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>49</v>
@@ -5581,7 +5596,7 @@
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:short</v>
+        <v>xsd:int</v>
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -5592,7 +5607,7 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>49</v>
@@ -5600,7 +5615,7 @@
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:byte</v>
+        <v>xsd:short</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
@@ -5611,7 +5626,7 @@
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>49</v>
@@ -5619,7 +5634,7 @@
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:nonNegativeInteger</v>
+        <v>xsd:byte</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
@@ -5630,7 +5645,7 @@
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>49</v>
@@ -5638,7 +5653,7 @@
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedLong</v>
+        <v>xsd:nonNegativeInteger</v>
       </c>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
@@ -5649,7 +5664,7 @@
     </row>
     <row r="127" spans="1:10" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>49</v>
@@ -5657,7 +5672,7 @@
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedInt</v>
+        <v>xsd:unsignedLong</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
@@ -5668,7 +5683,7 @@
     </row>
     <row r="128" spans="1:10" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>49</v>
@@ -5676,7 +5691,7 @@
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedShort</v>
+        <v>xsd:unsignedInt</v>
       </c>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
@@ -5687,7 +5702,7 @@
     </row>
     <row r="129" spans="1:10" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>49</v>
@@ -5695,7 +5710,7 @@
       <c r="C129" s="4"/>
       <c r="D129" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:unsignedByte</v>
+        <v>xsd:unsignedShort</v>
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
@@ -5706,7 +5721,7 @@
     </row>
     <row r="130" spans="1:10" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>49</v>
@@ -5714,7 +5729,7 @@
       <c r="C130" s="4"/>
       <c r="D130" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:positiveInteger</v>
+        <v>xsd:unsignedByte</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
@@ -5725,7 +5740,7 @@
     </row>
     <row r="131" spans="1:10" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>49</v>
@@ -5733,7 +5748,7 @@
       <c r="C131" s="4"/>
       <c r="D131" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:float</v>
+        <v>xsd:positiveInteger</v>
       </c>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
@@ -5744,7 +5759,7 @@
     </row>
     <row r="132" spans="1:10" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>49</v>
@@ -5752,7 +5767,7 @@
       <c r="C132" s="4"/>
       <c r="D132" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:double</v>
+        <v>xsd:float</v>
       </c>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
@@ -5763,7 +5778,7 @@
     </row>
     <row r="133" spans="1:10" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>49</v>
@@ -5771,7 +5786,7 @@
       <c r="C133" s="4"/>
       <c r="D133" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:duration</v>
+        <v>xsd:double</v>
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
@@ -5782,7 +5797,7 @@
     </row>
     <row r="134" spans="1:10" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>49</v>
@@ -5790,7 +5805,7 @@
       <c r="C134" s="4"/>
       <c r="D134" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:dateTime</v>
+        <v>xsd:duration</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
@@ -5801,7 +5816,7 @@
     </row>
     <row r="135" spans="1:10" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>49</v>
@@ -5809,7 +5824,7 @@
       <c r="C135" s="4"/>
       <c r="D135" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:time</v>
+        <v>xsd:dateTime</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
@@ -5820,7 +5835,7 @@
     </row>
     <row r="136" spans="1:10" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>49</v>
@@ -5828,7 +5843,7 @@
       <c r="C136" s="4"/>
       <c r="D136" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:date</v>
+        <v>xsd:time</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
@@ -5839,7 +5854,7 @@
     </row>
     <row r="137" spans="1:10" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>49</v>
@@ -5847,7 +5862,7 @@
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYearMonth</v>
+        <v>xsd:date</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
@@ -5858,7 +5873,7 @@
     </row>
     <row r="138" spans="1:10" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>49</v>
@@ -5866,7 +5881,7 @@
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gYear</v>
+        <v>xsd:gYearMonth</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
@@ -5877,7 +5892,7 @@
     </row>
     <row r="139" spans="1:10" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>49</v>
@@ -5885,7 +5900,7 @@
       <c r="C139" s="4"/>
       <c r="D139" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonthDay</v>
+        <v>xsd:gYear</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
@@ -5896,7 +5911,7 @@
     </row>
     <row r="140" spans="1:10" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>49</v>
@@ -5904,7 +5919,7 @@
       <c r="C140" s="4"/>
       <c r="D140" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gDay</v>
+        <v>xsd:gMonthDay</v>
       </c>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
@@ -5915,7 +5930,7 @@
     </row>
     <row r="141" spans="1:10" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>49</v>
@@ -5923,7 +5938,7 @@
       <c r="C141" s="4"/>
       <c r="D141" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:gMonth</v>
+        <v>xsd:gDay</v>
       </c>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
@@ -5934,7 +5949,7 @@
     </row>
     <row r="142" spans="1:10" ht="15" customHeight="1">
       <c r="A142" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>49</v>
@@ -5942,7 +5957,7 @@
       <c r="C142" s="4"/>
       <c r="D142" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:hexBinary</v>
+        <v>xsd:gMonth</v>
       </c>
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
@@ -5953,7 +5968,7 @@
     </row>
     <row r="143" spans="1:10" ht="15" customHeight="1">
       <c r="A143" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>49</v>
@@ -5961,7 +5976,7 @@
       <c r="C143" s="4"/>
       <c r="D143" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:base64Binary</v>
+        <v>xsd:hexBinary</v>
       </c>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
@@ -5972,7 +5987,7 @@
     </row>
     <row r="144" spans="1:10" ht="15" customHeight="1">
       <c r="A144" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>49</v>
@@ -5980,7 +5995,7 @@
       <c r="C144" s="4"/>
       <c r="D144" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>xsd:anyURI</v>
+        <v>xsd:base64Binary</v>
       </c>
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
@@ -5988,6 +6003,25 @@
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
       <c r="J144" s="7"/>
+    </row>
+    <row r="145" spans="1:10" ht="15" customHeight="1">
+      <c r="A145" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>xsd:anyURI</v>
+      </c>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+      <c r="I145" s="5"/>
+      <c r="J145" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>